<commit_message>
[DATA] update planet data formatting (transpose, sort oldest to newest)
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\Downloads\planet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E71B5DC-562C-4911-94AC-37F03F4643E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5571222F-429E-42BA-B80A-3ECDB0B54C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12945" yWindow="0" windowWidth="15960" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="consolidated" sheetId="1" r:id="rId1"/>
-    <sheet name="income" sheetId="2" r:id="rId2"/>
+    <sheet name="consolidated" sheetId="3" r:id="rId1"/>
+    <sheet name="income" sheetId="4" r:id="rId2"/>
+    <sheet name="pre-consolidation" sheetId="1" r:id="rId3"/>
+    <sheet name="pre-income" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>Cash and cash equivalents</t>
   </si>
@@ -185,6 +187,9 @@
   <si>
     <t>Total other income, net</t>
   </si>
+  <si>
+    <t>Quarter</t>
+  </si>
 </sst>
 </file>
 
@@ -193,8 +198,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -274,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -293,19 +298,19 @@
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -314,8 +319,11 @@
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -597,11 +605,2220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
+  <dimension ref="A1:AG10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44227</v>
+      </c>
+      <c r="B2" s="13">
+        <v>71183000</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>47110000</v>
+      </c>
+      <c r="E2" s="13">
+        <v>7134000</v>
+      </c>
+      <c r="F2" s="13">
+        <v>125427000</v>
+      </c>
+      <c r="G2" s="13">
+        <v>159855000</v>
+      </c>
+      <c r="H2" s="13">
+        <v>11994000</v>
+      </c>
+      <c r="I2" s="13">
+        <v>88393000</v>
+      </c>
+      <c r="J2" s="13">
+        <v>5673000</v>
+      </c>
+      <c r="K2" s="13">
+        <v>4982000</v>
+      </c>
+      <c r="L2" s="13">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13">
+        <v>2984000</v>
+      </c>
+      <c r="N2" s="13">
+        <v>399308000</v>
+      </c>
+      <c r="O2" s="13">
+        <v>1446000</v>
+      </c>
+      <c r="P2" s="13">
+        <v>30195000</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>57570000</v>
+      </c>
+      <c r="R2" s="13">
+        <v>0</v>
+      </c>
+      <c r="S2" s="13">
+        <v>0</v>
+      </c>
+      <c r="T2" s="13">
+        <v>108814000</v>
+      </c>
+      <c r="U2" s="13">
+        <v>15122000</v>
+      </c>
+      <c r="V2" s="13">
+        <v>7971000</v>
+      </c>
+      <c r="W2" s="13">
+        <v>0</v>
+      </c>
+      <c r="X2" s="13">
+        <v>2991000</v>
+      </c>
+      <c r="Y2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="13">
+        <v>1287000</v>
+      </c>
+      <c r="AB2" s="13">
+        <v>291797000</v>
+      </c>
+      <c r="AC2" s="13">
+        <v>745630000</v>
+      </c>
+      <c r="AD2" s="13">
+        <v>1769000</v>
+      </c>
+      <c r="AE2" s="13">
+        <v>-639905000</v>
+      </c>
+      <c r="AF2" s="13">
+        <v>107511000</v>
+      </c>
+      <c r="AG2" s="13">
+        <v>399308000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>44592</v>
+      </c>
+      <c r="B3" s="5">
+        <v>490762000</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>44373000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>16385000</v>
+      </c>
+      <c r="F3" s="5">
+        <v>551520000</v>
+      </c>
+      <c r="G3" s="5">
+        <v>133280000</v>
+      </c>
+      <c r="H3" s="5">
+        <v>10768000</v>
+      </c>
+      <c r="I3" s="5">
+        <v>103219000</v>
+      </c>
+      <c r="J3" s="5">
+        <v>14197000</v>
+      </c>
+      <c r="K3" s="5">
+        <v>5743000</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2714000</v>
+      </c>
+      <c r="N3" s="5">
+        <v>821441000</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2850000</v>
+      </c>
+      <c r="P3" s="5">
+        <v>48823000</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>64233000</v>
+      </c>
+      <c r="R3" s="5">
+        <v>16135000</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="5">
+        <v>132041000</v>
+      </c>
+      <c r="U3" s="5">
+        <v>3579000</v>
+      </c>
+      <c r="V3" s="5">
+        <v>12149000</v>
+      </c>
+      <c r="W3" s="5">
+        <v>23224000</v>
+      </c>
+      <c r="X3" s="5">
+        <v>798000</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>1405000</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>173196000</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>1423151000</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>2096000</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>-777029000</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>648245000</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>821441000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>44592</v>
+      </c>
+      <c r="B4" s="13">
+        <v>490762000</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>44373000</v>
+      </c>
+      <c r="E4" s="13">
+        <v>16385000</v>
+      </c>
+      <c r="F4" s="13">
+        <v>551520000</v>
+      </c>
+      <c r="G4" s="13">
+        <v>133280000</v>
+      </c>
+      <c r="H4" s="13">
+        <v>10768000</v>
+      </c>
+      <c r="I4" s="13">
+        <v>103219000</v>
+      </c>
+      <c r="J4" s="13">
+        <v>14197000</v>
+      </c>
+      <c r="K4" s="13">
+        <v>5743000</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
+        <v>2714000</v>
+      </c>
+      <c r="N4" s="13">
+        <v>821441000</v>
+      </c>
+      <c r="O4" s="13">
+        <v>2850000</v>
+      </c>
+      <c r="P4" s="13">
+        <v>48823000</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>64233000</v>
+      </c>
+      <c r="R4" s="13">
+        <v>16135000</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="13">
+        <v>132041000</v>
+      </c>
+      <c r="U4" s="13">
+        <v>3579000</v>
+      </c>
+      <c r="V4" s="13">
+        <v>12149000</v>
+      </c>
+      <c r="W4" s="13">
+        <v>23224000</v>
+      </c>
+      <c r="X4" s="13">
+        <v>798000</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="13">
+        <v>1405000</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>173196000</v>
+      </c>
+      <c r="AC4" s="13">
+        <v>1423151000</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>2096000</v>
+      </c>
+      <c r="AE4" s="13">
+        <v>-777029000</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>648245000</v>
+      </c>
+      <c r="AG4" s="13">
+        <v>821441000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>44681</v>
+      </c>
+      <c r="B5" s="13">
+        <v>484489000</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>24581000</v>
+      </c>
+      <c r="E5" s="13">
+        <v>18192000</v>
+      </c>
+      <c r="F5" s="13">
+        <v>527262000</v>
+      </c>
+      <c r="G5" s="13">
+        <v>125329000</v>
+      </c>
+      <c r="H5" s="13">
+        <v>11105000</v>
+      </c>
+      <c r="I5" s="13">
+        <v>103219000</v>
+      </c>
+      <c r="J5" s="13">
+        <v>13604000</v>
+      </c>
+      <c r="K5" s="13">
+        <v>5653000</v>
+      </c>
+      <c r="L5" s="13">
+        <v>7035000</v>
+      </c>
+      <c r="M5" s="13">
+        <v>2787000</v>
+      </c>
+      <c r="N5" s="13">
+        <v>795994000</v>
+      </c>
+      <c r="O5" s="13">
+        <v>3168000</v>
+      </c>
+      <c r="P5" s="13">
+        <v>43184000</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>60672000</v>
+      </c>
+      <c r="R5" s="13">
+        <v>15239000</v>
+      </c>
+      <c r="S5" s="13">
+        <v>7188000</v>
+      </c>
+      <c r="T5" s="13">
+        <v>129451000</v>
+      </c>
+      <c r="U5" s="13">
+        <v>0</v>
+      </c>
+      <c r="V5" s="13">
+        <v>12199000</v>
+      </c>
+      <c r="W5" s="13">
+        <v>19948000</v>
+      </c>
+      <c r="X5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>2271000</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>1419000</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>165288000</v>
+      </c>
+      <c r="AC5" s="13">
+        <v>1450098000</v>
+      </c>
+      <c r="AD5" s="13">
+        <v>2271000</v>
+      </c>
+      <c r="AE5" s="13">
+        <v>-821690000</v>
+      </c>
+      <c r="AF5" s="13">
+        <v>630706000</v>
+      </c>
+      <c r="AG5" s="13">
+        <v>795994000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>44865</v>
+      </c>
+      <c r="B6" s="5">
+        <v>199124000</v>
+      </c>
+      <c r="C6" s="5">
+        <v>226163000</v>
+      </c>
+      <c r="D6" s="5">
+        <v>29009000</v>
+      </c>
+      <c r="E6" s="5">
+        <v>26347000</v>
+      </c>
+      <c r="F6" s="5">
+        <v>480643000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>115385000</v>
+      </c>
+      <c r="H6" s="5">
+        <v>11181000</v>
+      </c>
+      <c r="I6" s="5">
+        <v>103219000</v>
+      </c>
+      <c r="J6" s="5">
+        <v>12419000</v>
+      </c>
+      <c r="K6" s="5">
+        <v>5163000</v>
+      </c>
+      <c r="L6" s="5">
+        <v>15806000</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3412000</v>
+      </c>
+      <c r="N6" s="5">
+        <v>747228000</v>
+      </c>
+      <c r="O6" s="5">
+        <v>2557000</v>
+      </c>
+      <c r="P6" s="5">
+        <v>42629000</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>47698000</v>
+      </c>
+      <c r="R6" s="5">
+        <v>13446000</v>
+      </c>
+      <c r="S6" s="5">
+        <v>3538000</v>
+      </c>
+      <c r="T6" s="5">
+        <v>109868000</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>9853000</v>
+      </c>
+      <c r="W6" s="5">
+        <v>17855000</v>
+      </c>
+      <c r="X6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>14024000</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>1461000</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>153061000</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>1494652000</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>943000</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>-901455000</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>594167000</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>747228000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>44957</v>
+      </c>
+      <c r="B7" s="5">
+        <v>181892000</v>
+      </c>
+      <c r="C7" s="5">
+        <v>226868000</v>
+      </c>
+      <c r="D7" s="5">
+        <v>38952000</v>
+      </c>
+      <c r="E7" s="5">
+        <v>27943000</v>
+      </c>
+      <c r="F7" s="5">
+        <v>475655000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>108091000</v>
+      </c>
+      <c r="H7" s="5">
+        <v>11417000</v>
+      </c>
+      <c r="I7" s="5">
+        <v>112748000</v>
+      </c>
+      <c r="J7" s="5">
+        <v>14831000</v>
+      </c>
+      <c r="K7" s="5">
+        <v>5657000</v>
+      </c>
+      <c r="L7" s="5">
+        <v>20403000</v>
+      </c>
+      <c r="M7" s="5">
+        <v>3921000</v>
+      </c>
+      <c r="N7" s="5">
+        <v>752723000</v>
+      </c>
+      <c r="O7" s="5">
+        <v>6900000</v>
+      </c>
+      <c r="P7" s="5">
+        <v>46022000</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>51900000</v>
+      </c>
+      <c r="R7" s="5">
+        <v>12550000</v>
+      </c>
+      <c r="S7" s="5">
+        <v>4885000</v>
+      </c>
+      <c r="T7" s="5">
+        <v>122257000</v>
+      </c>
+      <c r="U7" s="5">
+        <v>2882000</v>
+      </c>
+      <c r="V7" s="5">
+        <v>8679000</v>
+      </c>
+      <c r="W7" s="5">
+        <v>16670000</v>
+      </c>
+      <c r="X7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>17145000</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>7499000</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>1487000</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>176619000</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>1513102000</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>2271000</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>-939296000</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>576104000</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>752723000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>45046</v>
+      </c>
+      <c r="B8" s="5">
+        <v>140763000</v>
+      </c>
+      <c r="C8" s="5">
+        <v>235415000</v>
+      </c>
+      <c r="D8" s="5">
+        <v>39072000</v>
+      </c>
+      <c r="E8" s="5">
+        <v>19275000</v>
+      </c>
+      <c r="F8" s="5">
+        <v>434525000</v>
+      </c>
+      <c r="G8" s="5">
+        <v>118193000</v>
+      </c>
+      <c r="H8" s="5">
+        <v>11878000</v>
+      </c>
+      <c r="I8" s="5">
+        <v>112748000</v>
+      </c>
+      <c r="J8" s="5">
+        <v>13999000</v>
+      </c>
+      <c r="K8" s="5">
+        <v>5660000</v>
+      </c>
+      <c r="L8" s="5">
+        <v>23697000</v>
+      </c>
+      <c r="M8" s="5">
+        <v>2757000</v>
+      </c>
+      <c r="N8" s="5">
+        <v>723457000</v>
+      </c>
+      <c r="O8" s="5">
+        <v>14657000</v>
+      </c>
+      <c r="P8" s="5">
+        <v>34432000</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>44620000</v>
+      </c>
+      <c r="R8" s="5">
+        <v>11653000</v>
+      </c>
+      <c r="S8" s="5">
+        <v>6320000</v>
+      </c>
+      <c r="T8" s="5">
+        <v>111682000</v>
+      </c>
+      <c r="U8" s="5">
+        <v>2474000</v>
+      </c>
+      <c r="V8" s="5">
+        <v>10671000</v>
+      </c>
+      <c r="W8" s="5">
+        <v>10725000</v>
+      </c>
+      <c r="X8" s="5">
+        <v>19912000</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>7142000</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>1502000</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>164108000</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>1531380000</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>1682000</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>-973740000</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>559349000</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>723457000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>45138</v>
+      </c>
+      <c r="B9" s="12">
+        <v>118808000</v>
+      </c>
+      <c r="C9" s="12">
+        <v>248979000</v>
+      </c>
+      <c r="D9" s="12">
+        <v>40349000</v>
+      </c>
+      <c r="E9" s="12">
+        <v>19725000</v>
+      </c>
+      <c r="F9" s="12">
+        <v>427861000</v>
+      </c>
+      <c r="G9" s="12">
+        <v>120193000</v>
+      </c>
+      <c r="H9" s="12">
+        <v>12992000</v>
+      </c>
+      <c r="I9" s="12">
+        <v>112750000</v>
+      </c>
+      <c r="J9" s="12">
+        <v>14867000</v>
+      </c>
+      <c r="K9" s="12">
+        <v>5707000</v>
+      </c>
+      <c r="L9" s="12">
+        <v>23485000</v>
+      </c>
+      <c r="M9" s="12">
+        <v>2562000</v>
+      </c>
+      <c r="N9" s="12">
+        <v>720417000</v>
+      </c>
+      <c r="O9" s="12">
+        <v>3825000</v>
+      </c>
+      <c r="P9" s="15">
+        <v>37841000</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>56575000</v>
+      </c>
+      <c r="R9" s="12">
+        <v>10757000</v>
+      </c>
+      <c r="S9" s="12">
+        <v>7261000</v>
+      </c>
+      <c r="T9" s="12">
+        <v>116259000</v>
+      </c>
+      <c r="U9" s="15">
+        <v>18186000</v>
+      </c>
+      <c r="V9" s="15">
+        <v>9605000</v>
+      </c>
+      <c r="W9" s="12">
+        <v>9499000</v>
+      </c>
+      <c r="X9" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>19139000</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>5926000</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>2235000</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>180849000</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>1549920000</v>
+      </c>
+      <c r="AD9" s="12">
+        <v>1336000</v>
+      </c>
+      <c r="AE9" s="12">
+        <v>-1011715000</v>
+      </c>
+      <c r="AF9" s="12">
+        <v>539568000</v>
+      </c>
+      <c r="AG9" s="12">
+        <v>720417000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>45230</v>
+      </c>
+      <c r="B10" s="7">
+        <v>101547000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>7880000</v>
+      </c>
+      <c r="D10" s="7">
+        <v>213347000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>45145000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>19616000</v>
+      </c>
+      <c r="G10" s="7">
+        <v>387535000</v>
+      </c>
+      <c r="H10" s="7">
+        <v>114058000</v>
+      </c>
+      <c r="I10" s="7">
+        <v>14050000</v>
+      </c>
+      <c r="J10" s="7">
+        <v>135701000</v>
+      </c>
+      <c r="K10" s="7">
+        <v>27427000</v>
+      </c>
+      <c r="L10" s="7">
+        <v>10321000</v>
+      </c>
+      <c r="M10" s="7">
+        <v>22091000</v>
+      </c>
+      <c r="N10" s="7">
+        <v>2337000</v>
+      </c>
+      <c r="O10" s="13">
+        <v>713520000</v>
+      </c>
+      <c r="P10" s="7">
+        <v>4589000</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>41961000</v>
+      </c>
+      <c r="R10" s="7">
+        <v>67228000</v>
+      </c>
+      <c r="S10" s="7">
+        <v>9860000</v>
+      </c>
+      <c r="T10" s="7">
+        <v>7500000</v>
+      </c>
+      <c r="U10" s="7">
+        <v>131138000</v>
+      </c>
+      <c r="V10" s="7">
+        <v>7763000</v>
+      </c>
+      <c r="W10" s="7">
+        <v>8353000</v>
+      </c>
+      <c r="X10" s="7">
+        <v>2666000</v>
+      </c>
+      <c r="Y10" s="7">
+        <v>17321000</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>5588000</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>7093000</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>179922000</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>1583531000</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>-242000</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>-1049719000</v>
+      </c>
+      <c r="AF10" s="7">
+        <v>533598000</v>
+      </c>
+      <c r="AG10" s="7">
+        <v>713520000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG10">
+    <sortCondition ref="A4:A10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD2C593-D154-4E49-995E-B05FC984C60F}">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>43677</v>
+      </c>
+      <c r="B2" s="6">
+        <v>23934000</v>
+      </c>
+      <c r="C2" s="6">
+        <v>25598250</v>
+      </c>
+      <c r="D2" s="6">
+        <v>-1664250</v>
+      </c>
+      <c r="E2" s="6">
+        <v>9467750</v>
+      </c>
+      <c r="F2" s="6">
+        <v>8728250</v>
+      </c>
+      <c r="G2" s="6">
+        <v>6754750</v>
+      </c>
+      <c r="H2" s="6">
+        <v>24950750</v>
+      </c>
+      <c r="I2" s="6">
+        <v>-26615000</v>
+      </c>
+      <c r="J2" s="6">
+        <v>-2882250</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>-1736500</v>
+      </c>
+      <c r="M2" s="6">
+        <v>51750</v>
+      </c>
+      <c r="N2" s="6">
+        <v>286000</v>
+      </c>
+      <c r="O2" s="6">
+        <v>-4281000</v>
+      </c>
+      <c r="P2" s="6">
+        <v>-30896000</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>32500</v>
+      </c>
+      <c r="R2" s="6">
+        <v>-30928500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>43769</v>
+      </c>
+      <c r="B3" s="6">
+        <v>23934000</v>
+      </c>
+      <c r="C3" s="6">
+        <v>25598250</v>
+      </c>
+      <c r="D3" s="6">
+        <v>-1664250</v>
+      </c>
+      <c r="E3" s="6">
+        <v>9467750</v>
+      </c>
+      <c r="F3" s="6">
+        <v>8728250</v>
+      </c>
+      <c r="G3" s="6">
+        <v>6754750</v>
+      </c>
+      <c r="H3" s="6">
+        <v>24950750</v>
+      </c>
+      <c r="I3" s="6">
+        <v>-26615000</v>
+      </c>
+      <c r="J3" s="6">
+        <v>-2882250</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>-1736500</v>
+      </c>
+      <c r="M3" s="6">
+        <v>51750</v>
+      </c>
+      <c r="N3" s="6">
+        <v>286000</v>
+      </c>
+      <c r="O3" s="6">
+        <v>-4281000</v>
+      </c>
+      <c r="P3" s="6">
+        <v>-30896000</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>32500</v>
+      </c>
+      <c r="R3" s="6">
+        <v>-30928500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>43861</v>
+      </c>
+      <c r="B4" s="6">
+        <v>23934000</v>
+      </c>
+      <c r="C4" s="6">
+        <v>25598250</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-1664250</v>
+      </c>
+      <c r="E4" s="6">
+        <v>9467750</v>
+      </c>
+      <c r="F4" s="6">
+        <v>8728250</v>
+      </c>
+      <c r="G4" s="6">
+        <v>6754750</v>
+      </c>
+      <c r="H4" s="6">
+        <v>24950750</v>
+      </c>
+      <c r="I4" s="6">
+        <v>-26615000</v>
+      </c>
+      <c r="J4" s="6">
+        <v>-2882250</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>-1736500</v>
+      </c>
+      <c r="M4" s="6">
+        <v>51750</v>
+      </c>
+      <c r="N4" s="6">
+        <v>286000</v>
+      </c>
+      <c r="O4" s="6">
+        <v>-4281000</v>
+      </c>
+      <c r="P4" s="6">
+        <v>-30896000</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>32500</v>
+      </c>
+      <c r="R4" s="6">
+        <v>-30928500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>43951</v>
+      </c>
+      <c r="B5" s="6">
+        <v>28292000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>21845750</v>
+      </c>
+      <c r="D5" s="6">
+        <v>6446250</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10956250</v>
+      </c>
+      <c r="F5" s="6">
+        <v>9317000</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8033500</v>
+      </c>
+      <c r="H5" s="6">
+        <v>28306750</v>
+      </c>
+      <c r="I5" s="6">
+        <v>-21860500</v>
+      </c>
+      <c r="J5" s="6">
+        <v>168250</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>-2361750</v>
+      </c>
+      <c r="M5" s="6">
+        <v>-7513250</v>
+      </c>
+      <c r="N5" s="6">
+        <v>59750</v>
+      </c>
+      <c r="O5" s="6">
+        <v>-9647000</v>
+      </c>
+      <c r="P5" s="6">
+        <v>-31507500</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>268250</v>
+      </c>
+      <c r="R5" s="6">
+        <v>-31775750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>43951</v>
+      </c>
+      <c r="B6" s="6">
+        <v>23934000</v>
+      </c>
+      <c r="C6" s="6">
+        <v>25598250</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-1664250</v>
+      </c>
+      <c r="E6" s="6">
+        <v>9467750</v>
+      </c>
+      <c r="F6" s="6">
+        <v>8728250</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6754750</v>
+      </c>
+      <c r="H6" s="6">
+        <v>24950750</v>
+      </c>
+      <c r="I6" s="6">
+        <v>-26615000</v>
+      </c>
+      <c r="J6" s="6">
+        <v>-2882250</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>-1736500</v>
+      </c>
+      <c r="M6" s="6">
+        <v>51750</v>
+      </c>
+      <c r="N6" s="6">
+        <v>286000</v>
+      </c>
+      <c r="O6" s="6">
+        <v>-4281000</v>
+      </c>
+      <c r="P6" s="6">
+        <v>-30896000</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>32500</v>
+      </c>
+      <c r="R6" s="6">
+        <v>-30928500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>44043</v>
+      </c>
+      <c r="B7" s="6">
+        <v>28292000</v>
+      </c>
+      <c r="C7" s="6">
+        <v>21845750</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6446250</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10956250</v>
+      </c>
+      <c r="F7" s="6">
+        <v>9317000</v>
+      </c>
+      <c r="G7" s="6">
+        <v>8033500</v>
+      </c>
+      <c r="H7" s="6">
+        <v>28306750</v>
+      </c>
+      <c r="I7" s="6">
+        <v>-21860500</v>
+      </c>
+      <c r="J7" s="6">
+        <v>168250</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>-2361750</v>
+      </c>
+      <c r="M7" s="6">
+        <v>-7513250</v>
+      </c>
+      <c r="N7" s="6">
+        <v>59750</v>
+      </c>
+      <c r="O7" s="6">
+        <v>-9647000</v>
+      </c>
+      <c r="P7" s="6">
+        <v>-31507500</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>268250</v>
+      </c>
+      <c r="R7" s="6">
+        <v>-31775750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>44135</v>
+      </c>
+      <c r="B8" s="6">
+        <v>28292000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>21845750</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6446250</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10956250</v>
+      </c>
+      <c r="F8" s="6">
+        <v>9317000</v>
+      </c>
+      <c r="G8" s="6">
+        <v>8033500</v>
+      </c>
+      <c r="H8" s="6">
+        <v>28306750</v>
+      </c>
+      <c r="I8" s="6">
+        <v>-21860500</v>
+      </c>
+      <c r="J8" s="6">
+        <v>168250</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>-2361750</v>
+      </c>
+      <c r="M8" s="6">
+        <v>-7513250</v>
+      </c>
+      <c r="N8" s="6">
+        <v>59750</v>
+      </c>
+      <c r="O8" s="6">
+        <v>-9647000</v>
+      </c>
+      <c r="P8" s="6">
+        <v>-31507500</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>268250</v>
+      </c>
+      <c r="R8" s="6">
+        <v>-31775750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>44227</v>
+      </c>
+      <c r="B9" s="6">
+        <v>28292000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>21845750</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6446250</v>
+      </c>
+      <c r="E9" s="6">
+        <v>10956250</v>
+      </c>
+      <c r="F9" s="6">
+        <v>9317000</v>
+      </c>
+      <c r="G9" s="6">
+        <v>8033500</v>
+      </c>
+      <c r="H9" s="6">
+        <v>28306750</v>
+      </c>
+      <c r="I9" s="6">
+        <v>-21860500</v>
+      </c>
+      <c r="J9" s="6">
+        <v>168250</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>-2361750</v>
+      </c>
+      <c r="M9" s="6">
+        <v>-7513250</v>
+      </c>
+      <c r="N9" s="6">
+        <v>59750</v>
+      </c>
+      <c r="O9" s="6">
+        <v>-9647000</v>
+      </c>
+      <c r="P9" s="6">
+        <v>-31507500</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>268250</v>
+      </c>
+      <c r="R9" s="6">
+        <v>-31775750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>44316</v>
+      </c>
+      <c r="B10" s="6">
+        <v>31957000</v>
+      </c>
+      <c r="C10" s="6">
+        <v>19126000</v>
+      </c>
+      <c r="D10" s="6">
+        <v>12831000</v>
+      </c>
+      <c r="E10" s="6">
+        <v>12130000</v>
+      </c>
+      <c r="F10" s="6">
+        <v>10653000</v>
+      </c>
+      <c r="G10" s="6">
+        <v>8315000</v>
+      </c>
+      <c r="H10" s="6">
+        <v>31098000</v>
+      </c>
+      <c r="I10" s="6">
+        <v>-18267000</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>-2527000</v>
+      </c>
+      <c r="M10" s="6">
+        <v>-8026000</v>
+      </c>
+      <c r="N10" s="6">
+        <v>-177000</v>
+      </c>
+      <c r="O10" s="6">
+        <v>-10730000</v>
+      </c>
+      <c r="P10" s="6">
+        <v>-28997000</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>258000</v>
+      </c>
+      <c r="R10" s="6">
+        <v>-29255000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>44408</v>
+      </c>
+      <c r="B11" s="6">
+        <v>30406000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>19820000</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10586000</v>
+      </c>
+      <c r="E11" s="6">
+        <v>12432000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>10597000</v>
+      </c>
+      <c r="G11" s="6">
+        <v>11824000</v>
+      </c>
+      <c r="H11" s="6">
+        <v>34853000</v>
+      </c>
+      <c r="I11" s="6">
+        <v>-24267000</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>-2611000</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>-84000</v>
+      </c>
+      <c r="O11" s="6">
+        <v>4074000</v>
+      </c>
+      <c r="P11" s="6">
+        <v>-20193000</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>170000</v>
+      </c>
+      <c r="R11" s="6">
+        <v>-20363000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>44500</v>
+      </c>
+      <c r="B12" s="6">
+        <v>31700000</v>
+      </c>
+      <c r="C12" s="6">
+        <v>20811000</v>
+      </c>
+      <c r="D12" s="6">
+        <v>10889000</v>
+      </c>
+      <c r="E12" s="6">
+        <v>14959000</v>
+      </c>
+      <c r="F12" s="6">
+        <v>12441000</v>
+      </c>
+      <c r="G12" s="6">
+        <v>11800000</v>
+      </c>
+      <c r="H12" s="6">
+        <v>39200000</v>
+      </c>
+      <c r="I12" s="6">
+        <v>-28311000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>8000</v>
+      </c>
+      <c r="L12" s="6">
+        <v>-2612000</v>
+      </c>
+      <c r="M12" s="6">
+        <v>-10172000</v>
+      </c>
+      <c r="N12" s="6">
+        <v>-60000</v>
+      </c>
+      <c r="O12" s="6">
+        <v>-12836000</v>
+      </c>
+      <c r="P12" s="6">
+        <v>-41147000</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>394000</v>
+      </c>
+      <c r="R12" s="6">
+        <v>-41541000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>44592</v>
+      </c>
+      <c r="B13" s="6">
+        <v>37146000</v>
+      </c>
+      <c r="C13" s="6">
+        <v>23230000</v>
+      </c>
+      <c r="D13" s="6">
+        <v>13916000</v>
+      </c>
+      <c r="E13" s="6">
+        <v>27163000</v>
+      </c>
+      <c r="F13" s="6">
+        <v>19226000</v>
+      </c>
+      <c r="G13" s="6">
+        <v>24733000</v>
+      </c>
+      <c r="H13" s="6">
+        <v>71122000</v>
+      </c>
+      <c r="I13" s="6">
+        <v>-57206000</v>
+      </c>
+      <c r="J13" s="6">
+        <v>-1690000</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>-1022000</v>
+      </c>
+      <c r="M13" s="6">
+        <v>23924000</v>
+      </c>
+      <c r="N13" s="6">
+        <v>-1906000</v>
+      </c>
+      <c r="O13" s="6">
+        <v>12529000</v>
+      </c>
+      <c r="P13" s="6">
+        <v>-44677000</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>1288000</v>
+      </c>
+      <c r="R13" s="6">
+        <v>-45965000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>44681</v>
+      </c>
+      <c r="B14" s="6">
+        <v>40127000</v>
+      </c>
+      <c r="C14" s="6">
+        <v>23628000</v>
+      </c>
+      <c r="D14" s="6">
+        <v>16499000</v>
+      </c>
+      <c r="E14" s="6">
+        <v>24750000</v>
+      </c>
+      <c r="F14" s="6">
+        <v>18855000</v>
+      </c>
+      <c r="G14" s="6">
+        <v>20608000</v>
+      </c>
+      <c r="H14" s="6">
+        <v>64213000</v>
+      </c>
+      <c r="I14" s="6">
+        <v>-47714000</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>3276000</v>
+      </c>
+      <c r="N14" s="6">
+        <v>392000</v>
+      </c>
+      <c r="O14" s="6">
+        <v>3668000</v>
+      </c>
+      <c r="P14" s="6">
+        <v>-44046000</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>314000</v>
+      </c>
+      <c r="R14" s="6">
+        <v>-44360000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>44773</v>
+      </c>
+      <c r="B15" s="6">
+        <v>48450000</v>
+      </c>
+      <c r="C15" s="6">
+        <v>24977000</v>
+      </c>
+      <c r="D15" s="6">
+        <v>23473000</v>
+      </c>
+      <c r="E15" s="6">
+        <v>26737000</v>
+      </c>
+      <c r="F15" s="6">
+        <v>19483000</v>
+      </c>
+      <c r="G15" s="6">
+        <v>19893000</v>
+      </c>
+      <c r="H15" s="6">
+        <v>66113000</v>
+      </c>
+      <c r="I15" s="6">
+        <v>-42640000</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1153000</v>
+      </c>
+      <c r="O15" s="6">
+        <v>3265000</v>
+      </c>
+      <c r="P15" s="6">
+        <v>-39375000</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>154000</v>
+      </c>
+      <c r="R15" s="6">
+        <v>-39529000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>44865</v>
+      </c>
+      <c r="B16" s="6">
+        <v>49704000</v>
+      </c>
+      <c r="C16" s="6">
+        <v>24728000</v>
+      </c>
+      <c r="D16" s="6">
+        <v>24976000</v>
+      </c>
+      <c r="E16" s="6">
+        <v>27598000</v>
+      </c>
+      <c r="F16" s="6">
+        <v>19383000</v>
+      </c>
+      <c r="G16" s="6">
+        <v>20627000</v>
+      </c>
+      <c r="H16" s="6">
+        <v>67608000</v>
+      </c>
+      <c r="I16" s="6">
+        <v>-42632000</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2853000</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>-19000</v>
+      </c>
+      <c r="N16" s="6">
+        <v>1000</v>
+      </c>
+      <c r="O16" s="6">
+        <v>2835000</v>
+      </c>
+      <c r="P16" s="6">
+        <v>-39797000</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>439000</v>
+      </c>
+      <c r="R16" s="6">
+        <v>-40236000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>44957</v>
+      </c>
+      <c r="B17" s="6">
+        <v>52975000</v>
+      </c>
+      <c r="C17" s="6">
+        <v>23915000</v>
+      </c>
+      <c r="D17" s="6">
+        <v>29060000</v>
+      </c>
+      <c r="E17" s="6">
+        <v>31831000</v>
+      </c>
+      <c r="F17" s="6">
+        <v>20299000</v>
+      </c>
+      <c r="G17" s="6">
+        <v>19619000</v>
+      </c>
+      <c r="H17" s="6">
+        <v>71749000</v>
+      </c>
+      <c r="I17" s="6">
+        <v>-42689000</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6">
+        <v>4819000</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="6">
+        <v>3297000</v>
+      </c>
+      <c r="N17" s="6">
+        <v>-1216000</v>
+      </c>
+      <c r="O17" s="6">
+        <v>4788000</v>
+      </c>
+      <c r="P17" s="6">
+        <v>-37901000</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>-60000</v>
+      </c>
+      <c r="R17" s="6">
+        <v>-37841000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>45046</v>
+      </c>
+      <c r="B18" s="6">
+        <v>52703000</v>
+      </c>
+      <c r="C18" s="6">
+        <v>24556000</v>
+      </c>
+      <c r="D18" s="6">
+        <v>28147000</v>
+      </c>
+      <c r="E18" s="6">
+        <v>28186000</v>
+      </c>
+      <c r="F18" s="6">
+        <v>23125000</v>
+      </c>
+      <c r="G18" s="6">
+        <v>21528000</v>
+      </c>
+      <c r="H18" s="6">
+        <v>72839000</v>
+      </c>
+      <c r="I18" s="6">
+        <v>-44692000</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <v>4506000</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6">
+        <v>-5945000</v>
+      </c>
+      <c r="N18" s="6">
+        <v>104000</v>
+      </c>
+      <c r="O18" s="6">
+        <v>10555000</v>
+      </c>
+      <c r="P18" s="6">
+        <v>-34137000</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>307000</v>
+      </c>
+      <c r="R18" s="6">
+        <v>-34444000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>45138</v>
+      </c>
+      <c r="B19" s="6">
+        <v>53761000</v>
+      </c>
+      <c r="C19" s="6">
+        <v>27469000</v>
+      </c>
+      <c r="D19" s="6">
+        <v>26292000</v>
+      </c>
+      <c r="E19" s="6">
+        <v>26741000</v>
+      </c>
+      <c r="F19" s="6">
+        <v>22310000</v>
+      </c>
+      <c r="G19" s="6">
+        <v>20521000</v>
+      </c>
+      <c r="H19" s="6">
+        <v>69572000</v>
+      </c>
+      <c r="I19" s="6">
+        <v>-43280000</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6">
+        <v>3802000</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
+      <c r="M19" s="6">
+        <v>1226000</v>
+      </c>
+      <c r="N19" s="6">
+        <v>859000</v>
+      </c>
+      <c r="O19" s="6">
+        <v>5887000</v>
+      </c>
+      <c r="P19" s="6">
+        <v>-37393000</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>582000</v>
+      </c>
+      <c r="R19" s="6">
+        <v>-37975000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>45230</v>
+      </c>
+      <c r="B20" s="6">
+        <v>55380000</v>
+      </c>
+      <c r="C20" s="6">
+        <v>29350000</v>
+      </c>
+      <c r="D20" s="6">
+        <v>26030000</v>
+      </c>
+      <c r="E20" s="6">
+        <v>33002000</v>
+      </c>
+      <c r="F20" s="6">
+        <v>20774000</v>
+      </c>
+      <c r="G20" s="6">
+        <v>20112000</v>
+      </c>
+      <c r="H20" s="6">
+        <v>73888000</v>
+      </c>
+      <c r="I20" s="6">
+        <v>-47858000</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <v>3445000</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" s="6">
+        <v>6833000</v>
+      </c>
+      <c r="N20" s="6">
+        <v>-69000</v>
+      </c>
+      <c r="O20" s="6">
+        <v>10209000</v>
+      </c>
+      <c r="P20" s="6">
+        <v>-37649000</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>355000</v>
+      </c>
+      <c r="R20" s="6">
+        <v>-38004000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R20">
+    <sortCondition ref="A4:A20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection sqref="A1:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,12 +3896,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9961904-157F-4234-8693-8A3031A539AB}">
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="T18" sqref="A1:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[ADD] update planet, add satellogic financial data
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\Downloads\planet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5571222F-429E-42BA-B80A-3ECDB0B54C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DFB521-A214-42F1-814B-8A0E8070C30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated" sheetId="3" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>Interest expense</t>
   </si>
   <si>
-    <t>Change in fair value of convertible notes and warrant liabilities</t>
-  </si>
-  <si>
     <t>Loss before provision for income taxes</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>Quarter</t>
+  </si>
+  <si>
+    <t>Change in fair value of financial instruments</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -325,6 +325,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -608,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -643,13 +653,13 @@
   <sheetData>
     <row r="1" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -676,7 +686,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
@@ -697,7 +707,7 @@
         <v>14</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>15</v>
@@ -715,10 +725,10 @@
         <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>19</v>
@@ -878,7 +888,7 @@
         <v>5743000</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M3" s="5">
         <v>2714000</v>
@@ -899,7 +909,7 @@
         <v>16135000</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T3" s="5">
         <v>132041000</v>
@@ -917,7 +927,7 @@
         <v>798000</v>
       </c>
       <c r="Y3" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z3" s="5">
         <v>0</v>
@@ -1664,7 +1674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD2C593-D154-4E49-995E-B05FC984C60F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1687,7 +1699,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>26</v>
@@ -1696,7 +1708,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
@@ -1714,31 +1726,31 @@
         <v>32</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2817,13 +2829,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection sqref="A1:J33"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.85546875" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -2900,7 +2912,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="7">
         <v>7880000</v>
@@ -3188,7 +3200,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="7">
         <v>10321000</v>
@@ -3206,7 +3218,7 @@
         <v>15806000</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="13">
         <v>7035000</v>
@@ -3412,7 +3424,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="7">
         <v>9860000</v>
@@ -3430,7 +3442,7 @@
         <v>3538000</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="13">
         <v>7188000</v>
@@ -3604,7 +3616,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="7">
         <v>17321000</v>
@@ -3622,7 +3634,7 @@
         <v>14024000</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="13">
         <v>2271000</v>
@@ -3636,7 +3648,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="7">
         <v>5588000</v>
@@ -3900,14 +3912,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9961904-157F-4234-8693-8A3031A539AB}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="T18" sqref="A1:T18"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" customWidth="1"/>
-    <col min="2" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -3971,7 +3984,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="6">
@@ -4033,7 +4046,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="6">
@@ -4095,8 +4108,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>41</v>
+      <c r="A4" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="6">
         <v>26030000</v>
@@ -4157,7 +4170,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="6">
@@ -4281,7 +4294,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="6">
@@ -4343,7 +4356,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="6">
@@ -4405,7 +4418,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="6">
@@ -4467,8 +4480,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>46</v>
+      <c r="A10" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B10" s="6">
         <v>0</v>
@@ -4530,7 +4543,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="6">
         <v>3445000</v>
@@ -4653,8 +4666,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
+      <c r="A13" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="B13" s="6">
         <v>6833000</v>
@@ -4715,8 +4728,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>47</v>
+      <c r="A14" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="B14" s="6">
         <v>-69000</v>
@@ -4777,8 +4790,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>48</v>
+      <c r="A15" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="6">
         <v>10209000</v>
@@ -4839,8 +4852,8 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
+      <c r="A16" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="6">
         <v>-37649000</v>
@@ -4901,8 +4914,8 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
+      <c r="A17" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="B17" s="6">
         <v>355000</v>
@@ -4963,8 +4976,8 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
+      <c r="A18" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="B18" s="6">
         <v>-38004000</v>
@@ -5023,6 +5036,9 @@
       <c r="T18" s="6">
         <v>-30928500</v>
       </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>

</xml_diff>

<commit_message>
[UPDATE] update  data, fixed 20231031 consolidated off-by-one error in pl.xlsx, update figs with new planet data
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6167F08-DA8B-4C86-9453-0346C937655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E6F741-1270-4179-A736-74B74A639E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated" sheetId="3" r:id="rId1"/>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -334,14 +334,17 @@
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,45 +627,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2:AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1372,100 +1374,100 @@
       <c r="A8" s="9">
         <v>45138</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="17">
         <v>118808000</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="17">
         <v>248979000</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="17">
         <v>40349000</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="17">
         <v>19725000</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="17">
         <v>427861000</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="17">
         <v>120193000</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="17">
         <v>12992000</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="17">
         <v>112750000</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="17">
         <v>14867000</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="17">
         <v>5707000</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="17">
         <v>23485000</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="17">
         <v>2562000</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="17">
         <v>720417000</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="17">
         <v>3825000</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="18">
         <v>37841000</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="18">
         <v>56575000</v>
       </c>
-      <c r="R8" s="12">
+      <c r="R8" s="17">
         <v>10757000</v>
       </c>
-      <c r="S8" s="12">
+      <c r="S8" s="17">
         <v>7261000</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8" s="17">
         <v>116259000</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="18">
         <v>18186000</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="18">
         <v>9605000</v>
       </c>
-      <c r="W8" s="12">
+      <c r="W8" s="17">
         <v>9499000</v>
       </c>
-      <c r="X8" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="12">
+      <c r="X8" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="17">
         <v>19139000</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="Z8" s="17">
         <v>5926000</v>
       </c>
-      <c r="AA8" s="12">
+      <c r="AA8" s="17">
         <v>2235000</v>
       </c>
-      <c r="AB8" s="12">
+      <c r="AB8" s="17">
         <v>180849000</v>
       </c>
-      <c r="AC8" s="12">
+      <c r="AC8" s="17">
         <v>1549920000</v>
       </c>
-      <c r="AD8" s="12">
+      <c r="AD8" s="17">
         <v>1336000</v>
       </c>
-      <c r="AE8" s="12">
+      <c r="AE8" s="17">
         <v>-1011715000</v>
       </c>
-      <c r="AF8" s="12">
+      <c r="AF8" s="17">
         <v>539568000</v>
       </c>
-      <c r="AG8" s="12">
+      <c r="AG8" s="17">
         <v>720417000</v>
       </c>
     </row>
@@ -1473,101 +1475,303 @@
       <c r="A9" s="9">
         <v>45230</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="17">
         <v>101547000</v>
       </c>
-      <c r="C9" s="7">
-        <v>7880000</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="17">
         <v>213347000</v>
       </c>
-      <c r="E9" s="7">
+      <c r="D9" s="17">
         <v>45145000</v>
       </c>
-      <c r="F9" s="7">
+      <c r="E9" s="17">
         <v>19616000</v>
       </c>
-      <c r="G9" s="7">
+      <c r="F9" s="17">
         <v>387535000</v>
       </c>
-      <c r="H9" s="7">
+      <c r="G9" s="17">
         <v>114058000</v>
       </c>
-      <c r="I9" s="7">
+      <c r="H9" s="17">
         <v>14050000</v>
       </c>
-      <c r="J9" s="7">
+      <c r="I9" s="17">
         <v>135701000</v>
       </c>
-      <c r="K9" s="7">
+      <c r="J9" s="17">
         <v>27427000</v>
       </c>
-      <c r="L9" s="7">
+      <c r="K9" s="17">
         <v>10321000</v>
       </c>
-      <c r="M9" s="7">
+      <c r="L9" s="17">
         <v>22091000</v>
       </c>
-      <c r="N9" s="7">
+      <c r="M9" s="17">
         <v>2337000</v>
       </c>
-      <c r="O9" s="13">
+      <c r="N9" s="17">
         <v>713520000</v>
       </c>
-      <c r="P9" s="7">
+      <c r="O9" s="17">
         <v>4589000</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="P9" s="17">
         <v>41961000</v>
       </c>
-      <c r="R9" s="7">
+      <c r="Q9" s="17">
         <v>67228000</v>
       </c>
-      <c r="S9" s="7">
+      <c r="R9" s="17">
         <v>9860000</v>
       </c>
-      <c r="T9" s="7">
+      <c r="S9" s="17">
         <v>7500000</v>
       </c>
-      <c r="U9" s="7">
+      <c r="T9" s="17">
         <v>131138000</v>
       </c>
-      <c r="V9" s="7">
+      <c r="U9" s="17">
         <v>7763000</v>
       </c>
-      <c r="W9" s="7">
+      <c r="V9" s="17">
         <v>8353000</v>
       </c>
-      <c r="X9" s="7">
+      <c r="W9" s="17">
         <v>2666000</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="X9" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="17">
         <v>17321000</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="17">
         <v>5588000</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AA9" s="17">
         <v>7093000</v>
       </c>
-      <c r="AB9" s="7">
+      <c r="AB9" s="17">
         <v>179922000</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AC9" s="17">
         <v>1583531000</v>
       </c>
-      <c r="AD9" s="7">
+      <c r="AD9" s="17">
         <v>-242000</v>
       </c>
-      <c r="AE9" s="7">
+      <c r="AE9" s="17">
         <v>-1049719000</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AF9" s="17">
         <v>533598000</v>
       </c>
-      <c r="AG9" s="7">
+      <c r="AG9" s="17">
         <v>713520000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>45322</v>
+      </c>
+      <c r="B10" s="7">
+        <v>83866000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>215041000</v>
+      </c>
+      <c r="D10" s="7">
+        <v>43320000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>19564000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>370151000</v>
+      </c>
+      <c r="G10" s="7">
+        <v>113429000</v>
+      </c>
+      <c r="H10" s="7">
+        <v>14973000</v>
+      </c>
+      <c r="I10" s="7">
+        <v>136256000</v>
+      </c>
+      <c r="J10" s="7">
+        <v>32448000</v>
+      </c>
+      <c r="K10" s="7">
+        <v>9972000</v>
+      </c>
+      <c r="L10" s="7">
+        <v>22339000</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2429000</v>
+      </c>
+      <c r="N10" s="7">
+        <v>701997000</v>
+      </c>
+      <c r="O10" s="7">
+        <v>2601000</v>
+      </c>
+      <c r="P10" s="7">
+        <v>44779000</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>72327000</v>
+      </c>
+      <c r="R10" s="7">
+        <v>8964000</v>
+      </c>
+      <c r="S10" s="7">
+        <v>7978000</v>
+      </c>
+      <c r="T10" s="7">
+        <v>136649000</v>
+      </c>
+      <c r="U10" s="7">
+        <v>5293000</v>
+      </c>
+      <c r="V10" s="7">
+        <v>7101000</v>
+      </c>
+      <c r="W10" s="7">
+        <v>2961000</v>
+      </c>
+      <c r="X10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="7">
+        <v>16952000</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>5885000</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>9138000</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>183979000</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>1596201000</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>1594000</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>-1079805000</v>
+      </c>
+      <c r="AF10" s="7">
+        <v>518018000</v>
+      </c>
+      <c r="AG10" s="7">
+        <v>701997000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>45412</v>
+      </c>
+      <c r="B11" s="7">
+        <v>107367000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>168218000</v>
+      </c>
+      <c r="D11" s="7">
+        <v>38527000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>23044000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>345958000</v>
+      </c>
+      <c r="G11" s="7">
+        <v>111338000</v>
+      </c>
+      <c r="H11" s="7">
+        <v>16066000</v>
+      </c>
+      <c r="I11" s="7">
+        <v>137110000</v>
+      </c>
+      <c r="J11" s="7">
+        <v>31403000</v>
+      </c>
+      <c r="K11" s="7">
+        <v>9564000</v>
+      </c>
+      <c r="L11" s="7">
+        <v>20966000</v>
+      </c>
+      <c r="M11" s="7">
+        <v>2199000</v>
+      </c>
+      <c r="N11" s="7">
+        <v>674604000</v>
+      </c>
+      <c r="O11" s="7">
+        <v>3131000</v>
+      </c>
+      <c r="P11" s="7">
+        <v>43361000</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>63646000</v>
+      </c>
+      <c r="R11" s="7">
+        <v>8068000</v>
+      </c>
+      <c r="S11" s="7">
+        <v>8175000</v>
+      </c>
+      <c r="T11" s="7">
+        <v>126381000</v>
+      </c>
+      <c r="U11" s="7">
+        <v>13247000</v>
+      </c>
+      <c r="V11" s="7">
+        <v>9261000</v>
+      </c>
+      <c r="W11" s="7">
+        <v>1431000</v>
+      </c>
+      <c r="X11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>15207000</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>2915000</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>5837000</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>174279000</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>1608847000</v>
+      </c>
+      <c r="AD11" s="7">
+        <v>548000</v>
+      </c>
+      <c r="AE11" s="7">
+        <v>-1109098000</v>
+      </c>
+      <c r="AF11" s="7">
+        <v>500325000</v>
+      </c>
+      <c r="AG11" s="7">
+        <v>674604000</v>
       </c>
     </row>
   </sheetData>
@@ -1581,16 +1785,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD2C593-D154-4E49-995E-B05FC984C60F}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
@@ -1607,7 +1812,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1643,7 +1848,7 @@
       <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>49</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -2502,7 +2707,7 @@
         <v>-40236000</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>44957</v>
       </c>
@@ -2558,7 +2763,7 @@
         <v>-37841000</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>45046</v>
       </c>
@@ -2614,7 +2819,7 @@
         <v>-34444000</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>45138</v>
       </c>
@@ -2670,7 +2875,7 @@
         <v>-37975000</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>45230</v>
       </c>
@@ -2724,6 +2929,163 @@
       </c>
       <c r="R20" s="6">
         <v>-38004000</v>
+      </c>
+      <c r="S20" s="12">
+        <v>7500000</v>
+      </c>
+      <c r="T20" s="12">
+        <v>131138000</v>
+      </c>
+      <c r="U20" s="12">
+        <v>7763000</v>
+      </c>
+      <c r="V20" s="12">
+        <v>8353000</v>
+      </c>
+      <c r="W20" s="12">
+        <v>2666000</v>
+      </c>
+      <c r="X20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="12">
+        <v>17321000</v>
+      </c>
+      <c r="Z20" s="12">
+        <v>5588000</v>
+      </c>
+      <c r="AA20" s="12">
+        <v>7093000</v>
+      </c>
+      <c r="AB20" s="12">
+        <v>179922000</v>
+      </c>
+      <c r="AC20" s="12">
+        <v>1583531000</v>
+      </c>
+      <c r="AD20" s="12">
+        <v>-242000</v>
+      </c>
+      <c r="AE20" s="12">
+        <v>-1049719000</v>
+      </c>
+      <c r="AF20" s="12">
+        <v>533598000</v>
+      </c>
+      <c r="AG20" s="12">
+        <v>713520000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>45322</v>
+      </c>
+      <c r="B21" s="6">
+        <v>220696000</v>
+      </c>
+      <c r="C21" s="6">
+        <v>107746000</v>
+      </c>
+      <c r="D21" s="6">
+        <v>112950000</v>
+      </c>
+      <c r="E21" s="6">
+        <v>116339000</v>
+      </c>
+      <c r="F21" s="6">
+        <v>86304000</v>
+      </c>
+      <c r="G21" s="6">
+        <v>80055000</v>
+      </c>
+      <c r="H21" s="6">
+        <v>282698000</v>
+      </c>
+      <c r="I21" s="6">
+        <v>-169748000</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>15414000</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>13709000</v>
+      </c>
+      <c r="N21" s="6">
+        <v>931000</v>
+      </c>
+      <c r="O21" s="6">
+        <v>30054000</v>
+      </c>
+      <c r="P21" s="6">
+        <v>-139694000</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>815000</v>
+      </c>
+      <c r="R21" s="6">
+        <v>-140509000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>45412</v>
+      </c>
+      <c r="B22" s="6">
+        <v>60440000</v>
+      </c>
+      <c r="C22" s="6">
+        <v>28757000</v>
+      </c>
+      <c r="D22" s="6">
+        <v>31683000</v>
+      </c>
+      <c r="E22" s="6">
+        <v>25589000</v>
+      </c>
+      <c r="F22" s="6">
+        <v>21485000</v>
+      </c>
+      <c r="G22" s="6">
+        <v>19180000</v>
+      </c>
+      <c r="H22" s="6">
+        <v>66254000</v>
+      </c>
+      <c r="I22" s="6">
+        <v>-34571000</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
+        <v>3107000</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>1530000</v>
+      </c>
+      <c r="N22" s="6">
+        <v>1083000</v>
+      </c>
+      <c r="O22" s="6">
+        <v>5720000</v>
+      </c>
+      <c r="P22" s="6">
+        <v>-28851000</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>442000</v>
+      </c>
+      <c r="R22" s="6">
+        <v>-29293000</v>
       </c>
     </row>
   </sheetData>
@@ -2736,1080 +3098,1448 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A33"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="9">
+        <v>45412</v>
+      </c>
+      <c r="C1" s="9">
+        <v>45322</v>
+      </c>
+      <c r="D1" s="9">
         <v>45230</v>
       </c>
-      <c r="C1" s="9">
+      <c r="E1" s="9">
         <v>45138</v>
       </c>
-      <c r="D1" s="9">
+      <c r="F1" s="9">
         <v>45046</v>
       </c>
-      <c r="E1" s="9">
+      <c r="G1" s="9">
         <v>44957</v>
       </c>
-      <c r="F1" s="9">
+      <c r="H1" s="9">
         <v>44865</v>
       </c>
-      <c r="G1" s="9">
+      <c r="I1" s="9">
         <v>44592</v>
       </c>
-      <c r="H1" s="10">
+      <c r="J1" s="10">
         <v>44681</v>
       </c>
-      <c r="I1" s="10">
+      <c r="K1" s="10">
         <v>44592</v>
       </c>
-      <c r="J1" s="10">
+      <c r="L1" s="10">
         <v>44227</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
+        <v>107367000</v>
+      </c>
+      <c r="C2" s="7">
+        <v>83866000</v>
+      </c>
+      <c r="D2" s="17">
         <v>101547000</v>
       </c>
-      <c r="C2" s="12">
+      <c r="E2" s="17">
         <v>118808000</v>
       </c>
-      <c r="D2" s="5">
+      <c r="F2" s="5">
         <v>140763000</v>
       </c>
-      <c r="E2" s="5">
+      <c r="G2" s="5">
         <v>181892000</v>
       </c>
-      <c r="F2" s="5">
+      <c r="H2" s="5">
         <v>199124000</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>490762000</v>
       </c>
-      <c r="H2" s="13">
+      <c r="J2" s="13">
         <v>484489000</v>
       </c>
-      <c r="I2" s="13">
+      <c r="K2" s="13">
         <v>490762000</v>
       </c>
-      <c r="J2" s="13">
+      <c r="L2" s="13">
         <v>71183000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="7">
-        <v>7880000</v>
-      </c>
-      <c r="C3" s="12">
+        <v>168218000</v>
+      </c>
+      <c r="C3" s="7">
+        <v>215041000</v>
+      </c>
+      <c r="D3" s="17">
+        <v>213347000</v>
+      </c>
+      <c r="E3" s="17">
         <v>248979000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="F3" s="5">
         <v>235415000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="G3" s="5">
         <v>226868000</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H3" s="5">
         <v>226163000</v>
       </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13">
+      <c r="I3" s="5">
         <v>0</v>
       </c>
       <c r="J3" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>213347000</v>
-      </c>
-      <c r="C4" s="12">
+        <v>38527000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>43320000</v>
+      </c>
+      <c r="D4" s="17">
+        <v>45145000</v>
+      </c>
+      <c r="E4" s="17">
         <v>40349000</v>
       </c>
-      <c r="D4" s="5">
+      <c r="F4" s="5">
         <v>39072000</v>
       </c>
-      <c r="E4" s="5">
+      <c r="G4" s="5">
         <v>38952000</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="5">
         <v>29009000</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>44373000</v>
       </c>
-      <c r="H4" s="13">
+      <c r="J4" s="13">
         <v>24581000</v>
       </c>
-      <c r="I4" s="13">
+      <c r="K4" s="13">
         <v>44373000</v>
       </c>
-      <c r="J4" s="13">
+      <c r="L4" s="13">
         <v>47110000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>45145000</v>
-      </c>
-      <c r="C5" s="12">
+        <v>23044000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>19564000</v>
+      </c>
+      <c r="D5" s="17">
+        <v>19616000</v>
+      </c>
+      <c r="E5" s="17">
         <v>19725000</v>
       </c>
-      <c r="D5" s="5">
+      <c r="F5" s="5">
         <v>19275000</v>
       </c>
-      <c r="E5" s="5">
+      <c r="G5" s="5">
         <v>27943000</v>
       </c>
-      <c r="F5" s="5">
+      <c r="H5" s="5">
         <v>26347000</v>
       </c>
-      <c r="G5" s="5">
+      <c r="I5" s="5">
         <v>16385000</v>
       </c>
-      <c r="H5" s="13">
+      <c r="J5" s="13">
         <v>18192000</v>
       </c>
-      <c r="I5" s="13">
+      <c r="K5" s="13">
         <v>16385000</v>
       </c>
-      <c r="J5" s="13">
+      <c r="L5" s="13">
         <v>7134000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>19616000</v>
-      </c>
-      <c r="C6" s="12">
+        <v>345958000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>370151000</v>
+      </c>
+      <c r="D6" s="17">
+        <v>387535000</v>
+      </c>
+      <c r="E6" s="17">
         <v>427861000</v>
       </c>
-      <c r="D6" s="5">
+      <c r="F6" s="5">
         <v>434525000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="G6" s="5">
         <v>475655000</v>
       </c>
-      <c r="F6" s="5">
+      <c r="H6" s="5">
         <v>480643000</v>
       </c>
-      <c r="G6" s="5">
+      <c r="I6" s="5">
         <v>551520000</v>
       </c>
-      <c r="H6" s="13">
+      <c r="J6" s="13">
         <v>527262000</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>551520000</v>
       </c>
-      <c r="J6" s="13">
+      <c r="L6" s="13">
         <v>125427000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="7">
-        <v>387535000</v>
-      </c>
-      <c r="C7" s="12">
+        <v>111338000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>113429000</v>
+      </c>
+      <c r="D7" s="17">
+        <v>114058000</v>
+      </c>
+      <c r="E7" s="17">
         <v>120193000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="F7" s="5">
         <v>118193000</v>
       </c>
-      <c r="E7" s="5">
+      <c r="G7" s="5">
         <v>108091000</v>
       </c>
-      <c r="F7" s="5">
+      <c r="H7" s="5">
         <v>115385000</v>
       </c>
-      <c r="G7" s="5">
+      <c r="I7" s="5">
         <v>133280000</v>
       </c>
-      <c r="H7" s="13">
+      <c r="J7" s="13">
         <v>125329000</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>133280000</v>
       </c>
-      <c r="J7" s="13">
+      <c r="L7" s="13">
         <v>159855000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7">
-        <v>114058000</v>
-      </c>
-      <c r="C8" s="12">
+        <v>16066000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>14973000</v>
+      </c>
+      <c r="D8" s="17">
+        <v>14050000</v>
+      </c>
+      <c r="E8" s="17">
         <v>12992000</v>
       </c>
-      <c r="D8" s="5">
+      <c r="F8" s="5">
         <v>11878000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="G8" s="5">
         <v>11417000</v>
       </c>
-      <c r="F8" s="5">
+      <c r="H8" s="5">
         <v>11181000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="I8" s="5">
         <v>10768000</v>
       </c>
-      <c r="H8" s="13">
+      <c r="J8" s="13">
         <v>11105000</v>
       </c>
-      <c r="I8" s="13">
+      <c r="K8" s="13">
         <v>10768000</v>
       </c>
-      <c r="J8" s="13">
+      <c r="L8" s="13">
         <v>11994000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7">
-        <v>14050000</v>
-      </c>
-      <c r="C9" s="12">
+        <v>137110000</v>
+      </c>
+      <c r="C9" s="7">
+        <v>136256000</v>
+      </c>
+      <c r="D9" s="17">
+        <v>135701000</v>
+      </c>
+      <c r="E9" s="17">
         <v>112750000</v>
       </c>
-      <c r="D9" s="5">
+      <c r="F9" s="5">
         <v>112748000</v>
       </c>
-      <c r="E9" s="5">
+      <c r="G9" s="5">
         <v>112748000</v>
       </c>
-      <c r="F9" s="5">
+      <c r="H9" s="5">
         <v>103219000</v>
       </c>
-      <c r="G9" s="5">
+      <c r="I9" s="5">
         <v>103219000</v>
       </c>
-      <c r="H9" s="13">
+      <c r="J9" s="13">
         <v>103219000</v>
       </c>
-      <c r="I9" s="13">
+      <c r="K9" s="13">
         <v>103219000</v>
       </c>
-      <c r="J9" s="13">
+      <c r="L9" s="13">
         <v>88393000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7">
-        <v>135701000</v>
-      </c>
-      <c r="C10" s="12">
+        <v>31403000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>32448000</v>
+      </c>
+      <c r="D10" s="17">
+        <v>27427000</v>
+      </c>
+      <c r="E10" s="17">
         <v>14867000</v>
       </c>
-      <c r="D10" s="5">
+      <c r="F10" s="5">
         <v>13999000</v>
       </c>
-      <c r="E10" s="5">
+      <c r="G10" s="5">
         <v>14831000</v>
       </c>
-      <c r="F10" s="5">
+      <c r="H10" s="5">
         <v>12419000</v>
       </c>
-      <c r="G10" s="5">
+      <c r="I10" s="5">
         <v>14197000</v>
       </c>
-      <c r="H10" s="13">
+      <c r="J10" s="13">
         <v>13604000</v>
       </c>
-      <c r="I10" s="13">
+      <c r="K10" s="13">
         <v>14197000</v>
       </c>
-      <c r="J10" s="13">
+      <c r="L10" s="13">
         <v>5673000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="7">
-        <v>27427000</v>
-      </c>
-      <c r="C11" s="12">
+        <v>9564000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>9972000</v>
+      </c>
+      <c r="D11" s="17">
+        <v>10321000</v>
+      </c>
+      <c r="E11" s="17">
         <v>5707000</v>
       </c>
-      <c r="D11" s="5">
+      <c r="F11" s="5">
         <v>5660000</v>
       </c>
-      <c r="E11" s="5">
+      <c r="G11" s="5">
         <v>5657000</v>
       </c>
-      <c r="F11" s="5">
+      <c r="H11" s="5">
         <v>5163000</v>
       </c>
-      <c r="G11" s="5">
+      <c r="I11" s="5">
         <v>5743000</v>
       </c>
-      <c r="H11" s="13">
+      <c r="J11" s="13">
         <v>5653000</v>
       </c>
-      <c r="I11" s="13">
+      <c r="K11" s="13">
         <v>5743000</v>
       </c>
-      <c r="J11" s="13">
+      <c r="L11" s="13">
         <v>4982000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="7">
-        <v>10321000</v>
-      </c>
-      <c r="C12" s="12">
+        <v>20966000</v>
+      </c>
+      <c r="C12" s="7">
+        <v>22339000</v>
+      </c>
+      <c r="D12" s="17">
+        <v>22091000</v>
+      </c>
+      <c r="E12" s="17">
         <v>23485000</v>
       </c>
-      <c r="D12" s="5">
+      <c r="F12" s="5">
         <v>23697000</v>
       </c>
-      <c r="E12" s="5">
+      <c r="G12" s="5">
         <v>20403000</v>
       </c>
-      <c r="F12" s="5">
+      <c r="H12" s="5">
         <v>15806000</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="13">
+      <c r="J12" s="13">
         <v>7035000</v>
       </c>
-      <c r="I12" s="13">
-        <v>0</v>
-      </c>
-      <c r="J12" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7">
-        <v>22091000</v>
-      </c>
-      <c r="C13" s="12">
+        <v>2199000</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2429000</v>
+      </c>
+      <c r="D13" s="17">
+        <v>2337000</v>
+      </c>
+      <c r="E13" s="17">
         <v>2562000</v>
       </c>
-      <c r="D13" s="5">
+      <c r="F13" s="5">
         <v>2757000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="G13" s="5">
         <v>3921000</v>
       </c>
-      <c r="F13" s="5">
+      <c r="H13" s="5">
         <v>3412000</v>
       </c>
-      <c r="G13" s="5">
+      <c r="I13" s="5">
         <v>2714000</v>
       </c>
-      <c r="H13" s="13">
+      <c r="J13" s="13">
         <v>2787000</v>
       </c>
-      <c r="I13" s="13">
+      <c r="K13" s="13">
         <v>2714000</v>
       </c>
-      <c r="J13" s="13">
+      <c r="L13" s="13">
         <v>2984000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="7">
-        <v>2337000</v>
-      </c>
-      <c r="C14" s="12">
+        <v>674604000</v>
+      </c>
+      <c r="C14" s="7">
+        <v>701997000</v>
+      </c>
+      <c r="D14" s="17">
+        <v>713520000</v>
+      </c>
+      <c r="E14" s="17">
         <v>720417000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="F14" s="5">
         <v>723457000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="G14" s="5">
         <v>752723000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="H14" s="5">
         <v>747228000</v>
       </c>
-      <c r="G14" s="5">
+      <c r="I14" s="5">
         <v>821441000</v>
       </c>
-      <c r="H14" s="13">
+      <c r="J14" s="13">
         <v>795994000</v>
       </c>
-      <c r="I14" s="13">
+      <c r="K14" s="13">
         <v>821441000</v>
       </c>
-      <c r="J14" s="13">
+      <c r="L14" s="13">
         <v>399308000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="13">
-        <v>713520000</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="B15" s="7">
+        <v>3131000</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2601000</v>
+      </c>
+      <c r="D15" s="17">
+        <v>4589000</v>
+      </c>
+      <c r="E15" s="17">
         <v>3825000</v>
       </c>
-      <c r="D15" s="5">
+      <c r="F15" s="5">
         <v>14657000</v>
       </c>
-      <c r="E15" s="5">
+      <c r="G15" s="5">
         <v>6900000</v>
       </c>
-      <c r="F15" s="5">
+      <c r="H15" s="5">
         <v>2557000</v>
       </c>
-      <c r="G15" s="5">
+      <c r="I15" s="5">
         <v>2850000</v>
       </c>
-      <c r="H15" s="13">
+      <c r="J15" s="13">
         <v>3168000</v>
       </c>
-      <c r="I15" s="13">
+      <c r="K15" s="13">
         <v>2850000</v>
       </c>
-      <c r="J15" s="13">
+      <c r="L15" s="13">
         <v>1446000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="7">
-        <v>4589000</v>
-      </c>
-      <c r="C16" s="15">
+        <v>43361000</v>
+      </c>
+      <c r="C16" s="7">
+        <v>44779000</v>
+      </c>
+      <c r="D16" s="17">
+        <v>41961000</v>
+      </c>
+      <c r="E16" s="18">
         <v>37841000</v>
       </c>
-      <c r="D16" s="5">
+      <c r="F16" s="5">
         <v>34432000</v>
       </c>
-      <c r="E16" s="5">
+      <c r="G16" s="5">
         <v>46022000</v>
       </c>
-      <c r="F16" s="5">
+      <c r="H16" s="5">
         <v>42629000</v>
       </c>
-      <c r="G16" s="5">
+      <c r="I16" s="5">
         <v>48823000</v>
       </c>
-      <c r="H16" s="13">
+      <c r="J16" s="13">
         <v>43184000</v>
       </c>
-      <c r="I16" s="13">
+      <c r="K16" s="13">
         <v>48823000</v>
       </c>
-      <c r="J16" s="13">
+      <c r="L16" s="13">
         <v>30195000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="7">
-        <v>41961000</v>
-      </c>
-      <c r="C17" s="15">
+        <v>63646000</v>
+      </c>
+      <c r="C17" s="7">
+        <v>72327000</v>
+      </c>
+      <c r="D17" s="17">
+        <v>67228000</v>
+      </c>
+      <c r="E17" s="18">
         <v>56575000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="F17" s="5">
         <v>44620000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="G17" s="5">
         <v>51900000</v>
       </c>
-      <c r="F17" s="5">
+      <c r="H17" s="5">
         <v>47698000</v>
       </c>
-      <c r="G17" s="5">
+      <c r="I17" s="5">
         <v>64233000</v>
       </c>
-      <c r="H17" s="13">
+      <c r="J17" s="13">
         <v>60672000</v>
       </c>
-      <c r="I17" s="13">
+      <c r="K17" s="13">
         <v>64233000</v>
       </c>
-      <c r="J17" s="13">
+      <c r="L17" s="13">
         <v>57570000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="7">
-        <v>67228000</v>
-      </c>
-      <c r="C18" s="12">
+        <v>8068000</v>
+      </c>
+      <c r="C18" s="7">
+        <v>8964000</v>
+      </c>
+      <c r="D18" s="17">
+        <v>9860000</v>
+      </c>
+      <c r="E18" s="17">
         <v>10757000</v>
       </c>
-      <c r="D18" s="5">
+      <c r="F18" s="5">
         <v>11653000</v>
       </c>
-      <c r="E18" s="5">
+      <c r="G18" s="5">
         <v>12550000</v>
       </c>
-      <c r="F18" s="5">
+      <c r="H18" s="5">
         <v>13446000</v>
       </c>
-      <c r="G18" s="5">
+      <c r="I18" s="5">
         <v>16135000</v>
       </c>
-      <c r="H18" s="13">
+      <c r="J18" s="13">
         <v>15239000</v>
       </c>
-      <c r="I18" s="13">
+      <c r="K18" s="13">
         <v>16135000</v>
       </c>
-      <c r="J18" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="7">
-        <v>9860000</v>
-      </c>
-      <c r="C19" s="12">
+        <v>8175000</v>
+      </c>
+      <c r="C19" s="7">
+        <v>7978000</v>
+      </c>
+      <c r="D19" s="17">
+        <v>7500000</v>
+      </c>
+      <c r="E19" s="17">
         <v>7261000</v>
       </c>
-      <c r="D19" s="5">
+      <c r="F19" s="5">
         <v>6320000</v>
       </c>
-      <c r="E19" s="5">
+      <c r="G19" s="5">
         <v>4885000</v>
       </c>
-      <c r="F19" s="5">
+      <c r="H19" s="5">
         <v>3538000</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="I19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="13">
+      <c r="J19" s="13">
         <v>7188000</v>
       </c>
-      <c r="I19" s="13">
-        <v>0</v>
-      </c>
-      <c r="J19" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="7">
-        <v>7500000</v>
-      </c>
-      <c r="C20" s="12">
+        <v>126381000</v>
+      </c>
+      <c r="C20" s="7">
+        <v>136649000</v>
+      </c>
+      <c r="D20" s="17">
+        <v>131138000</v>
+      </c>
+      <c r="E20" s="17">
         <v>116259000</v>
       </c>
-      <c r="D20" s="5">
+      <c r="F20" s="5">
         <v>111682000</v>
       </c>
-      <c r="E20" s="5">
+      <c r="G20" s="5">
         <v>122257000</v>
       </c>
-      <c r="F20" s="5">
+      <c r="H20" s="5">
         <v>109868000</v>
       </c>
-      <c r="G20" s="5">
+      <c r="I20" s="5">
         <v>132041000</v>
       </c>
-      <c r="H20" s="13">
+      <c r="J20" s="13">
         <v>129451000</v>
       </c>
-      <c r="I20" s="13">
+      <c r="K20" s="13">
         <v>132041000</v>
       </c>
-      <c r="J20" s="13">
+      <c r="L20" s="13">
         <v>108814000</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="7">
-        <v>131138000</v>
-      </c>
-      <c r="C21" s="15">
+        <v>13247000</v>
+      </c>
+      <c r="C21" s="7">
+        <v>5293000</v>
+      </c>
+      <c r="D21" s="17">
+        <v>7763000</v>
+      </c>
+      <c r="E21" s="18">
         <v>18186000</v>
       </c>
-      <c r="D21" s="5">
+      <c r="F21" s="5">
         <v>2474000</v>
       </c>
-      <c r="E21" s="5">
+      <c r="G21" s="5">
         <v>2882000</v>
       </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
         <v>3579000</v>
       </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13">
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
         <v>3579000</v>
       </c>
-      <c r="J21" s="13">
+      <c r="L21" s="13">
         <v>15122000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="7">
-        <v>7763000</v>
-      </c>
-      <c r="C22" s="15">
+        <v>9261000</v>
+      </c>
+      <c r="C22" s="7">
+        <v>7101000</v>
+      </c>
+      <c r="D22" s="17">
+        <v>8353000</v>
+      </c>
+      <c r="E22" s="18">
         <v>9605000</v>
       </c>
-      <c r="D22" s="5">
+      <c r="F22" s="5">
         <v>10671000</v>
       </c>
-      <c r="E22" s="5">
+      <c r="G22" s="5">
         <v>8679000</v>
       </c>
-      <c r="F22" s="5">
+      <c r="H22" s="5">
         <v>9853000</v>
       </c>
-      <c r="G22" s="5">
+      <c r="I22" s="5">
         <v>12149000</v>
       </c>
-      <c r="H22" s="13">
+      <c r="J22" s="13">
         <v>12199000</v>
       </c>
-      <c r="I22" s="13">
+      <c r="K22" s="13">
         <v>12149000</v>
       </c>
-      <c r="J22" s="13">
+      <c r="L22" s="13">
         <v>7971000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="7">
-        <v>8353000</v>
-      </c>
-      <c r="C23" s="12">
+        <v>1431000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2961000</v>
+      </c>
+      <c r="D23" s="17">
+        <v>2666000</v>
+      </c>
+      <c r="E23" s="17">
         <v>9499000</v>
       </c>
-      <c r="D23" s="5">
+      <c r="F23" s="5">
         <v>10725000</v>
       </c>
-      <c r="E23" s="5">
+      <c r="G23" s="5">
         <v>16670000</v>
       </c>
-      <c r="F23" s="5">
+      <c r="H23" s="5">
         <v>17855000</v>
       </c>
-      <c r="G23" s="5">
+      <c r="I23" s="5">
         <v>23224000</v>
       </c>
-      <c r="H23" s="13">
+      <c r="J23" s="13">
         <v>19948000</v>
       </c>
-      <c r="I23" s="13">
+      <c r="K23" s="13">
         <v>23224000</v>
       </c>
-      <c r="J23" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="7">
-        <v>2666000</v>
-      </c>
-      <c r="C24" s="12">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="17">
+        <v>0</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
         <v>19912000</v>
       </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0</v>
-      </c>
       <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
         <v>798000</v>
       </c>
-      <c r="H24" s="13">
-        <v>0</v>
-      </c>
-      <c r="I24" s="13">
+      <c r="J24" s="13">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
         <v>798000</v>
       </c>
-      <c r="J24" s="13">
+      <c r="L24" s="13">
         <v>2991000</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="7">
+        <v>15207000</v>
+      </c>
+      <c r="C25" s="7">
+        <v>16952000</v>
+      </c>
+      <c r="D25" s="17">
         <v>17321000</v>
       </c>
-      <c r="C25" s="12">
+      <c r="E25" s="17">
         <v>19139000</v>
       </c>
-      <c r="D25" s="5">
+      <c r="F25" s="5">
         <v>7142000</v>
       </c>
-      <c r="E25" s="5">
+      <c r="G25" s="5">
         <v>17145000</v>
       </c>
-      <c r="F25" s="5">
+      <c r="H25" s="5">
         <v>14024000</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="I25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H25" s="13">
+      <c r="J25" s="13">
         <v>2271000</v>
       </c>
-      <c r="I25" s="13">
-        <v>0</v>
-      </c>
-      <c r="J25" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="7">
+        <v>2915000</v>
+      </c>
+      <c r="C26" s="7">
+        <v>5885000</v>
+      </c>
+      <c r="D26" s="17">
         <v>5588000</v>
       </c>
-      <c r="C26" s="12">
+      <c r="E26" s="17">
         <v>5926000</v>
       </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
         <v>7499000</v>
       </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="13">
-        <v>0</v>
-      </c>
-      <c r="I26" s="13">
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
         <v>0</v>
       </c>
       <c r="J26" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="7">
+        <v>5837000</v>
+      </c>
+      <c r="C27" s="7">
+        <v>9138000</v>
+      </c>
+      <c r="D27" s="17">
         <v>7093000</v>
       </c>
-      <c r="C27" s="12">
+      <c r="E27" s="17">
         <v>2235000</v>
       </c>
-      <c r="D27" s="5">
+      <c r="F27" s="5">
         <v>1502000</v>
       </c>
-      <c r="E27" s="5">
+      <c r="G27" s="5">
         <v>1487000</v>
       </c>
-      <c r="F27" s="5">
+      <c r="H27" s="5">
         <v>1461000</v>
       </c>
-      <c r="G27" s="5">
+      <c r="I27" s="5">
         <v>1405000</v>
       </c>
-      <c r="H27" s="13">
+      <c r="J27" s="13">
         <v>1419000</v>
       </c>
-      <c r="I27" s="13">
+      <c r="K27" s="13">
         <v>1405000</v>
       </c>
-      <c r="J27" s="13">
+      <c r="L27" s="13">
         <v>1287000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="7">
+        <v>174279000</v>
+      </c>
+      <c r="C28" s="7">
+        <v>183979000</v>
+      </c>
+      <c r="D28" s="17">
         <v>179922000</v>
       </c>
-      <c r="C28" s="12">
+      <c r="E28" s="17">
         <v>180849000</v>
       </c>
-      <c r="D28" s="5">
+      <c r="F28" s="5">
         <v>164108000</v>
       </c>
-      <c r="E28" s="5">
+      <c r="G28" s="5">
         <v>176619000</v>
       </c>
-      <c r="F28" s="5">
+      <c r="H28" s="5">
         <v>153061000</v>
       </c>
-      <c r="G28" s="5">
+      <c r="I28" s="5">
         <v>173196000</v>
       </c>
-      <c r="H28" s="13">
+      <c r="J28" s="13">
         <v>165288000</v>
       </c>
-      <c r="I28" s="13">
+      <c r="K28" s="13">
         <v>173196000</v>
       </c>
-      <c r="J28" s="13">
+      <c r="L28" s="13">
         <v>291797000</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="7">
+        <v>1608847000</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1596201000</v>
+      </c>
+      <c r="D29" s="17">
         <v>1583531000</v>
       </c>
-      <c r="C29" s="12">
+      <c r="E29" s="17">
         <v>1549920000</v>
       </c>
-      <c r="D29" s="5">
+      <c r="F29" s="5">
         <v>1531380000</v>
       </c>
-      <c r="E29" s="5">
+      <c r="G29" s="5">
         <v>1513102000</v>
       </c>
-      <c r="F29" s="5">
+      <c r="H29" s="5">
         <v>1494652000</v>
       </c>
-      <c r="G29" s="5">
+      <c r="I29" s="5">
         <v>1423151000</v>
       </c>
-      <c r="H29" s="13">
+      <c r="J29" s="13">
         <v>1450098000</v>
       </c>
-      <c r="I29" s="13">
+      <c r="K29" s="13">
         <v>1423151000</v>
       </c>
-      <c r="J29" s="13">
+      <c r="L29" s="13">
         <v>745630000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="7">
+        <v>548000</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1594000</v>
+      </c>
+      <c r="D30" s="17">
         <v>-242000</v>
       </c>
-      <c r="C30" s="12">
+      <c r="E30" s="17">
         <v>1336000</v>
       </c>
-      <c r="D30" s="5">
+      <c r="F30" s="5">
         <v>1682000</v>
       </c>
-      <c r="E30" s="5">
+      <c r="G30" s="5">
         <v>2271000</v>
       </c>
-      <c r="F30" s="5">
+      <c r="H30" s="5">
         <v>943000</v>
       </c>
-      <c r="G30" s="5">
+      <c r="I30" s="5">
         <v>2096000</v>
       </c>
-      <c r="H30" s="13">
+      <c r="J30" s="13">
         <v>2271000</v>
       </c>
-      <c r="I30" s="13">
+      <c r="K30" s="13">
         <v>2096000</v>
       </c>
-      <c r="J30" s="13">
+      <c r="L30" s="13">
         <v>1769000</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="7">
+        <v>-1109098000</v>
+      </c>
+      <c r="C31" s="7">
+        <v>-1079805000</v>
+      </c>
+      <c r="D31" s="17">
         <v>-1049719000</v>
       </c>
-      <c r="C31" s="12">
+      <c r="E31" s="17">
         <v>-1011715000</v>
       </c>
-      <c r="D31" s="5">
+      <c r="F31" s="5">
         <v>-973740000</v>
       </c>
-      <c r="E31" s="5">
+      <c r="G31" s="5">
         <v>-939296000</v>
       </c>
-      <c r="F31" s="5">
+      <c r="H31" s="5">
         <v>-901455000</v>
       </c>
-      <c r="G31" s="5">
+      <c r="I31" s="5">
         <v>-777029000</v>
       </c>
-      <c r="H31" s="13">
+      <c r="J31" s="13">
         <v>-821690000</v>
       </c>
-      <c r="I31" s="13">
+      <c r="K31" s="13">
         <v>-777029000</v>
       </c>
-      <c r="J31" s="13">
+      <c r="L31" s="13">
         <v>-639905000</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="7">
+        <v>500325000</v>
+      </c>
+      <c r="C32" s="7">
+        <v>518018000</v>
+      </c>
+      <c r="D32" s="17">
         <v>533598000</v>
       </c>
-      <c r="C32" s="12">
+      <c r="E32" s="17">
         <v>539568000</v>
       </c>
-      <c r="D32" s="5">
+      <c r="F32" s="5">
         <v>559349000</v>
       </c>
-      <c r="E32" s="5">
+      <c r="G32" s="5">
         <v>576104000</v>
       </c>
-      <c r="F32" s="5">
+      <c r="H32" s="5">
         <v>594167000</v>
       </c>
-      <c r="G32" s="5">
+      <c r="I32" s="5">
         <v>648245000</v>
       </c>
-      <c r="H32" s="13">
+      <c r="J32" s="13">
         <v>630706000</v>
       </c>
-      <c r="I32" s="13">
+      <c r="K32" s="13">
         <v>648245000</v>
       </c>
-      <c r="J32" s="13">
+      <c r="L32" s="13">
         <v>107511000</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="7">
+        <v>674604000</v>
+      </c>
+      <c r="C33" s="7">
+        <v>701997000</v>
+      </c>
+      <c r="D33" s="17">
         <v>713520000</v>
       </c>
-      <c r="C33" s="12">
+      <c r="E33" s="17">
         <v>720417000</v>
       </c>
-      <c r="D33" s="5">
+      <c r="F33" s="5">
         <v>723457000</v>
       </c>
-      <c r="E33" s="5">
+      <c r="G33" s="5">
         <v>752723000</v>
       </c>
-      <c r="F33" s="5">
+      <c r="H33" s="5">
         <v>747228000</v>
       </c>
-      <c r="G33" s="5">
+      <c r="I33" s="5">
         <v>821441000</v>
       </c>
-      <c r="H33" s="13">
+      <c r="J33" s="13">
         <v>795994000</v>
       </c>
-      <c r="I33" s="13">
+      <c r="K33" s="13">
         <v>821441000</v>
       </c>
-      <c r="J33" s="13">
+      <c r="L33" s="13">
         <v>399308000</v>
       </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3819,121 +4549,131 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9961904-157F-4234-8693-8A3031A539AB}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="9">
+        <v>45412</v>
+      </c>
+      <c r="C1" s="9">
+        <v>45322</v>
+      </c>
+      <c r="D1" s="9">
         <v>45230</v>
       </c>
-      <c r="C1" s="9">
+      <c r="E1" s="9">
         <v>45138</v>
       </c>
-      <c r="D1" s="9">
+      <c r="F1" s="9">
         <v>45046</v>
       </c>
-      <c r="E1" s="9">
+      <c r="G1" s="9">
         <v>44957</v>
       </c>
-      <c r="F1" s="9">
+      <c r="H1" s="9">
         <v>44865</v>
       </c>
-      <c r="G1" s="10">
+      <c r="I1" s="10">
         <v>44773</v>
       </c>
-      <c r="H1" s="10">
+      <c r="J1" s="10">
         <v>44681</v>
       </c>
-      <c r="I1" s="10">
+      <c r="K1" s="10">
         <v>44592</v>
       </c>
-      <c r="J1" s="9">
+      <c r="L1" s="9">
         <v>44500</v>
       </c>
-      <c r="K1" s="10">
+      <c r="M1" s="10">
         <v>44408</v>
       </c>
-      <c r="L1" s="10">
+      <c r="N1" s="10">
         <v>44316</v>
       </c>
-      <c r="M1" s="8">
+      <c r="O1" s="8">
         <v>44227</v>
       </c>
-      <c r="N1" s="8">
+      <c r="P1" s="8">
         <v>44135</v>
       </c>
-      <c r="O1" s="8">
+      <c r="Q1" s="8">
         <v>44043</v>
       </c>
-      <c r="P1" s="8">
+      <c r="R1" s="8">
         <v>43951</v>
       </c>
-      <c r="Q1" s="11">
+      <c r="S1" s="11">
         <v>43861</v>
       </c>
-      <c r="R1" s="8">
+      <c r="T1" s="8">
         <v>43769</v>
       </c>
-      <c r="S1" s="8">
+      <c r="U1" s="8">
         <v>43677</v>
       </c>
-      <c r="T1" s="8">
+      <c r="V1" s="8">
         <v>43951</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="6">
+        <v>60440000</v>
+      </c>
+      <c r="C2" s="6">
+        <v>220696000</v>
+      </c>
+      <c r="D2" s="6">
         <v>55380000</v>
       </c>
-      <c r="C2" s="6">
+      <c r="E2" s="6">
         <v>53761000</v>
       </c>
-      <c r="D2" s="6">
+      <c r="F2" s="6">
         <v>52703000</v>
       </c>
-      <c r="E2" s="6">
+      <c r="G2" s="6">
         <v>52975000</v>
       </c>
-      <c r="F2" s="6">
+      <c r="H2" s="6">
         <v>49704000</v>
       </c>
-      <c r="G2" s="6">
+      <c r="I2" s="6">
         <v>48450000</v>
       </c>
-      <c r="H2" s="6">
+      <c r="J2" s="6">
         <v>40127000</v>
       </c>
-      <c r="I2" s="6">
+      <c r="K2" s="6">
         <v>37146000</v>
       </c>
-      <c r="J2" s="6">
+      <c r="L2" s="6">
         <v>31700000</v>
       </c>
-      <c r="K2" s="6">
+      <c r="M2" s="6">
         <v>30406000</v>
       </c>
-      <c r="L2" s="6">
+      <c r="N2" s="6">
         <v>31957000</v>
-      </c>
-      <c r="M2" s="6">
-        <v>28292000</v>
-      </c>
-      <c r="N2" s="6">
-        <v>28292000</v>
       </c>
       <c r="O2" s="6">
         <v>28292000</v>
@@ -3942,10 +4682,10 @@
         <v>28292000</v>
       </c>
       <c r="Q2" s="6">
-        <v>23934000</v>
+        <v>28292000</v>
       </c>
       <c r="R2" s="6">
-        <v>23934000</v>
+        <v>28292000</v>
       </c>
       <c r="S2" s="6">
         <v>23934000</v>
@@ -3953,49 +4693,55 @@
       <c r="T2" s="6">
         <v>23934000</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="6">
+        <v>23934000</v>
+      </c>
+      <c r="V2" s="6">
+        <v>23934000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="6">
+        <v>28757000</v>
+      </c>
+      <c r="C3" s="6">
+        <v>107746000</v>
+      </c>
+      <c r="D3" s="6">
         <v>29350000</v>
       </c>
-      <c r="C3" s="6">
+      <c r="E3" s="6">
         <v>27469000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="F3" s="6">
         <v>24556000</v>
       </c>
-      <c r="E3" s="6">
+      <c r="G3" s="6">
         <v>23915000</v>
       </c>
-      <c r="F3" s="6">
+      <c r="H3" s="6">
         <v>24728000</v>
       </c>
-      <c r="G3" s="6">
+      <c r="I3" s="6">
         <v>24977000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
         <v>23628000</v>
       </c>
-      <c r="I3" s="6">
+      <c r="K3" s="6">
         <v>23230000</v>
       </c>
-      <c r="J3" s="6">
+      <c r="L3" s="6">
         <v>20811000</v>
       </c>
-      <c r="K3" s="6">
+      <c r="M3" s="6">
         <v>19820000</v>
       </c>
-      <c r="L3" s="6">
+      <c r="N3" s="6">
         <v>19126000</v>
-      </c>
-      <c r="M3" s="6">
-        <v>21845750</v>
-      </c>
-      <c r="N3" s="6">
-        <v>21845750</v>
       </c>
       <c r="O3" s="6">
         <v>21845750</v>
@@ -4004,10 +4750,10 @@
         <v>21845750</v>
       </c>
       <c r="Q3" s="6">
-        <v>25598250</v>
+        <v>21845750</v>
       </c>
       <c r="R3" s="6">
-        <v>25598250</v>
+        <v>21845750</v>
       </c>
       <c r="S3" s="6">
         <v>25598250</v>
@@ -4015,49 +4761,55 @@
       <c r="T3" s="6">
         <v>25598250</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="6">
+        <v>25598250</v>
+      </c>
+      <c r="V3" s="6">
+        <v>25598250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="6">
+        <v>31683000</v>
+      </c>
+      <c r="C4" s="6">
+        <v>112950000</v>
+      </c>
+      <c r="D4" s="6">
         <v>26030000</v>
       </c>
-      <c r="C4" s="6">
+      <c r="E4" s="6">
         <v>26292000</v>
       </c>
-      <c r="D4" s="6">
+      <c r="F4" s="6">
         <v>28147000</v>
       </c>
-      <c r="E4" s="6">
+      <c r="G4" s="6">
         <v>29060000</v>
       </c>
-      <c r="F4" s="6">
+      <c r="H4" s="6">
         <v>24976000</v>
       </c>
-      <c r="G4" s="6">
+      <c r="I4" s="6">
         <v>23473000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="J4" s="6">
         <v>16499000</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>13916000</v>
       </c>
-      <c r="J4" s="6">
+      <c r="L4" s="6">
         <v>10889000</v>
       </c>
-      <c r="K4" s="6">
+      <c r="M4" s="6">
         <v>10586000</v>
       </c>
-      <c r="L4" s="6">
+      <c r="N4" s="6">
         <v>12831000</v>
-      </c>
-      <c r="M4" s="6">
-        <v>6446250</v>
-      </c>
-      <c r="N4" s="6">
-        <v>6446250</v>
       </c>
       <c r="O4" s="6">
         <v>6446250</v>
@@ -4066,10 +4818,10 @@
         <v>6446250</v>
       </c>
       <c r="Q4" s="6">
-        <v>-1664250</v>
+        <v>6446250</v>
       </c>
       <c r="R4" s="6">
-        <v>-1664250</v>
+        <v>6446250</v>
       </c>
       <c r="S4" s="6">
         <v>-1664250</v>
@@ -4077,49 +4829,55 @@
       <c r="T4" s="6">
         <v>-1664250</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="6">
+        <v>-1664250</v>
+      </c>
+      <c r="V4" s="6">
+        <v>-1664250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="6">
+        <v>25589000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>116339000</v>
+      </c>
+      <c r="D5" s="6">
         <v>33002000</v>
       </c>
-      <c r="C5" s="6">
+      <c r="E5" s="6">
         <v>26741000</v>
       </c>
-      <c r="D5" s="6">
+      <c r="F5" s="6">
         <v>28186000</v>
       </c>
-      <c r="E5" s="6">
+      <c r="G5" s="6">
         <v>31831000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="H5" s="6">
         <v>27598000</v>
       </c>
-      <c r="G5" s="6">
+      <c r="I5" s="6">
         <v>26737000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>24750000</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
         <v>27163000</v>
       </c>
-      <c r="J5" s="6">
+      <c r="L5" s="6">
         <v>14959000</v>
       </c>
-      <c r="K5" s="6">
+      <c r="M5" s="6">
         <v>12432000</v>
       </c>
-      <c r="L5" s="6">
+      <c r="N5" s="6">
         <v>12130000</v>
-      </c>
-      <c r="M5" s="6">
-        <v>10956250</v>
-      </c>
-      <c r="N5" s="6">
-        <v>10956250</v>
       </c>
       <c r="O5" s="6">
         <v>10956250</v>
@@ -4128,10 +4886,10 @@
         <v>10956250</v>
       </c>
       <c r="Q5" s="6">
-        <v>9467750</v>
+        <v>10956250</v>
       </c>
       <c r="R5" s="6">
-        <v>9467750</v>
+        <v>10956250</v>
       </c>
       <c r="S5" s="6">
         <v>9467750</v>
@@ -4139,49 +4897,55 @@
       <c r="T5" s="6">
         <v>9467750</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="6">
+        <v>9467750</v>
+      </c>
+      <c r="V5" s="6">
+        <v>9467750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="6">
+        <v>21485000</v>
+      </c>
+      <c r="C6" s="6">
+        <v>86304000</v>
+      </c>
+      <c r="D6" s="6">
         <v>20774000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="E6" s="6">
         <v>22310000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="F6" s="6">
         <v>23125000</v>
       </c>
-      <c r="E6" s="6">
+      <c r="G6" s="6">
         <v>20299000</v>
       </c>
-      <c r="F6" s="6">
+      <c r="H6" s="6">
         <v>19383000</v>
       </c>
-      <c r="G6" s="6">
+      <c r="I6" s="6">
         <v>19483000</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>18855000</v>
       </c>
-      <c r="I6" s="6">
+      <c r="K6" s="6">
         <v>19226000</v>
       </c>
-      <c r="J6" s="6">
+      <c r="L6" s="6">
         <v>12441000</v>
       </c>
-      <c r="K6" s="6">
+      <c r="M6" s="6">
         <v>10597000</v>
       </c>
-      <c r="L6" s="6">
+      <c r="N6" s="6">
         <v>10653000</v>
-      </c>
-      <c r="M6" s="6">
-        <v>9317000</v>
-      </c>
-      <c r="N6" s="6">
-        <v>9317000</v>
       </c>
       <c r="O6" s="6">
         <v>9317000</v>
@@ -4190,10 +4954,10 @@
         <v>9317000</v>
       </c>
       <c r="Q6" s="6">
-        <v>8728250</v>
+        <v>9317000</v>
       </c>
       <c r="R6" s="6">
-        <v>8728250</v>
+        <v>9317000</v>
       </c>
       <c r="S6" s="6">
         <v>8728250</v>
@@ -4201,49 +4965,55 @@
       <c r="T6" s="6">
         <v>8728250</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="6">
+        <v>8728250</v>
+      </c>
+      <c r="V6" s="6">
+        <v>8728250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="6">
+        <v>19180000</v>
+      </c>
+      <c r="C7" s="6">
+        <v>80055000</v>
+      </c>
+      <c r="D7" s="6">
         <v>20112000</v>
       </c>
-      <c r="C7" s="6">
+      <c r="E7" s="6">
         <v>20521000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="F7" s="6">
         <v>21528000</v>
       </c>
-      <c r="E7" s="6">
+      <c r="G7" s="6">
         <v>19619000</v>
       </c>
-      <c r="F7" s="6">
+      <c r="H7" s="6">
         <v>20627000</v>
       </c>
-      <c r="G7" s="6">
+      <c r="I7" s="6">
         <v>19893000</v>
       </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
         <v>20608000</v>
       </c>
-      <c r="I7" s="6">
+      <c r="K7" s="6">
         <v>24733000</v>
       </c>
-      <c r="J7" s="6">
+      <c r="L7" s="6">
         <v>11800000</v>
       </c>
-      <c r="K7" s="6">
+      <c r="M7" s="6">
         <v>11824000</v>
       </c>
-      <c r="L7" s="6">
+      <c r="N7" s="6">
         <v>8315000</v>
-      </c>
-      <c r="M7" s="6">
-        <v>8033500</v>
-      </c>
-      <c r="N7" s="6">
-        <v>8033500</v>
       </c>
       <c r="O7" s="6">
         <v>8033500</v>
@@ -4252,10 +5022,10 @@
         <v>8033500</v>
       </c>
       <c r="Q7" s="6">
-        <v>6754750</v>
+        <v>8033500</v>
       </c>
       <c r="R7" s="6">
-        <v>6754750</v>
+        <v>8033500</v>
       </c>
       <c r="S7" s="6">
         <v>6754750</v>
@@ -4263,49 +5033,55 @@
       <c r="T7" s="6">
         <v>6754750</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="6">
+        <v>6754750</v>
+      </c>
+      <c r="V7" s="6">
+        <v>6754750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="6">
+        <v>66254000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>282698000</v>
+      </c>
+      <c r="D8" s="6">
         <v>73888000</v>
       </c>
-      <c r="C8" s="6">
+      <c r="E8" s="6">
         <v>69572000</v>
       </c>
-      <c r="D8" s="6">
+      <c r="F8" s="6">
         <v>72839000</v>
       </c>
-      <c r="E8" s="6">
+      <c r="G8" s="6">
         <v>71749000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="H8" s="6">
         <v>67608000</v>
       </c>
-      <c r="G8" s="6">
+      <c r="I8" s="6">
         <v>66113000</v>
       </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
         <v>64213000</v>
       </c>
-      <c r="I8" s="6">
+      <c r="K8" s="6">
         <v>71122000</v>
       </c>
-      <c r="J8" s="6">
+      <c r="L8" s="6">
         <v>39200000</v>
       </c>
-      <c r="K8" s="6">
+      <c r="M8" s="6">
         <v>34853000</v>
       </c>
-      <c r="L8" s="6">
+      <c r="N8" s="6">
         <v>31098000</v>
-      </c>
-      <c r="M8" s="6">
-        <v>28306750</v>
-      </c>
-      <c r="N8" s="6">
-        <v>28306750</v>
       </c>
       <c r="O8" s="6">
         <v>28306750</v>
@@ -4314,10 +5090,10 @@
         <v>28306750</v>
       </c>
       <c r="Q8" s="6">
-        <v>24950750</v>
+        <v>28306750</v>
       </c>
       <c r="R8" s="6">
-        <v>24950750</v>
+        <v>28306750</v>
       </c>
       <c r="S8" s="6">
         <v>24950750</v>
@@ -4325,49 +5101,55 @@
       <c r="T8" s="6">
         <v>24950750</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="6">
+        <v>24950750</v>
+      </c>
+      <c r="V8" s="6">
+        <v>24950750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="6">
+        <v>-34571000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-169748000</v>
+      </c>
+      <c r="D9" s="6">
         <v>-47858000</v>
       </c>
-      <c r="C9" s="6">
+      <c r="E9" s="6">
         <v>-43280000</v>
       </c>
-      <c r="D9" s="6">
+      <c r="F9" s="6">
         <v>-44692000</v>
       </c>
-      <c r="E9" s="6">
+      <c r="G9" s="6">
         <v>-42689000</v>
       </c>
-      <c r="F9" s="6">
+      <c r="H9" s="6">
         <v>-42632000</v>
       </c>
-      <c r="G9" s="6">
+      <c r="I9" s="6">
         <v>-42640000</v>
       </c>
-      <c r="H9" s="6">
+      <c r="J9" s="6">
         <v>-47714000</v>
       </c>
-      <c r="I9" s="6">
+      <c r="K9" s="6">
         <v>-57206000</v>
       </c>
-      <c r="J9" s="6">
+      <c r="L9" s="6">
         <v>-28311000</v>
       </c>
-      <c r="K9" s="6">
+      <c r="M9" s="6">
         <v>-24267000</v>
       </c>
-      <c r="L9" s="6">
+      <c r="N9" s="6">
         <v>-18267000</v>
-      </c>
-      <c r="M9" s="6">
-        <v>-21860500</v>
-      </c>
-      <c r="N9" s="6">
-        <v>-21860500</v>
       </c>
       <c r="O9" s="6">
         <v>-21860500</v>
@@ -4376,10 +5158,10 @@
         <v>-21860500</v>
       </c>
       <c r="Q9" s="6">
-        <v>-26615000</v>
+        <v>-21860500</v>
       </c>
       <c r="R9" s="6">
-        <v>-26615000</v>
+        <v>-21860500</v>
       </c>
       <c r="S9" s="6">
         <v>-26615000</v>
@@ -4387,8 +5169,14 @@
       <c r="T9" s="6">
         <v>-26615000</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="6">
+        <v>-26615000</v>
+      </c>
+      <c r="V9" s="6">
+        <v>-26615000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
@@ -4414,22 +5202,22 @@
         <v>0</v>
       </c>
       <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
         <v>-1690000</v>
       </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
       <c r="L10" s="6">
         <v>0</v>
       </c>
       <c r="M10" s="6">
-        <v>168250</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6">
-        <v>168250</v>
+        <v>0</v>
       </c>
       <c r="O10" s="6">
         <v>168250</v>
@@ -4438,10 +5226,10 @@
         <v>168250</v>
       </c>
       <c r="Q10" s="6">
-        <v>-2882250</v>
+        <v>168250</v>
       </c>
       <c r="R10" s="6">
-        <v>-2882250</v>
+        <v>168250</v>
       </c>
       <c r="S10" s="6">
         <v>-2882250</v>
@@ -4449,44 +5237,50 @@
       <c r="T10" s="6">
         <v>-2882250</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="6">
+        <v>-2882250</v>
+      </c>
+      <c r="V10" s="6">
+        <v>-2882250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="6">
+        <v>3107000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>15414000</v>
+      </c>
+      <c r="D11" s="6">
         <v>3445000</v>
       </c>
-      <c r="C11" s="6">
+      <c r="E11" s="6">
         <v>3802000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="F11" s="6">
         <v>4506000</v>
       </c>
-      <c r="E11" s="6">
+      <c r="G11" s="6">
         <v>4819000</v>
       </c>
-      <c r="F11" s="6">
+      <c r="H11" s="6">
         <v>2853000</v>
       </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
       <c r="I11" s="6">
         <v>0</v>
       </c>
       <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
         <v>8000</v>
       </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
       <c r="M11" s="6">
         <v>0</v>
       </c>
@@ -4511,8 +5305,14 @@
       <c r="T11" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -4538,22 +5338,22 @@
         <v>0</v>
       </c>
       <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
         <v>-1022000</v>
       </c>
-      <c r="J12" s="6">
+      <c r="L12" s="6">
         <v>-2612000</v>
       </c>
-      <c r="K12" s="6">
+      <c r="M12" s="6">
         <v>-2611000</v>
       </c>
-      <c r="L12" s="6">
+      <c r="N12" s="6">
         <v>-2527000</v>
-      </c>
-      <c r="M12" s="6">
-        <v>-2361750</v>
-      </c>
-      <c r="N12" s="6">
-        <v>-2361750</v>
       </c>
       <c r="O12" s="6">
         <v>-2361750</v>
@@ -4562,10 +5362,10 @@
         <v>-2361750</v>
       </c>
       <c r="Q12" s="6">
-        <v>-1736500</v>
+        <v>-2361750</v>
       </c>
       <c r="R12" s="6">
-        <v>-1736500</v>
+        <v>-2361750</v>
       </c>
       <c r="S12" s="6">
         <v>-1736500</v>
@@ -4573,49 +5373,55 @@
       <c r="T12" s="6">
         <v>-1736500</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="6">
+        <v>-1736500</v>
+      </c>
+      <c r="V12" s="6">
+        <v>-1736500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="6">
+        <v>1530000</v>
+      </c>
+      <c r="C13" s="6">
+        <v>13709000</v>
+      </c>
+      <c r="D13" s="6">
         <v>6833000</v>
       </c>
-      <c r="C13" s="6">
+      <c r="E13" s="6">
         <v>1226000</v>
       </c>
-      <c r="D13" s="6">
+      <c r="F13" s="6">
         <v>-5945000</v>
       </c>
-      <c r="E13" s="6">
+      <c r="G13" s="6">
         <v>3297000</v>
       </c>
-      <c r="F13" s="6">
+      <c r="H13" s="6">
         <v>-19000</v>
       </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
         <v>3276000</v>
       </c>
-      <c r="I13" s="6">
+      <c r="K13" s="6">
         <v>23924000</v>
       </c>
-      <c r="J13" s="6">
+      <c r="L13" s="6">
         <v>-10172000</v>
       </c>
-      <c r="K13" s="6">
-        <v>0</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
         <v>-8026000</v>
-      </c>
-      <c r="M13" s="6">
-        <v>-7513250</v>
-      </c>
-      <c r="N13" s="6">
-        <v>-7513250</v>
       </c>
       <c r="O13" s="6">
         <v>-7513250</v>
@@ -4624,10 +5430,10 @@
         <v>-7513250</v>
       </c>
       <c r="Q13" s="6">
-        <v>51750</v>
+        <v>-7513250</v>
       </c>
       <c r="R13" s="6">
-        <v>51750</v>
+        <v>-7513250</v>
       </c>
       <c r="S13" s="6">
         <v>51750</v>
@@ -4635,49 +5441,55 @@
       <c r="T13" s="6">
         <v>51750</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="6">
+        <v>51750</v>
+      </c>
+      <c r="V13" s="6">
+        <v>51750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="6">
+        <v>1083000</v>
+      </c>
+      <c r="C14" s="6">
+        <v>931000</v>
+      </c>
+      <c r="D14" s="6">
         <v>-69000</v>
       </c>
-      <c r="C14" s="6">
+      <c r="E14" s="6">
         <v>859000</v>
       </c>
-      <c r="D14" s="6">
+      <c r="F14" s="6">
         <v>104000</v>
       </c>
-      <c r="E14" s="6">
+      <c r="G14" s="6">
         <v>-1216000</v>
       </c>
-      <c r="F14" s="6">
+      <c r="H14" s="6">
         <v>1000</v>
       </c>
-      <c r="G14" s="6">
+      <c r="I14" s="6">
         <v>1153000</v>
       </c>
-      <c r="H14" s="6">
+      <c r="J14" s="6">
         <v>392000</v>
       </c>
-      <c r="I14" s="6">
+      <c r="K14" s="6">
         <v>-1906000</v>
       </c>
-      <c r="J14" s="6">
+      <c r="L14" s="6">
         <v>-60000</v>
       </c>
-      <c r="K14" s="6">
+      <c r="M14" s="6">
         <v>-84000</v>
       </c>
-      <c r="L14" s="6">
+      <c r="N14" s="6">
         <v>-177000</v>
-      </c>
-      <c r="M14" s="6">
-        <v>59750</v>
-      </c>
-      <c r="N14" s="6">
-        <v>59750</v>
       </c>
       <c r="O14" s="6">
         <v>59750</v>
@@ -4686,10 +5498,10 @@
         <v>59750</v>
       </c>
       <c r="Q14" s="6">
-        <v>286000</v>
+        <v>59750</v>
       </c>
       <c r="R14" s="6">
-        <v>286000</v>
+        <v>59750</v>
       </c>
       <c r="S14" s="6">
         <v>286000</v>
@@ -4697,49 +5509,55 @@
       <c r="T14" s="6">
         <v>286000</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="6">
+        <v>286000</v>
+      </c>
+      <c r="V14" s="6">
+        <v>286000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="6">
+        <v>5720000</v>
+      </c>
+      <c r="C15" s="6">
+        <v>30054000</v>
+      </c>
+      <c r="D15" s="6">
         <v>10209000</v>
       </c>
-      <c r="C15" s="6">
+      <c r="E15" s="6">
         <v>5887000</v>
       </c>
-      <c r="D15" s="6">
+      <c r="F15" s="6">
         <v>10555000</v>
       </c>
-      <c r="E15" s="6">
+      <c r="G15" s="6">
         <v>4788000</v>
       </c>
-      <c r="F15" s="6">
+      <c r="H15" s="6">
         <v>2835000</v>
       </c>
-      <c r="G15" s="6">
+      <c r="I15" s="6">
         <v>3265000</v>
       </c>
-      <c r="H15" s="6">
+      <c r="J15" s="6">
         <v>3668000</v>
       </c>
-      <c r="I15" s="6">
+      <c r="K15" s="6">
         <v>12529000</v>
       </c>
-      <c r="J15" s="6">
+      <c r="L15" s="6">
         <v>-12836000</v>
       </c>
-      <c r="K15" s="6">
+      <c r="M15" s="6">
         <v>4074000</v>
       </c>
-      <c r="L15" s="6">
+      <c r="N15" s="6">
         <v>-10730000</v>
-      </c>
-      <c r="M15" s="6">
-        <v>-9647000</v>
-      </c>
-      <c r="N15" s="6">
-        <v>-9647000</v>
       </c>
       <c r="O15" s="6">
         <v>-9647000</v>
@@ -4748,10 +5566,10 @@
         <v>-9647000</v>
       </c>
       <c r="Q15" s="6">
-        <v>-4281000</v>
+        <v>-9647000</v>
       </c>
       <c r="R15" s="6">
-        <v>-4281000</v>
+        <v>-9647000</v>
       </c>
       <c r="S15" s="6">
         <v>-4281000</v>
@@ -4759,49 +5577,55 @@
       <c r="T15" s="6">
         <v>-4281000</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="6">
+        <v>-4281000</v>
+      </c>
+      <c r="V15" s="6">
+        <v>-4281000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="6">
+        <v>-28851000</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-139694000</v>
+      </c>
+      <c r="D16" s="6">
         <v>-37649000</v>
       </c>
-      <c r="C16" s="6">
+      <c r="E16" s="6">
         <v>-37393000</v>
       </c>
-      <c r="D16" s="6">
+      <c r="F16" s="6">
         <v>-34137000</v>
       </c>
-      <c r="E16" s="6">
+      <c r="G16" s="6">
         <v>-37901000</v>
       </c>
-      <c r="F16" s="6">
+      <c r="H16" s="6">
         <v>-39797000</v>
       </c>
-      <c r="G16" s="6">
+      <c r="I16" s="6">
         <v>-39375000</v>
       </c>
-      <c r="H16" s="6">
+      <c r="J16" s="6">
         <v>-44046000</v>
       </c>
-      <c r="I16" s="6">
+      <c r="K16" s="6">
         <v>-44677000</v>
       </c>
-      <c r="J16" s="6">
+      <c r="L16" s="6">
         <v>-41147000</v>
       </c>
-      <c r="K16" s="6">
+      <c r="M16" s="6">
         <v>-20193000</v>
       </c>
-      <c r="L16" s="6">
+      <c r="N16" s="6">
         <v>-28997000</v>
-      </c>
-      <c r="M16" s="6">
-        <v>-31507500</v>
-      </c>
-      <c r="N16" s="6">
-        <v>-31507500</v>
       </c>
       <c r="O16" s="6">
         <v>-31507500</v>
@@ -4810,10 +5634,10 @@
         <v>-31507500</v>
       </c>
       <c r="Q16" s="6">
-        <v>-30896000</v>
+        <v>-31507500</v>
       </c>
       <c r="R16" s="6">
-        <v>-30896000</v>
+        <v>-31507500</v>
       </c>
       <c r="S16" s="6">
         <v>-30896000</v>
@@ -4821,49 +5645,55 @@
       <c r="T16" s="6">
         <v>-30896000</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="6">
+        <v>-30896000</v>
+      </c>
+      <c r="V16" s="6">
+        <v>-30896000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="6">
+        <v>442000</v>
+      </c>
+      <c r="C17" s="6">
+        <v>815000</v>
+      </c>
+      <c r="D17" s="6">
         <v>355000</v>
       </c>
-      <c r="C17" s="6">
+      <c r="E17" s="6">
         <v>582000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="F17" s="6">
         <v>307000</v>
       </c>
-      <c r="E17" s="6">
+      <c r="G17" s="6">
         <v>-60000</v>
       </c>
-      <c r="F17" s="6">
+      <c r="H17" s="6">
         <v>439000</v>
       </c>
-      <c r="G17" s="6">
+      <c r="I17" s="6">
         <v>154000</v>
       </c>
-      <c r="H17" s="6">
+      <c r="J17" s="6">
         <v>314000</v>
       </c>
-      <c r="I17" s="6">
+      <c r="K17" s="6">
         <v>1288000</v>
       </c>
-      <c r="J17" s="6">
+      <c r="L17" s="6">
         <v>394000</v>
       </c>
-      <c r="K17" s="6">
+      <c r="M17" s="6">
         <v>170000</v>
       </c>
-      <c r="L17" s="6">
+      <c r="N17" s="6">
         <v>258000</v>
-      </c>
-      <c r="M17" s="6">
-        <v>268250</v>
-      </c>
-      <c r="N17" s="6">
-        <v>268250</v>
       </c>
       <c r="O17" s="6">
         <v>268250</v>
@@ -4872,10 +5702,10 @@
         <v>268250</v>
       </c>
       <c r="Q17" s="6">
-        <v>32500</v>
+        <v>268250</v>
       </c>
       <c r="R17" s="6">
-        <v>32500</v>
+        <v>268250</v>
       </c>
       <c r="S17" s="6">
         <v>32500</v>
@@ -4883,49 +5713,55 @@
       <c r="T17" s="6">
         <v>32500</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="6">
+        <v>32500</v>
+      </c>
+      <c r="V17" s="6">
+        <v>32500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="6">
+        <v>-29293000</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-140509000</v>
+      </c>
+      <c r="D18" s="6">
         <v>-38004000</v>
       </c>
-      <c r="C18" s="6">
+      <c r="E18" s="6">
         <v>-37975000</v>
       </c>
-      <c r="D18" s="6">
+      <c r="F18" s="6">
         <v>-34444000</v>
       </c>
-      <c r="E18" s="6">
+      <c r="G18" s="6">
         <v>-37841000</v>
       </c>
-      <c r="F18" s="6">
+      <c r="H18" s="6">
         <v>-40236000</v>
       </c>
-      <c r="G18" s="6">
+      <c r="I18" s="6">
         <v>-39529000</v>
       </c>
-      <c r="H18" s="6">
+      <c r="J18" s="6">
         <v>-44360000</v>
       </c>
-      <c r="I18" s="6">
+      <c r="K18" s="6">
         <v>-45965000</v>
       </c>
-      <c r="J18" s="6">
+      <c r="L18" s="6">
         <v>-41541000</v>
       </c>
-      <c r="K18" s="6">
+      <c r="M18" s="6">
         <v>-20363000</v>
       </c>
-      <c r="L18" s="6">
+      <c r="N18" s="6">
         <v>-29255000</v>
-      </c>
-      <c r="M18" s="6">
-        <v>-31775750</v>
-      </c>
-      <c r="N18" s="6">
-        <v>-31775750</v>
       </c>
       <c r="O18" s="6">
         <v>-31775750</v>
@@ -4934,10 +5770,10 @@
         <v>-31775750</v>
       </c>
       <c r="Q18" s="6">
-        <v>-30928500</v>
+        <v>-31775750</v>
       </c>
       <c r="R18" s="6">
-        <v>-30928500</v>
+        <v>-31775750</v>
       </c>
       <c r="S18" s="6">
         <v>-30928500</v>
@@ -4945,11 +5781,18 @@
       <c r="T18" s="6">
         <v>-30928500</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="6">
+        <v>-30928500</v>
+      </c>
+      <c r="V18" s="6">
+        <v>-30928500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DATA] planet.xlsx minor cleanup
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EBF729-1C5F-4D20-8BC2-2F0BAF3FA94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6932D11-E047-4C64-96C4-F225FDD16B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,7 +195,7 @@
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -245,12 +245,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,7 +274,6 @@
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -559,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
-  <dimension ref="A1:AX27"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,682 +605,682 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AS1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>43677</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="6">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="5">
         <v>23934000</v>
       </c>
-      <c r="AI2" s="6">
+      <c r="AI2" s="5">
         <v>25598250</v>
       </c>
-      <c r="AJ2" s="6">
+      <c r="AJ2" s="5">
         <v>-1664250</v>
       </c>
-      <c r="AK2" s="6">
+      <c r="AK2" s="5">
         <v>9467750</v>
       </c>
-      <c r="AL2" s="6">
+      <c r="AL2" s="5">
         <v>8728250</v>
       </c>
-      <c r="AM2" s="6">
+      <c r="AM2" s="5">
         <v>6754750</v>
       </c>
-      <c r="AN2" s="6">
+      <c r="AN2" s="5">
         <v>24950750</v>
       </c>
-      <c r="AO2" s="6">
+      <c r="AO2" s="5">
         <v>-26615000</v>
       </c>
-      <c r="AP2" s="6">
+      <c r="AP2" s="5">
         <v>-2882250</v>
       </c>
-      <c r="AQ2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="6">
+      <c r="AQ2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="5">
         <v>-1736500</v>
       </c>
-      <c r="AS2" s="6">
+      <c r="AS2" s="5">
         <v>51750</v>
       </c>
-      <c r="AT2" s="6">
+      <c r="AT2" s="5">
         <v>286000</v>
       </c>
-      <c r="AU2" s="6">
+      <c r="AU2" s="5">
         <v>-4281000</v>
       </c>
-      <c r="AV2" s="6">
+      <c r="AV2" s="5">
         <v>-30896000</v>
       </c>
-      <c r="AW2" s="6">
+      <c r="AW2" s="5">
         <v>32500</v>
       </c>
-      <c r="AX2" s="6">
+      <c r="AX2" s="5">
         <v>-30928500</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>43769</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="6">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="5">
         <v>23934000</v>
       </c>
-      <c r="AI3" s="6">
+      <c r="AI3" s="5">
         <v>25598250</v>
       </c>
-      <c r="AJ3" s="6">
+      <c r="AJ3" s="5">
         <v>-1664250</v>
       </c>
-      <c r="AK3" s="6">
+      <c r="AK3" s="5">
         <v>9467750</v>
       </c>
-      <c r="AL3" s="6">
+      <c r="AL3" s="5">
         <v>8728250</v>
       </c>
-      <c r="AM3" s="6">
+      <c r="AM3" s="5">
         <v>6754750</v>
       </c>
-      <c r="AN3" s="6">
+      <c r="AN3" s="5">
         <v>24950750</v>
       </c>
-      <c r="AO3" s="6">
+      <c r="AO3" s="5">
         <v>-26615000</v>
       </c>
-      <c r="AP3" s="6">
+      <c r="AP3" s="5">
         <v>-2882250</v>
       </c>
-      <c r="AQ3" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="6">
+      <c r="AQ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="5">
         <v>-1736500</v>
       </c>
-      <c r="AS3" s="6">
+      <c r="AS3" s="5">
         <v>51750</v>
       </c>
-      <c r="AT3" s="6">
+      <c r="AT3" s="5">
         <v>286000</v>
       </c>
-      <c r="AU3" s="6">
+      <c r="AU3" s="5">
         <v>-4281000</v>
       </c>
-      <c r="AV3" s="6">
+      <c r="AV3" s="5">
         <v>-30896000</v>
       </c>
-      <c r="AW3" s="6">
+      <c r="AW3" s="5">
         <v>32500</v>
       </c>
-      <c r="AX3" s="6">
+      <c r="AX3" s="5">
         <v>-30928500</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>43861</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="6">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="5">
         <v>23934000</v>
       </c>
-      <c r="AI4" s="6">
+      <c r="AI4" s="5">
         <v>25598250</v>
       </c>
-      <c r="AJ4" s="6">
+      <c r="AJ4" s="5">
         <v>-1664250</v>
       </c>
-      <c r="AK4" s="6">
+      <c r="AK4" s="5">
         <v>9467750</v>
       </c>
-      <c r="AL4" s="6">
+      <c r="AL4" s="5">
         <v>8728250</v>
       </c>
-      <c r="AM4" s="6">
+      <c r="AM4" s="5">
         <v>6754750</v>
       </c>
-      <c r="AN4" s="6">
+      <c r="AN4" s="5">
         <v>24950750</v>
       </c>
-      <c r="AO4" s="6">
+      <c r="AO4" s="5">
         <v>-26615000</v>
       </c>
-      <c r="AP4" s="6">
+      <c r="AP4" s="5">
         <v>-2882250</v>
       </c>
-      <c r="AQ4" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="6">
+      <c r="AQ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="5">
         <v>-1736500</v>
       </c>
-      <c r="AS4" s="6">
+      <c r="AS4" s="5">
         <v>51750</v>
       </c>
-      <c r="AT4" s="6">
+      <c r="AT4" s="5">
         <v>286000</v>
       </c>
-      <c r="AU4" s="6">
+      <c r="AU4" s="5">
         <v>-4281000</v>
       </c>
-      <c r="AV4" s="6">
+      <c r="AV4" s="5">
         <v>-30896000</v>
       </c>
-      <c r="AW4" s="6">
+      <c r="AW4" s="5">
         <v>32500</v>
       </c>
-      <c r="AX4" s="6">
+      <c r="AX4" s="5">
         <v>-30928500</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>43951</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="6">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="5">
         <v>28292000</v>
       </c>
-      <c r="AI5" s="6">
+      <c r="AI5" s="5">
         <v>21845750</v>
       </c>
-      <c r="AJ5" s="6">
+      <c r="AJ5" s="5">
         <v>6446250</v>
       </c>
-      <c r="AK5" s="6">
+      <c r="AK5" s="5">
         <v>10956250</v>
       </c>
-      <c r="AL5" s="6">
+      <c r="AL5" s="5">
         <v>9317000</v>
       </c>
-      <c r="AM5" s="6">
+      <c r="AM5" s="5">
         <v>8033500</v>
       </c>
-      <c r="AN5" s="6">
+      <c r="AN5" s="5">
         <v>28306750</v>
       </c>
-      <c r="AO5" s="6">
+      <c r="AO5" s="5">
         <v>-21860500</v>
       </c>
-      <c r="AP5" s="6">
+      <c r="AP5" s="5">
         <v>168250</v>
       </c>
-      <c r="AQ5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="6">
+      <c r="AQ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="5">
         <v>-2361750</v>
       </c>
-      <c r="AS5" s="6">
+      <c r="AS5" s="5">
         <v>-7513250</v>
       </c>
-      <c r="AT5" s="6">
+      <c r="AT5" s="5">
         <v>59750</v>
       </c>
-      <c r="AU5" s="6">
+      <c r="AU5" s="5">
         <v>-9647000</v>
       </c>
-      <c r="AV5" s="6">
+      <c r="AV5" s="5">
         <v>-31507500</v>
       </c>
-      <c r="AW5" s="6">
+      <c r="AW5" s="5">
         <v>268250</v>
       </c>
-      <c r="AX5" s="6">
+      <c r="AX5" s="5">
         <v>-31775750</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>44043</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="5">
         <v>28292000</v>
       </c>
-      <c r="AI6" s="6">
+      <c r="AI6" s="5">
         <v>21845750</v>
       </c>
-      <c r="AJ6" s="6">
+      <c r="AJ6" s="5">
         <v>6446250</v>
       </c>
-      <c r="AK6" s="6">
+      <c r="AK6" s="5">
         <v>10956250</v>
       </c>
-      <c r="AL6" s="6">
+      <c r="AL6" s="5">
         <v>9317000</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AM6" s="5">
         <v>8033500</v>
       </c>
-      <c r="AN6" s="6">
+      <c r="AN6" s="5">
         <v>28306750</v>
       </c>
-      <c r="AO6" s="6">
+      <c r="AO6" s="5">
         <v>-21860500</v>
       </c>
-      <c r="AP6" s="6">
+      <c r="AP6" s="5">
         <v>168250</v>
       </c>
-      <c r="AQ6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="6">
+      <c r="AQ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="5">
         <v>-2361750</v>
       </c>
-      <c r="AS6" s="6">
+      <c r="AS6" s="5">
         <v>-7513250</v>
       </c>
-      <c r="AT6" s="6">
+      <c r="AT6" s="5">
         <v>59750</v>
       </c>
-      <c r="AU6" s="6">
+      <c r="AU6" s="5">
         <v>-9647000</v>
       </c>
-      <c r="AV6" s="6">
+      <c r="AV6" s="5">
         <v>-31507500</v>
       </c>
-      <c r="AW6" s="6">
+      <c r="AW6" s="5">
         <v>268250</v>
       </c>
-      <c r="AX6" s="6">
+      <c r="AX6" s="5">
         <v>-31775750</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>44135</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
-      <c r="AG7" s="4"/>
-      <c r="AH7" s="6">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="5">
         <v>28292000</v>
       </c>
-      <c r="AI7" s="6">
+      <c r="AI7" s="5">
         <v>21845750</v>
       </c>
-      <c r="AJ7" s="6">
+      <c r="AJ7" s="5">
         <v>6446250</v>
       </c>
-      <c r="AK7" s="6">
+      <c r="AK7" s="5">
         <v>10956250</v>
       </c>
-      <c r="AL7" s="6">
+      <c r="AL7" s="5">
         <v>9317000</v>
       </c>
-      <c r="AM7" s="6">
+      <c r="AM7" s="5">
         <v>8033500</v>
       </c>
-      <c r="AN7" s="6">
+      <c r="AN7" s="5">
         <v>28306750</v>
       </c>
-      <c r="AO7" s="6">
+      <c r="AO7" s="5">
         <v>-21860500</v>
       </c>
-      <c r="AP7" s="6">
+      <c r="AP7" s="5">
         <v>168250</v>
       </c>
-      <c r="AQ7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="6">
+      <c r="AQ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="5">
         <v>-2361750</v>
       </c>
-      <c r="AS7" s="6">
+      <c r="AS7" s="5">
         <v>-7513250</v>
       </c>
-      <c r="AT7" s="6">
+      <c r="AT7" s="5">
         <v>59750</v>
       </c>
-      <c r="AU7" s="6">
+      <c r="AU7" s="5">
         <v>-9647000</v>
       </c>
-      <c r="AV7" s="6">
+      <c r="AV7" s="5">
         <v>-31507500</v>
       </c>
-      <c r="AW7" s="6">
+      <c r="AW7" s="5">
         <v>268250</v>
       </c>
-      <c r="AX7" s="6">
+      <c r="AX7" s="5">
         <v>-31775750</v>
       </c>
     </row>
@@ -1292,151 +1288,151 @@
       <c r="A8" s="1">
         <v>44227</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>71183000</v>
       </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
         <v>47110000</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>7134000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>125427000</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>159855000</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>11994000</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>88393000</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>5673000</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>4982000</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
         <v>2984000</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>399308000</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="5">
         <v>1446000</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="5">
         <v>30195000</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>57570000</v>
       </c>
-      <c r="R8" s="6">
-        <v>0</v>
-      </c>
-      <c r="S8" s="6">
-        <v>0</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
         <v>108814000</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="5">
         <v>15122000</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="5">
         <v>7971000</v>
       </c>
-      <c r="W8" s="6">
-        <v>0</v>
-      </c>
-      <c r="X8" s="6">
+      <c r="W8" s="5">
+        <v>0</v>
+      </c>
+      <c r="X8" s="5">
         <v>2991000</v>
       </c>
-      <c r="Y8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="6">
+      <c r="Y8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="5">
         <v>1287000</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="AB8" s="5">
         <v>291797000</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AC8" s="5">
         <v>745630000</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="AD8" s="5">
         <v>1769000</v>
       </c>
-      <c r="AE8" s="6">
+      <c r="AE8" s="5">
         <v>-639905000</v>
       </c>
-      <c r="AF8" s="6">
+      <c r="AF8" s="5">
         <v>107511000</v>
       </c>
-      <c r="AG8" s="6">
+      <c r="AG8" s="5">
         <v>399308000</v>
       </c>
-      <c r="AH8" s="6">
+      <c r="AH8" s="5">
         <v>28292000</v>
       </c>
-      <c r="AI8" s="6">
+      <c r="AI8" s="5">
         <v>21845750</v>
       </c>
-      <c r="AJ8" s="6">
+      <c r="AJ8" s="5">
         <v>6446250</v>
       </c>
-      <c r="AK8" s="6">
+      <c r="AK8" s="5">
         <v>10956250</v>
       </c>
-      <c r="AL8" s="6">
+      <c r="AL8" s="5">
         <v>9317000</v>
       </c>
-      <c r="AM8" s="6">
+      <c r="AM8" s="5">
         <v>8033500</v>
       </c>
-      <c r="AN8" s="6">
+      <c r="AN8" s="5">
         <v>28306750</v>
       </c>
-      <c r="AO8" s="6">
+      <c r="AO8" s="5">
         <v>-21860500</v>
       </c>
-      <c r="AP8" s="6">
+      <c r="AP8" s="5">
         <v>168250</v>
       </c>
-      <c r="AQ8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="6">
+      <c r="AQ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="5">
         <v>-2361750</v>
       </c>
-      <c r="AS8" s="6">
+      <c r="AS8" s="5">
         <v>-7513250</v>
       </c>
-      <c r="AT8" s="6">
+      <c r="AT8" s="5">
         <v>59750</v>
       </c>
-      <c r="AU8" s="6">
+      <c r="AU8" s="5">
         <v>-9647000</v>
       </c>
-      <c r="AV8" s="6">
+      <c r="AV8" s="5">
         <v>-31507500</v>
       </c>
-      <c r="AW8" s="6">
+      <c r="AW8" s="5">
         <v>268250</v>
       </c>
-      <c r="AX8" s="6">
+      <c r="AX8" s="5">
         <v>-31775750</v>
       </c>
     </row>
@@ -1444,87 +1440,87 @@
       <c r="A9" s="1">
         <v>44316</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="6"/>
-      <c r="AH9" s="6">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5">
         <v>31957000</v>
       </c>
-      <c r="AI9" s="6">
+      <c r="AI9" s="5">
         <v>19126000</v>
       </c>
-      <c r="AJ9" s="6">
+      <c r="AJ9" s="5">
         <v>12831000</v>
       </c>
-      <c r="AK9" s="6">
+      <c r="AK9" s="5">
         <v>12130000</v>
       </c>
-      <c r="AL9" s="6">
+      <c r="AL9" s="5">
         <v>10653000</v>
       </c>
-      <c r="AM9" s="6">
+      <c r="AM9" s="5">
         <v>8315000</v>
       </c>
-      <c r="AN9" s="6">
+      <c r="AN9" s="5">
         <v>31098000</v>
       </c>
-      <c r="AO9" s="6">
+      <c r="AO9" s="5">
         <v>-18267000</v>
       </c>
-      <c r="AP9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="6">
+      <c r="AP9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="5">
         <v>-2527000</v>
       </c>
-      <c r="AS9" s="6">
+      <c r="AS9" s="5">
         <v>-8026000</v>
       </c>
-      <c r="AT9" s="6">
+      <c r="AT9" s="5">
         <v>-177000</v>
       </c>
-      <c r="AU9" s="6">
+      <c r="AU9" s="5">
         <v>-10730000</v>
       </c>
-      <c r="AV9" s="6">
+      <c r="AV9" s="5">
         <v>-28997000</v>
       </c>
-      <c r="AW9" s="6">
+      <c r="AW9" s="5">
         <v>258000</v>
       </c>
-      <c r="AX9" s="6">
+      <c r="AX9" s="5">
         <v>-29255000</v>
       </c>
     </row>
@@ -1532,87 +1528,87 @@
       <c r="A10" s="1">
         <v>44408</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5">
         <v>30406000</v>
       </c>
-      <c r="AI10" s="6">
+      <c r="AI10" s="5">
         <v>19820000</v>
       </c>
-      <c r="AJ10" s="6">
+      <c r="AJ10" s="5">
         <v>10586000</v>
       </c>
-      <c r="AK10" s="6">
+      <c r="AK10" s="5">
         <v>12432000</v>
       </c>
-      <c r="AL10" s="6">
+      <c r="AL10" s="5">
         <v>10597000</v>
       </c>
-      <c r="AM10" s="6">
+      <c r="AM10" s="5">
         <v>11824000</v>
       </c>
-      <c r="AN10" s="6">
+      <c r="AN10" s="5">
         <v>34853000</v>
       </c>
-      <c r="AO10" s="6">
+      <c r="AO10" s="5">
         <v>-24267000</v>
       </c>
-      <c r="AP10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="6">
+      <c r="AP10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="5">
         <v>-2611000</v>
       </c>
-      <c r="AS10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="6">
+      <c r="AS10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="5">
         <v>-84000</v>
       </c>
-      <c r="AU10" s="6">
+      <c r="AU10" s="5">
         <v>4074000</v>
       </c>
-      <c r="AV10" s="6">
+      <c r="AV10" s="5">
         <v>-20193000</v>
       </c>
-      <c r="AW10" s="6">
+      <c r="AW10" s="5">
         <v>170000</v>
       </c>
-      <c r="AX10" s="6">
+      <c r="AX10" s="5">
         <v>-20363000</v>
       </c>
     </row>
@@ -1620,87 +1616,87 @@
       <c r="A11" s="1">
         <v>44500</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5">
         <v>31700000</v>
       </c>
-      <c r="AI11" s="6">
+      <c r="AI11" s="5">
         <v>20811000</v>
       </c>
-      <c r="AJ11" s="6">
+      <c r="AJ11" s="5">
         <v>10889000</v>
       </c>
-      <c r="AK11" s="6">
+      <c r="AK11" s="5">
         <v>14959000</v>
       </c>
-      <c r="AL11" s="6">
+      <c r="AL11" s="5">
         <v>12441000</v>
       </c>
-      <c r="AM11" s="6">
+      <c r="AM11" s="5">
         <v>11800000</v>
       </c>
-      <c r="AN11" s="6">
+      <c r="AN11" s="5">
         <v>39200000</v>
       </c>
-      <c r="AO11" s="6">
+      <c r="AO11" s="5">
         <v>-28311000</v>
       </c>
-      <c r="AP11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="6">
+      <c r="AP11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="5">
         <v>8000</v>
       </c>
-      <c r="AR11" s="6">
+      <c r="AR11" s="5">
         <v>-2612000</v>
       </c>
-      <c r="AS11" s="6">
+      <c r="AS11" s="5">
         <v>-10172000</v>
       </c>
-      <c r="AT11" s="6">
+      <c r="AT11" s="5">
         <v>-60000</v>
       </c>
-      <c r="AU11" s="6">
+      <c r="AU11" s="5">
         <v>-12836000</v>
       </c>
-      <c r="AV11" s="6">
+      <c r="AV11" s="5">
         <v>-41147000</v>
       </c>
-      <c r="AW11" s="6">
+      <c r="AW11" s="5">
         <v>394000</v>
       </c>
-      <c r="AX11" s="6">
+      <c r="AX11" s="5">
         <v>-41541000</v>
       </c>
     </row>
@@ -1708,151 +1704,151 @@
       <c r="A12" s="1">
         <v>44592</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>490762000</v>
       </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
         <v>44373000</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>16385000</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>551520000</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>133280000</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>10768000</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>103219000</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>14197000</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>5743000</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>2714000</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <v>821441000</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="6">
         <v>2850000</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>48823000</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="6">
         <v>64233000</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>16135000</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>132041000</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <v>3579000</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="6">
         <v>12149000</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="6">
         <v>23224000</v>
       </c>
-      <c r="X12" s="7">
+      <c r="X12" s="6">
         <v>798000</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Y12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Z12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="7">
+      <c r="Z12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="6">
         <v>1405000</v>
       </c>
-      <c r="AB12" s="7">
+      <c r="AB12" s="6">
         <v>173196000</v>
       </c>
-      <c r="AC12" s="7">
+      <c r="AC12" s="6">
         <v>1423151000</v>
       </c>
-      <c r="AD12" s="7">
+      <c r="AD12" s="6">
         <v>2096000</v>
       </c>
-      <c r="AE12" s="7">
+      <c r="AE12" s="6">
         <v>-777029000</v>
       </c>
-      <c r="AF12" s="7">
+      <c r="AF12" s="6">
         <v>648245000</v>
       </c>
-      <c r="AG12" s="7">
+      <c r="AG12" s="6">
         <v>821441000</v>
       </c>
-      <c r="AH12" s="6">
+      <c r="AH12" s="5">
         <v>37146000</v>
       </c>
-      <c r="AI12" s="6">
+      <c r="AI12" s="5">
         <v>23230000</v>
       </c>
-      <c r="AJ12" s="6">
+      <c r="AJ12" s="5">
         <v>13916000</v>
       </c>
-      <c r="AK12" s="6">
+      <c r="AK12" s="5">
         <v>27163000</v>
       </c>
-      <c r="AL12" s="6">
+      <c r="AL12" s="5">
         <v>19226000</v>
       </c>
-      <c r="AM12" s="6">
+      <c r="AM12" s="5">
         <v>24733000</v>
       </c>
-      <c r="AN12" s="6">
+      <c r="AN12" s="5">
         <v>71122000</v>
       </c>
-      <c r="AO12" s="6">
+      <c r="AO12" s="5">
         <v>-57206000</v>
       </c>
-      <c r="AP12" s="6">
+      <c r="AP12" s="5">
         <v>-1690000</v>
       </c>
-      <c r="AQ12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="6">
+      <c r="AQ12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="5">
         <v>-1022000</v>
       </c>
-      <c r="AS12" s="6">
+      <c r="AS12" s="5">
         <v>23924000</v>
       </c>
-      <c r="AT12" s="6">
+      <c r="AT12" s="5">
         <v>-1906000</v>
       </c>
-      <c r="AU12" s="6">
+      <c r="AU12" s="5">
         <v>12529000</v>
       </c>
-      <c r="AV12" s="6">
+      <c r="AV12" s="5">
         <v>-44677000</v>
       </c>
-      <c r="AW12" s="6">
+      <c r="AW12" s="5">
         <v>1288000</v>
       </c>
-      <c r="AX12" s="6">
+      <c r="AX12" s="5">
         <v>-45965000</v>
       </c>
     </row>
@@ -1860,151 +1856,151 @@
       <c r="A13" s="1">
         <v>44681</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>484489000</v>
       </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
         <v>24581000</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>18192000</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>527262000</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>125329000</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>11105000</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>103219000</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>13604000</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>5653000</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>7035000</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <v>2787000</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>795994000</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>3168000</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>43184000</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>60672000</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>15239000</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="5">
         <v>7188000</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="5">
         <v>129451000</v>
       </c>
-      <c r="U13" s="6">
-        <v>0</v>
-      </c>
-      <c r="V13" s="6">
+      <c r="U13" s="5">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5">
         <v>12199000</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="5">
         <v>19948000</v>
       </c>
-      <c r="X13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="6">
+      <c r="X13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="5">
         <v>2271000</v>
       </c>
-      <c r="Z13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="6">
+      <c r="Z13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="5">
         <v>1419000</v>
       </c>
-      <c r="AB13" s="6">
+      <c r="AB13" s="5">
         <v>165288000</v>
       </c>
-      <c r="AC13" s="6">
+      <c r="AC13" s="5">
         <v>1450098000</v>
       </c>
-      <c r="AD13" s="6">
+      <c r="AD13" s="5">
         <v>2271000</v>
       </c>
-      <c r="AE13" s="6">
+      <c r="AE13" s="5">
         <v>-821690000</v>
       </c>
-      <c r="AF13" s="6">
+      <c r="AF13" s="5">
         <v>630706000</v>
       </c>
-      <c r="AG13" s="6">
+      <c r="AG13" s="5">
         <v>795994000</v>
       </c>
-      <c r="AH13" s="6">
+      <c r="AH13" s="5">
         <v>40127000</v>
       </c>
-      <c r="AI13" s="6">
+      <c r="AI13" s="5">
         <v>23628000</v>
       </c>
-      <c r="AJ13" s="6">
+      <c r="AJ13" s="5">
         <v>16499000</v>
       </c>
-      <c r="AK13" s="6">
+      <c r="AK13" s="5">
         <v>24750000</v>
       </c>
-      <c r="AL13" s="6">
+      <c r="AL13" s="5">
         <v>18855000</v>
       </c>
-      <c r="AM13" s="6">
+      <c r="AM13" s="5">
         <v>20608000</v>
       </c>
-      <c r="AN13" s="6">
+      <c r="AN13" s="5">
         <v>64213000</v>
       </c>
-      <c r="AO13" s="6">
+      <c r="AO13" s="5">
         <v>-47714000</v>
       </c>
-      <c r="AP13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="6">
+      <c r="AP13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="5">
         <v>3276000</v>
       </c>
-      <c r="AT13" s="6">
+      <c r="AT13" s="5">
         <v>392000</v>
       </c>
-      <c r="AU13" s="6">
+      <c r="AU13" s="5">
         <v>3668000</v>
       </c>
-      <c r="AV13" s="6">
+      <c r="AV13" s="5">
         <v>-44046000</v>
       </c>
-      <c r="AW13" s="6">
+      <c r="AW13" s="5">
         <v>314000</v>
       </c>
-      <c r="AX13" s="6">
+      <c r="AX13" s="5">
         <v>-44360000</v>
       </c>
     </row>
@@ -2012,87 +2008,87 @@
       <c r="A14" s="1">
         <v>44773</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5">
         <v>48450000</v>
       </c>
-      <c r="AI14" s="6">
+      <c r="AI14" s="5">
         <v>24977000</v>
       </c>
-      <c r="AJ14" s="6">
+      <c r="AJ14" s="5">
         <v>23473000</v>
       </c>
-      <c r="AK14" s="6">
+      <c r="AK14" s="5">
         <v>26737000</v>
       </c>
-      <c r="AL14" s="6">
+      <c r="AL14" s="5">
         <v>19483000</v>
       </c>
-      <c r="AM14" s="6">
+      <c r="AM14" s="5">
         <v>19893000</v>
       </c>
-      <c r="AN14" s="6">
+      <c r="AN14" s="5">
         <v>66113000</v>
       </c>
-      <c r="AO14" s="6">
+      <c r="AO14" s="5">
         <v>-42640000</v>
       </c>
-      <c r="AP14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="6">
+      <c r="AP14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="5">
         <v>1153000</v>
       </c>
-      <c r="AU14" s="6">
+      <c r="AU14" s="5">
         <v>3265000</v>
       </c>
-      <c r="AV14" s="6">
+      <c r="AV14" s="5">
         <v>-39375000</v>
       </c>
-      <c r="AW14" s="6">
+      <c r="AW14" s="5">
         <v>154000</v>
       </c>
-      <c r="AX14" s="6">
+      <c r="AX14" s="5">
         <v>-39529000</v>
       </c>
     </row>
@@ -2100,151 +2096,151 @@
       <c r="A15" s="1">
         <v>44865</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>199124000</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>226163000</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>29009000</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>26347000</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>480643000</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>115385000</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>11181000</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>103219000</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <v>12419000</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>5163000</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <v>15806000</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <v>3412000</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <v>747228000</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="6">
         <v>2557000</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="6">
         <v>42629000</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="6">
         <v>47698000</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="6">
         <v>13446000</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="6">
         <v>3538000</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="6">
         <v>109868000</v>
       </c>
-      <c r="U15" s="7">
-        <v>0</v>
-      </c>
-      <c r="V15" s="7">
+      <c r="U15" s="6">
+        <v>0</v>
+      </c>
+      <c r="V15" s="6">
         <v>9853000</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="6">
         <v>17855000</v>
       </c>
-      <c r="X15" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="7">
+      <c r="X15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="6">
         <v>14024000</v>
       </c>
-      <c r="Z15" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="7">
+      <c r="Z15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="6">
         <v>1461000</v>
       </c>
-      <c r="AB15" s="7">
+      <c r="AB15" s="6">
         <v>153061000</v>
       </c>
-      <c r="AC15" s="7">
+      <c r="AC15" s="6">
         <v>1494652000</v>
       </c>
-      <c r="AD15" s="7">
+      <c r="AD15" s="6">
         <v>943000</v>
       </c>
-      <c r="AE15" s="7">
+      <c r="AE15" s="6">
         <v>-901455000</v>
       </c>
-      <c r="AF15" s="7">
+      <c r="AF15" s="6">
         <v>594167000</v>
       </c>
-      <c r="AG15" s="7">
+      <c r="AG15" s="6">
         <v>747228000</v>
       </c>
-      <c r="AH15" s="6">
+      <c r="AH15" s="5">
         <v>49704000</v>
       </c>
-      <c r="AI15" s="6">
+      <c r="AI15" s="5">
         <v>24728000</v>
       </c>
-      <c r="AJ15" s="6">
+      <c r="AJ15" s="5">
         <v>24976000</v>
       </c>
-      <c r="AK15" s="6">
+      <c r="AK15" s="5">
         <v>27598000</v>
       </c>
-      <c r="AL15" s="6">
+      <c r="AL15" s="5">
         <v>19383000</v>
       </c>
-      <c r="AM15" s="6">
+      <c r="AM15" s="5">
         <v>20627000</v>
       </c>
-      <c r="AN15" s="6">
+      <c r="AN15" s="5">
         <v>67608000</v>
       </c>
-      <c r="AO15" s="6">
+      <c r="AO15" s="5">
         <v>-42632000</v>
       </c>
-      <c r="AP15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="6">
+      <c r="AP15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="5">
         <v>2853000</v>
       </c>
-      <c r="AR15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS15" s="6">
+      <c r="AR15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="5">
         <v>-19000</v>
       </c>
-      <c r="AT15" s="6">
+      <c r="AT15" s="5">
         <v>1000</v>
       </c>
-      <c r="AU15" s="6">
+      <c r="AU15" s="5">
         <v>2835000</v>
       </c>
-      <c r="AV15" s="6">
+      <c r="AV15" s="5">
         <v>-39797000</v>
       </c>
-      <c r="AW15" s="6">
+      <c r="AW15" s="5">
         <v>439000</v>
       </c>
-      <c r="AX15" s="6">
+      <c r="AX15" s="5">
         <v>-40236000</v>
       </c>
     </row>
@@ -2252,151 +2248,151 @@
       <c r="A16" s="1">
         <v>44957</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>181892000</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>226868000</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>38952000</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>27943000</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>475655000</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>108091000</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>11417000</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>112748000</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>14831000</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>5657000</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>20403000</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <v>3921000</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <v>752723000</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>6900000</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="6">
         <v>46022000</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="6">
         <v>51900000</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="6">
         <v>12550000</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S16" s="6">
         <v>4885000</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="6">
         <v>122257000</v>
       </c>
-      <c r="U16" s="7">
+      <c r="U16" s="6">
         <v>2882000</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V16" s="6">
         <v>8679000</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W16" s="6">
         <v>16670000</v>
       </c>
-      <c r="X16" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="7">
+      <c r="X16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="6">
         <v>17145000</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="Z16" s="6">
         <v>7499000</v>
       </c>
-      <c r="AA16" s="7">
+      <c r="AA16" s="6">
         <v>1487000</v>
       </c>
-      <c r="AB16" s="7">
+      <c r="AB16" s="6">
         <v>176619000</v>
       </c>
-      <c r="AC16" s="7">
+      <c r="AC16" s="6">
         <v>1513102000</v>
       </c>
-      <c r="AD16" s="7">
+      <c r="AD16" s="6">
         <v>2271000</v>
       </c>
-      <c r="AE16" s="7">
+      <c r="AE16" s="6">
         <v>-939296000</v>
       </c>
-      <c r="AF16" s="7">
+      <c r="AF16" s="6">
         <v>576104000</v>
       </c>
-      <c r="AG16" s="7">
+      <c r="AG16" s="6">
         <v>752723000</v>
       </c>
-      <c r="AH16" s="6">
+      <c r="AH16" s="5">
         <v>52975000</v>
       </c>
-      <c r="AI16" s="6">
+      <c r="AI16" s="5">
         <v>23915000</v>
       </c>
-      <c r="AJ16" s="6">
+      <c r="AJ16" s="5">
         <v>29060000</v>
       </c>
-      <c r="AK16" s="6">
+      <c r="AK16" s="5">
         <v>31831000</v>
       </c>
-      <c r="AL16" s="6">
+      <c r="AL16" s="5">
         <v>20299000</v>
       </c>
-      <c r="AM16" s="6">
+      <c r="AM16" s="5">
         <v>19619000</v>
       </c>
-      <c r="AN16" s="6">
+      <c r="AN16" s="5">
         <v>71749000</v>
       </c>
-      <c r="AO16" s="6">
+      <c r="AO16" s="5">
         <v>-42689000</v>
       </c>
-      <c r="AP16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="6">
+      <c r="AP16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="5">
         <v>4819000</v>
       </c>
-      <c r="AR16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS16" s="6">
+      <c r="AR16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="5">
         <v>3297000</v>
       </c>
-      <c r="AT16" s="6">
+      <c r="AT16" s="5">
         <v>-1216000</v>
       </c>
-      <c r="AU16" s="6">
+      <c r="AU16" s="5">
         <v>4788000</v>
       </c>
-      <c r="AV16" s="6">
+      <c r="AV16" s="5">
         <v>-37901000</v>
       </c>
-      <c r="AW16" s="6">
+      <c r="AW16" s="5">
         <v>-60000</v>
       </c>
-      <c r="AX16" s="6">
+      <c r="AX16" s="5">
         <v>-37841000</v>
       </c>
     </row>
@@ -2404,151 +2400,151 @@
       <c r="A17" s="1">
         <v>45046</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>140763000</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>235415000</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>39072000</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>19275000</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>434525000</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>118193000</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>11878000</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>112748000</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <v>13999000</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>5660000</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>23697000</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <v>2757000</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="6">
         <v>723457000</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="6">
         <v>14657000</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="6">
         <v>34432000</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="6">
         <v>44620000</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="6">
         <v>11653000</v>
       </c>
-      <c r="S17" s="7">
+      <c r="S17" s="6">
         <v>6320000</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="6">
         <v>111682000</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17" s="6">
         <v>2474000</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V17" s="6">
         <v>10671000</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="6">
         <v>10725000</v>
       </c>
-      <c r="X17" s="7">
+      <c r="X17" s="6">
         <v>19912000</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Y17" s="6">
         <v>7142000</v>
       </c>
-      <c r="Z17" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="7">
+      <c r="Z17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="6">
         <v>1502000</v>
       </c>
-      <c r="AB17" s="7">
+      <c r="AB17" s="6">
         <v>164108000</v>
       </c>
-      <c r="AC17" s="7">
+      <c r="AC17" s="6">
         <v>1531380000</v>
       </c>
-      <c r="AD17" s="7">
+      <c r="AD17" s="6">
         <v>1682000</v>
       </c>
-      <c r="AE17" s="7">
+      <c r="AE17" s="6">
         <v>-973740000</v>
       </c>
-      <c r="AF17" s="7">
+      <c r="AF17" s="6">
         <v>559349000</v>
       </c>
-      <c r="AG17" s="7">
+      <c r="AG17" s="6">
         <v>723457000</v>
       </c>
-      <c r="AH17" s="6">
+      <c r="AH17" s="5">
         <v>52703000</v>
       </c>
-      <c r="AI17" s="6">
+      <c r="AI17" s="5">
         <v>24556000</v>
       </c>
-      <c r="AJ17" s="6">
+      <c r="AJ17" s="5">
         <v>28147000</v>
       </c>
-      <c r="AK17" s="6">
+      <c r="AK17" s="5">
         <v>28186000</v>
       </c>
-      <c r="AL17" s="6">
+      <c r="AL17" s="5">
         <v>23125000</v>
       </c>
-      <c r="AM17" s="6">
+      <c r="AM17" s="5">
         <v>21528000</v>
       </c>
-      <c r="AN17" s="6">
+      <c r="AN17" s="5">
         <v>72839000</v>
       </c>
-      <c r="AO17" s="6">
+      <c r="AO17" s="5">
         <v>-44692000</v>
       </c>
-      <c r="AP17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="6">
+      <c r="AP17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="5">
         <v>4506000</v>
       </c>
-      <c r="AR17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="6">
+      <c r="AR17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="5">
         <v>-5945000</v>
       </c>
-      <c r="AT17" s="6">
+      <c r="AT17" s="5">
         <v>104000</v>
       </c>
-      <c r="AU17" s="6">
+      <c r="AU17" s="5">
         <v>10555000</v>
       </c>
-      <c r="AV17" s="6">
+      <c r="AV17" s="5">
         <v>-34137000</v>
       </c>
-      <c r="AW17" s="6">
+      <c r="AW17" s="5">
         <v>307000</v>
       </c>
-      <c r="AX17" s="6">
+      <c r="AX17" s="5">
         <v>-34444000</v>
       </c>
     </row>
@@ -2556,151 +2552,151 @@
       <c r="A18" s="1">
         <v>45138</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>118808000</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>248979000</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>40349000</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>19725000</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>427861000</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>120193000</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>12992000</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>112750000</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>14867000</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>5707000</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <v>23485000</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="5">
         <v>2562000</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N18" s="5">
         <v>720417000</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="5">
         <v>3825000</v>
       </c>
-      <c r="P18" s="9">
+      <c r="P18" s="8">
         <v>37841000</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="8">
         <v>56575000</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R18" s="5">
         <v>10757000</v>
       </c>
-      <c r="S18" s="6">
+      <c r="S18" s="5">
         <v>7261000</v>
       </c>
-      <c r="T18" s="6">
+      <c r="T18" s="5">
         <v>116259000</v>
       </c>
-      <c r="U18" s="9">
+      <c r="U18" s="8">
         <v>18186000</v>
       </c>
-      <c r="V18" s="9">
+      <c r="V18" s="8">
         <v>9605000</v>
       </c>
-      <c r="W18" s="6">
+      <c r="W18" s="5">
         <v>9499000</v>
       </c>
-      <c r="X18" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="6">
+      <c r="X18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="5">
         <v>19139000</v>
       </c>
-      <c r="Z18" s="6">
+      <c r="Z18" s="5">
         <v>5926000</v>
       </c>
-      <c r="AA18" s="6">
+      <c r="AA18" s="5">
         <v>2235000</v>
       </c>
-      <c r="AB18" s="6">
+      <c r="AB18" s="5">
         <v>180849000</v>
       </c>
-      <c r="AC18" s="6">
+      <c r="AC18" s="5">
         <v>1549920000</v>
       </c>
-      <c r="AD18" s="6">
+      <c r="AD18" s="5">
         <v>1336000</v>
       </c>
-      <c r="AE18" s="6">
+      <c r="AE18" s="5">
         <v>-1011715000</v>
       </c>
-      <c r="AF18" s="6">
+      <c r="AF18" s="5">
         <v>539568000</v>
       </c>
-      <c r="AG18" s="6">
+      <c r="AG18" s="5">
         <v>720417000</v>
       </c>
-      <c r="AH18" s="6">
+      <c r="AH18" s="5">
         <v>53761000</v>
       </c>
-      <c r="AI18" s="6">
+      <c r="AI18" s="5">
         <v>27469000</v>
       </c>
-      <c r="AJ18" s="6">
+      <c r="AJ18" s="5">
         <v>26292000</v>
       </c>
-      <c r="AK18" s="6">
+      <c r="AK18" s="5">
         <v>26741000</v>
       </c>
-      <c r="AL18" s="6">
+      <c r="AL18" s="5">
         <v>22310000</v>
       </c>
-      <c r="AM18" s="6">
+      <c r="AM18" s="5">
         <v>20521000</v>
       </c>
-      <c r="AN18" s="6">
+      <c r="AN18" s="5">
         <v>69572000</v>
       </c>
-      <c r="AO18" s="6">
+      <c r="AO18" s="5">
         <v>-43280000</v>
       </c>
-      <c r="AP18" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="6">
+      <c r="AP18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="5">
         <v>3802000</v>
       </c>
-      <c r="AR18" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="6">
+      <c r="AR18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="5">
         <v>1226000</v>
       </c>
-      <c r="AT18" s="6">
+      <c r="AT18" s="5">
         <v>859000</v>
       </c>
-      <c r="AU18" s="6">
+      <c r="AU18" s="5">
         <v>5887000</v>
       </c>
-      <c r="AV18" s="6">
+      <c r="AV18" s="5">
         <v>-37393000</v>
       </c>
-      <c r="AW18" s="6">
+      <c r="AW18" s="5">
         <v>582000</v>
       </c>
-      <c r="AX18" s="6">
+      <c r="AX18" s="5">
         <v>-37975000</v>
       </c>
     </row>
@@ -2708,151 +2704,151 @@
       <c r="A19" s="1">
         <v>45230</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>101547000</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>213347000</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>45145000</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>19616000</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>387535000</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>114058000</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>14050000</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>135701000</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>27427000</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>10321000</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="5">
         <v>22091000</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="5">
         <v>2337000</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="5">
         <v>713520000</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <v>4589000</v>
       </c>
-      <c r="P19" s="6">
+      <c r="P19" s="5">
         <v>41961000</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="Q19" s="5">
         <v>67228000</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="5">
         <v>9860000</v>
       </c>
-      <c r="S19" s="6">
+      <c r="S19" s="5">
         <v>7500000</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="5">
         <v>131138000</v>
       </c>
-      <c r="U19" s="6">
+      <c r="U19" s="5">
         <v>7763000</v>
       </c>
-      <c r="V19" s="6">
+      <c r="V19" s="5">
         <v>8353000</v>
       </c>
-      <c r="W19" s="6">
+      <c r="W19" s="5">
         <v>2666000</v>
       </c>
-      <c r="X19" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="6">
+      <c r="X19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="5">
         <v>17321000</v>
       </c>
-      <c r="Z19" s="6">
+      <c r="Z19" s="5">
         <v>5588000</v>
       </c>
-      <c r="AA19" s="6">
+      <c r="AA19" s="5">
         <v>7093000</v>
       </c>
-      <c r="AB19" s="6">
+      <c r="AB19" s="5">
         <v>179922000</v>
       </c>
-      <c r="AC19" s="6">
+      <c r="AC19" s="5">
         <v>1583531000</v>
       </c>
-      <c r="AD19" s="6">
+      <c r="AD19" s="5">
         <v>-242000</v>
       </c>
-      <c r="AE19" s="6">
+      <c r="AE19" s="5">
         <v>-1049719000</v>
       </c>
-      <c r="AF19" s="6">
+      <c r="AF19" s="5">
         <v>533598000</v>
       </c>
-      <c r="AG19" s="6">
+      <c r="AG19" s="5">
         <v>713520000</v>
       </c>
-      <c r="AH19" s="6">
+      <c r="AH19" s="5">
         <v>55380000</v>
       </c>
-      <c r="AI19" s="6">
+      <c r="AI19" s="5">
         <v>29350000</v>
       </c>
-      <c r="AJ19" s="6">
+      <c r="AJ19" s="5">
         <v>26030000</v>
       </c>
-      <c r="AK19" s="6">
+      <c r="AK19" s="5">
         <v>33002000</v>
       </c>
-      <c r="AL19" s="6">
+      <c r="AL19" s="5">
         <v>20774000</v>
       </c>
-      <c r="AM19" s="6">
+      <c r="AM19" s="5">
         <v>20112000</v>
       </c>
-      <c r="AN19" s="6">
+      <c r="AN19" s="5">
         <v>73888000</v>
       </c>
-      <c r="AO19" s="6">
+      <c r="AO19" s="5">
         <v>-47858000</v>
       </c>
-      <c r="AP19" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="6">
+      <c r="AP19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="5">
         <v>3445000</v>
       </c>
-      <c r="AR19" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="6">
+      <c r="AR19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="5">
         <v>6833000</v>
       </c>
-      <c r="AT19" s="6">
+      <c r="AT19" s="5">
         <v>-69000</v>
       </c>
-      <c r="AU19" s="6">
+      <c r="AU19" s="5">
         <v>10209000</v>
       </c>
-      <c r="AV19" s="6">
+      <c r="AV19" s="5">
         <v>-37649000</v>
       </c>
-      <c r="AW19" s="6">
+      <c r="AW19" s="5">
         <v>355000</v>
       </c>
-      <c r="AX19" s="6">
+      <c r="AX19" s="5">
         <v>-38004000</v>
       </c>
     </row>
@@ -2860,151 +2856,151 @@
       <c r="A20" s="1">
         <v>45322</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>83866000</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>215041000</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>43320000</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>19564000</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>370151000</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>113429000</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="9">
         <v>14973000</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>136256000</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>32448000</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>9972000</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>22339000</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>2429000</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="9">
         <v>701997000</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>2601000</v>
       </c>
-      <c r="P20" s="10">
+      <c r="P20" s="9">
         <v>44779000</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="Q20" s="9">
         <v>72327000</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="9">
         <v>8964000</v>
       </c>
-      <c r="S20" s="10">
+      <c r="S20" s="9">
         <v>7978000</v>
       </c>
-      <c r="T20" s="10">
+      <c r="T20" s="9">
         <v>136649000</v>
       </c>
-      <c r="U20" s="10">
+      <c r="U20" s="9">
         <v>5293000</v>
       </c>
-      <c r="V20" s="10">
+      <c r="V20" s="9">
         <v>7101000</v>
       </c>
-      <c r="W20" s="10">
+      <c r="W20" s="9">
         <v>2961000</v>
       </c>
-      <c r="X20" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="10">
+      <c r="X20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="9">
         <v>16952000</v>
       </c>
-      <c r="Z20" s="10">
+      <c r="Z20" s="9">
         <v>5885000</v>
       </c>
-      <c r="AA20" s="10">
+      <c r="AA20" s="9">
         <v>9138000</v>
       </c>
-      <c r="AB20" s="10">
+      <c r="AB20" s="9">
         <v>183979000</v>
       </c>
-      <c r="AC20" s="10">
+      <c r="AC20" s="9">
         <v>1596201000</v>
       </c>
-      <c r="AD20" s="10">
+      <c r="AD20" s="9">
         <v>1594000</v>
       </c>
-      <c r="AE20" s="10">
+      <c r="AE20" s="9">
         <v>-1079805000</v>
       </c>
-      <c r="AF20" s="10">
+      <c r="AF20" s="9">
         <v>518018000</v>
       </c>
-      <c r="AG20" s="10">
+      <c r="AG20" s="9">
         <v>701997000</v>
       </c>
-      <c r="AH20" s="6">
+      <c r="AH20" s="5">
         <v>220696000</v>
       </c>
-      <c r="AI20" s="6">
+      <c r="AI20" s="5">
         <v>107746000</v>
       </c>
-      <c r="AJ20" s="6">
+      <c r="AJ20" s="5">
         <v>112950000</v>
       </c>
-      <c r="AK20" s="6">
+      <c r="AK20" s="5">
         <v>116339000</v>
       </c>
-      <c r="AL20" s="6">
+      <c r="AL20" s="5">
         <v>86304000</v>
       </c>
-      <c r="AM20" s="6">
+      <c r="AM20" s="5">
         <v>80055000</v>
       </c>
-      <c r="AN20" s="6">
+      <c r="AN20" s="5">
         <v>282698000</v>
       </c>
-      <c r="AO20" s="6">
+      <c r="AO20" s="5">
         <v>-169748000</v>
       </c>
-      <c r="AP20" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="6">
+      <c r="AP20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="5">
         <v>15414000</v>
       </c>
-      <c r="AR20" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="6">
+      <c r="AR20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="5">
         <v>13709000</v>
       </c>
-      <c r="AT20" s="6">
+      <c r="AT20" s="5">
         <v>931000</v>
       </c>
-      <c r="AU20" s="6">
+      <c r="AU20" s="5">
         <v>30054000</v>
       </c>
-      <c r="AV20" s="6">
+      <c r="AV20" s="5">
         <v>-139694000</v>
       </c>
-      <c r="AW20" s="6">
+      <c r="AW20" s="5">
         <v>815000</v>
       </c>
-      <c r="AX20" s="6">
+      <c r="AX20" s="5">
         <v>-140509000</v>
       </c>
     </row>
@@ -3012,156 +3008,153 @@
       <c r="A21" s="1">
         <v>45412</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>107367000</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>168218000</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>38527000</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>23044000</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>345958000</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>111338000</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="9">
         <v>16066000</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>137110000</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="9">
         <v>31403000</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <v>9564000</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="9">
         <v>20966000</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>2199000</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="9">
         <v>674604000</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>3131000</v>
       </c>
-      <c r="P21" s="10">
+      <c r="P21" s="9">
         <v>43361000</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="9">
         <v>63646000</v>
       </c>
-      <c r="R21" s="10">
+      <c r="R21" s="9">
         <v>8068000</v>
       </c>
-      <c r="S21" s="10">
+      <c r="S21" s="9">
         <v>8175000</v>
       </c>
-      <c r="T21" s="10">
+      <c r="T21" s="9">
         <v>126381000</v>
       </c>
-      <c r="U21" s="10">
+      <c r="U21" s="9">
         <v>13247000</v>
       </c>
-      <c r="V21" s="10">
+      <c r="V21" s="9">
         <v>9261000</v>
       </c>
-      <c r="W21" s="10">
+      <c r="W21" s="9">
         <v>1431000</v>
       </c>
-      <c r="X21" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="10">
+      <c r="X21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="9">
         <v>15207000</v>
       </c>
-      <c r="Z21" s="10">
+      <c r="Z21" s="9">
         <v>2915000</v>
       </c>
-      <c r="AA21" s="10">
+      <c r="AA21" s="9">
         <v>5837000</v>
       </c>
-      <c r="AB21" s="10">
+      <c r="AB21" s="9">
         <v>174279000</v>
       </c>
-      <c r="AC21" s="10">
+      <c r="AC21" s="9">
         <v>1608847000</v>
       </c>
-      <c r="AD21" s="10">
+      <c r="AD21" s="9">
         <v>548000</v>
       </c>
-      <c r="AE21" s="10">
+      <c r="AE21" s="9">
         <v>-1109098000</v>
       </c>
-      <c r="AF21" s="10">
+      <c r="AF21" s="9">
         <v>500325000</v>
       </c>
-      <c r="AG21" s="10">
+      <c r="AG21" s="9">
         <v>674604000</v>
       </c>
-      <c r="AH21" s="6">
+      <c r="AH21" s="5">
         <v>60440000</v>
       </c>
-      <c r="AI21" s="6">
+      <c r="AI21" s="5">
         <v>28757000</v>
       </c>
-      <c r="AJ21" s="6">
+      <c r="AJ21" s="5">
         <v>31683000</v>
       </c>
-      <c r="AK21" s="6">
+      <c r="AK21" s="5">
         <v>25589000</v>
       </c>
-      <c r="AL21" s="6">
+      <c r="AL21" s="5">
         <v>21485000</v>
       </c>
-      <c r="AM21" s="6">
+      <c r="AM21" s="5">
         <v>19180000</v>
       </c>
-      <c r="AN21" s="6">
+      <c r="AN21" s="5">
         <v>66254000</v>
       </c>
-      <c r="AO21" s="6">
+      <c r="AO21" s="5">
         <v>-34571000</v>
       </c>
-      <c r="AP21" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ21" s="6">
+      <c r="AP21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="5">
         <v>3107000</v>
       </c>
-      <c r="AR21" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS21" s="6">
+      <c r="AR21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="5">
         <v>1530000</v>
       </c>
-      <c r="AT21" s="6">
+      <c r="AT21" s="5">
         <v>1083000</v>
       </c>
-      <c r="AU21" s="6">
+      <c r="AU21" s="5">
         <v>5720000</v>
       </c>
-      <c r="AV21" s="6">
+      <c r="AV21" s="5">
         <v>-28851000</v>
       </c>
-      <c r="AW21" s="6">
+      <c r="AW21" s="5">
         <v>442000</v>
       </c>
-      <c r="AX21" s="6">
+      <c r="AX21" s="5">
         <v>-29293000</v>
       </c>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:AG19">

</xml_diff>

<commit_message>
[DATA] interpolate missing planet.xlsx data
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6932D11-E047-4C64-96C4-F225FDD16B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6208252B-8241-4C13-8C3F-7077B95E5A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated" sheetId="3" r:id="rId1"/>
+    <sheet name="key" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Cash and cash equivalents</t>
   </si>
@@ -149,9 +150,6 @@
     <t>Short-term investments</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>Interest income</t>
   </si>
   <si>
@@ -186,6 +184,9 @@
   </si>
   <si>
     <t>Total Equity</t>
+  </si>
+  <si>
+    <t>interpolated</t>
   </si>
 </sst>
 </file>
@@ -224,12 +225,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -265,14 +272,18 @@
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="42" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,9 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
   <dimension ref="A1:AX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -606,7 +615,7 @@
   <sheetData>
     <row r="1" spans="1:50" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -621,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -645,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>9</v>
@@ -663,7 +672,7 @@
         <v>33</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>11</v>
@@ -681,13 +690,13 @@
         <v>34</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>17</v>
@@ -699,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AG1" s="3" t="s">
         <v>20</v>
@@ -729,22 +738,22 @@
         <v>27</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>29</v>
@@ -1437,41 +1446,130 @@
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="11">
         <v>44316</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
+      <c r="B9" s="10">
+        <f xml:space="preserve"> B$8 +(($A$9-$A$8)/($A$12-$A$8))*(B$12-B$8)</f>
+        <v>173491304.10958904</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <f xml:space="preserve"> D$8 +(($A$9-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
+        <v>46442621.91780822</v>
+      </c>
+      <c r="E9" s="10">
+        <f xml:space="preserve"> E$8 +(($A$9-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
+        <v>9389723.2876712326</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" ref="F9:J9" si="0" xml:space="preserve"> F$8 +(($A$9-$A$8)/($A$12-$A$8))*(F$12-F$8)</f>
+        <v>229323649.31506848</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>153375068.49315068</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="0"/>
+        <v>11695057.534246575</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="0"/>
+        <v>92008106.849315062</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
+        <v>7751454.7945205476</v>
+      </c>
+      <c r="K9" s="10">
+        <f xml:space="preserve"> K$8 +(($A$9-$A$8)/($A$12-$A$8))*(K$12-K$8)</f>
+        <v>5167558.9041095888</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <f xml:space="preserve"> M$8 +(($A$9-$A$8)/($A$12-$A$8))*(M$12-M$8)</f>
+        <v>2918164.3835616438</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" ref="N9:X9" si="1" xml:space="preserve"> N$8 +(($A$9-$A$8)/($A$12-$A$8))*(N$12-N$8)</f>
+        <v>502239060.27397263</v>
+      </c>
+      <c r="O9" s="10">
+        <f t="shared" si="1"/>
+        <v>1788345.2054794519</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="1"/>
+        <v>34737169.8630137</v>
+      </c>
+      <c r="Q9" s="10">
+        <f t="shared" si="1"/>
+        <v>59194676.712328769</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0</v>
+      </c>
+      <c r="S9" s="10">
+        <v>0</v>
+      </c>
+      <c r="T9" s="10">
+        <f t="shared" si="1"/>
+        <v>114477569.8630137</v>
+      </c>
+      <c r="U9" s="10">
+        <f t="shared" si="1"/>
+        <v>12307405.479452055</v>
+      </c>
+      <c r="V9" s="10">
+        <f t="shared" si="1"/>
+        <v>8989745.2054794524</v>
+      </c>
+      <c r="W9" s="10">
+        <v>0</v>
+      </c>
+      <c r="X9" s="10">
+        <f t="shared" si="1"/>
+        <v>2456268.493150685</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="10">
+        <f t="shared" ref="AA9:AG9" si="2" xml:space="preserve"> AA$8 +(($A$9-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
+        <v>1315772.602739726</v>
+      </c>
+      <c r="AB9" s="10">
+        <f t="shared" si="2"/>
+        <v>262877852.05479452</v>
+      </c>
+      <c r="AC9" s="10">
+        <f t="shared" si="2"/>
+        <v>910833750.68493152</v>
+      </c>
+      <c r="AD9" s="10">
+        <f t="shared" si="2"/>
+        <v>1848734.2465753425</v>
+      </c>
+      <c r="AE9" s="10">
+        <f t="shared" si="2"/>
+        <v>-673340715.06849313</v>
+      </c>
+      <c r="AF9" s="10">
+        <f t="shared" si="2"/>
+        <v>239361208.21917808</v>
+      </c>
+      <c r="AG9" s="10">
+        <f t="shared" si="2"/>
+        <v>502239060.27397263</v>
+      </c>
       <c r="AH9" s="5">
         <v>31957000</v>
       </c>
@@ -1525,41 +1623,130 @@
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="11">
         <v>44408</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
+      <c r="B10" s="10">
+        <f xml:space="preserve"> B9 +((A10-A9)/(A12-A9))*(B12-B9)</f>
+        <v>279248202.73972601</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <f xml:space="preserve"> D$8 +(($A$10-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
+        <v>45752747.94520548</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" ref="E10:Q10" si="3" xml:space="preserve"> E$8 +(($A$10-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
+        <v>11721482.191780822</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="3"/>
+        <v>336722432.87671232</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="3"/>
+        <v>146676712.32876712</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="3"/>
+        <v>11386038.356164383</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="3"/>
+        <v>95745071.232876718</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="3"/>
+        <v>9899969.8630136997</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="3"/>
+        <v>5359372.6027397262</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="3"/>
+        <v>2850109.5890410957</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" si="3"/>
+        <v>608639706.84931505</v>
+      </c>
+      <c r="O10" s="10">
+        <f t="shared" si="3"/>
+        <v>2142230.1369863013</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="3"/>
+        <v>39432446.575342461</v>
+      </c>
+      <c r="Q10" s="10">
+        <f t="shared" si="3"/>
+        <v>60874117.80821918</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
+        <f t="shared" ref="T10:X10" si="4" xml:space="preserve"> T$8 +(($A$10-$A$8)/($A$12-$A$8))*(T$12-T$8)</f>
+        <v>120332046.57534246</v>
+      </c>
+      <c r="U10" s="10">
+        <f t="shared" si="4"/>
+        <v>9397936.98630137</v>
+      </c>
+      <c r="V10" s="10">
+        <f t="shared" si="4"/>
+        <v>10042830.136986302</v>
+      </c>
+      <c r="W10" s="10">
+        <v>0</v>
+      </c>
+      <c r="X10" s="10">
+        <f t="shared" si="4"/>
+        <v>1903512.3287671232</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="10">
+        <f t="shared" ref="AA10:AG10" si="5" xml:space="preserve"> AA$8 +(($A$10-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
+        <v>1345515.0684931506</v>
+      </c>
+      <c r="AB10" s="10">
+        <f t="shared" si="5"/>
+        <v>232983901.369863</v>
+      </c>
+      <c r="AC10" s="10">
+        <f t="shared" si="5"/>
+        <v>1081606167.1232877</v>
+      </c>
+      <c r="AD10" s="10">
+        <f t="shared" si="5"/>
+        <v>1931156.1643835616</v>
+      </c>
+      <c r="AE10" s="10">
+        <f t="shared" si="5"/>
+        <v>-707903476.71232879</v>
+      </c>
+      <c r="AF10" s="10">
+        <f t="shared" si="5"/>
+        <v>375655805.47945207</v>
+      </c>
+      <c r="AG10" s="10">
+        <f t="shared" si="5"/>
+        <v>608639706.84931505</v>
+      </c>
       <c r="AH10" s="5">
         <v>30406000</v>
       </c>
@@ -1613,41 +1800,130 @@
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="11">
         <v>44500</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="5"/>
+      <c r="B11" s="10">
+        <f xml:space="preserve"> B10 +((A11-A10)/(A12-A10))*(B12-B10)</f>
+        <v>385005101.36986303</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <f xml:space="preserve"> D$8 +(($A$11-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
+        <v>45062873.97260274</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" ref="E11:Q11" si="6" xml:space="preserve"> E$8 +(($A$11-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
+        <v>14053241.09589041</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="6"/>
+        <v>444121216.43835616</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="6"/>
+        <v>139978356.16438356</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="6"/>
+        <v>11077019.178082192</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="6"/>
+        <v>99482035.616438359</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="6"/>
+        <v>12048484.93150685</v>
+      </c>
+      <c r="K11" s="10">
+        <f t="shared" si="6"/>
+        <v>5551186.3013698626</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <f t="shared" si="6"/>
+        <v>2782054.7945205481</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="6"/>
+        <v>715040353.42465758</v>
+      </c>
+      <c r="O11" s="10">
+        <f t="shared" si="6"/>
+        <v>2496115.0684931506</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="6"/>
+        <v>44127723.287671238</v>
+      </c>
+      <c r="Q11" s="10">
+        <f t="shared" si="6"/>
+        <v>62553558.90410959</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0</v>
+      </c>
+      <c r="T11" s="10">
+        <f t="shared" ref="T11:X11" si="7" xml:space="preserve"> T$8 +(($A$11-$A$8)/($A$12-$A$8))*(T$12-T$8)</f>
+        <v>126186523.28767124</v>
+      </c>
+      <c r="U11" s="10">
+        <f t="shared" si="7"/>
+        <v>6488468.493150685</v>
+      </c>
+      <c r="V11" s="10">
+        <f t="shared" si="7"/>
+        <v>11095915.06849315</v>
+      </c>
+      <c r="W11" s="10">
+        <v>0</v>
+      </c>
+      <c r="X11" s="10">
+        <f t="shared" si="7"/>
+        <v>1350756.1643835616</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="10">
+        <f t="shared" ref="AA11:AG11" si="8" xml:space="preserve"> AA$8 +(($A$11-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
+        <v>1375257.5342465753</v>
+      </c>
+      <c r="AB11" s="10">
+        <f t="shared" si="8"/>
+        <v>203089950.68493152</v>
+      </c>
+      <c r="AC11" s="10">
+        <f t="shared" si="8"/>
+        <v>1252378583.5616438</v>
+      </c>
+      <c r="AD11" s="10">
+        <f t="shared" si="8"/>
+        <v>2013578.0821917809</v>
+      </c>
+      <c r="AE11" s="10">
+        <f t="shared" si="8"/>
+        <v>-742466238.35616446</v>
+      </c>
+      <c r="AF11" s="10">
+        <f t="shared" si="8"/>
+        <v>511950402.73972607</v>
+      </c>
+      <c r="AG11" s="10">
+        <f t="shared" si="8"/>
+        <v>715040353.42465758</v>
+      </c>
       <c r="AH11" s="5">
         <v>31700000</v>
       </c>
@@ -1707,7 +1983,7 @@
       <c r="B12" s="6">
         <v>490762000</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0</v>
       </c>
       <c r="D12" s="6">
@@ -1734,8 +2010,8 @@
       <c r="K12" s="6">
         <v>5743000</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>37</v>
+      <c r="L12" s="5">
+        <v>0</v>
       </c>
       <c r="M12" s="6">
         <v>2714000</v>
@@ -1755,8 +2031,8 @@
       <c r="R12" s="6">
         <v>16135000</v>
       </c>
-      <c r="S12" s="7" t="s">
-        <v>37</v>
+      <c r="S12" s="5">
+        <v>0</v>
       </c>
       <c r="T12" s="6">
         <v>132041000</v>
@@ -1773,8 +2049,8 @@
       <c r="X12" s="6">
         <v>798000</v>
       </c>
-      <c r="Y12" s="7" t="s">
-        <v>37</v>
+      <c r="Y12" s="5">
+        <v>0</v>
       </c>
       <c r="Z12" s="6">
         <v>0</v>
@@ -2005,41 +2281,136 @@
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="11">
         <v>44773</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
+      <c r="B14" s="10">
+        <f xml:space="preserve"> B$13 + (($A$14-$A$13)/($A$15-$A$13))*(B$15-B$13)</f>
+        <v>341806500</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <f xml:space="preserve"> D$13 + (($A$14-$A$13)/($A$15-$A$13))*(D$15-D$13)</f>
+        <v>26795000</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" ref="E14:AG14" si="9" xml:space="preserve"> E$13 + (($A$14-$A$13)/($A$15-$A$13))*(E$15-E$13)</f>
+        <v>22269500</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="9"/>
+        <v>503952500</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="9"/>
+        <v>120357000</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="9"/>
+        <v>11143000</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="9"/>
+        <v>103219000</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="9"/>
+        <v>13011500</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="9"/>
+        <v>5408000</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="9"/>
+        <v>11420500</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="9"/>
+        <v>3099500</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" si="9"/>
+        <v>771611000</v>
+      </c>
+      <c r="O14" s="10">
+        <f t="shared" si="9"/>
+        <v>2862500</v>
+      </c>
+      <c r="P14" s="10">
+        <f t="shared" si="9"/>
+        <v>42906500</v>
+      </c>
+      <c r="Q14" s="10">
+        <f t="shared" si="9"/>
+        <v>54185000</v>
+      </c>
+      <c r="R14" s="10">
+        <f t="shared" si="9"/>
+        <v>14342500</v>
+      </c>
+      <c r="S14" s="10">
+        <f t="shared" si="9"/>
+        <v>5363000</v>
+      </c>
+      <c r="T14" s="10">
+        <f t="shared" si="9"/>
+        <v>119659500</v>
+      </c>
+      <c r="U14" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="10">
+        <f t="shared" si="9"/>
+        <v>11026000</v>
+      </c>
+      <c r="W14" s="10">
+        <f t="shared" si="9"/>
+        <v>18901500</v>
+      </c>
+      <c r="X14" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="10">
+        <f t="shared" si="9"/>
+        <v>8147500</v>
+      </c>
+      <c r="Z14" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="10">
+        <f t="shared" si="9"/>
+        <v>1440000</v>
+      </c>
+      <c r="AB14" s="10">
+        <f t="shared" si="9"/>
+        <v>159174500</v>
+      </c>
+      <c r="AC14" s="10">
+        <f t="shared" si="9"/>
+        <v>1472375000</v>
+      </c>
+      <c r="AD14" s="10">
+        <f t="shared" si="9"/>
+        <v>1607000</v>
+      </c>
+      <c r="AE14" s="10">
+        <f t="shared" si="9"/>
+        <v>-861572500</v>
+      </c>
+      <c r="AF14" s="10">
+        <f t="shared" si="9"/>
+        <v>612436500</v>
+      </c>
+      <c r="AG14" s="10">
+        <f t="shared" si="9"/>
+        <v>771611000</v>
+      </c>
       <c r="AH14" s="5">
         <v>48450000</v>
       </c>
@@ -2594,10 +2965,10 @@
       <c r="O18" s="5">
         <v>3825000</v>
       </c>
-      <c r="P18" s="8">
+      <c r="P18" s="7">
         <v>37841000</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q18" s="7">
         <v>56575000</v>
       </c>
       <c r="R18" s="5">
@@ -2609,10 +2980,10 @@
       <c r="T18" s="5">
         <v>116259000</v>
       </c>
-      <c r="U18" s="8">
+      <c r="U18" s="7">
         <v>18186000</v>
       </c>
-      <c r="V18" s="8">
+      <c r="V18" s="7">
         <v>9605000</v>
       </c>
       <c r="W18" s="5">
@@ -2856,100 +3227,100 @@
       <c r="A20" s="1">
         <v>45322</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>83866000</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>215041000</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>43320000</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>19564000</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>370151000</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>113429000</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>14973000</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>136256000</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>32448000</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>9972000</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>22339000</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="8">
         <v>2429000</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="8">
         <v>701997000</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="8">
         <v>2601000</v>
       </c>
-      <c r="P20" s="9">
+      <c r="P20" s="8">
         <v>44779000</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q20" s="8">
         <v>72327000</v>
       </c>
-      <c r="R20" s="9">
+      <c r="R20" s="8">
         <v>8964000</v>
       </c>
-      <c r="S20" s="9">
+      <c r="S20" s="8">
         <v>7978000</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="8">
         <v>136649000</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="8">
         <v>5293000</v>
       </c>
-      <c r="V20" s="9">
+      <c r="V20" s="8">
         <v>7101000</v>
       </c>
-      <c r="W20" s="9">
+      <c r="W20" s="8">
         <v>2961000</v>
       </c>
-      <c r="X20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="9">
+      <c r="X20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="8">
         <v>16952000</v>
       </c>
-      <c r="Z20" s="9">
+      <c r="Z20" s="8">
         <v>5885000</v>
       </c>
-      <c r="AA20" s="9">
+      <c r="AA20" s="8">
         <v>9138000</v>
       </c>
-      <c r="AB20" s="9">
+      <c r="AB20" s="8">
         <v>183979000</v>
       </c>
-      <c r="AC20" s="9">
+      <c r="AC20" s="8">
         <v>1596201000</v>
       </c>
-      <c r="AD20" s="9">
+      <c r="AD20" s="8">
         <v>1594000</v>
       </c>
-      <c r="AE20" s="9">
+      <c r="AE20" s="8">
         <v>-1079805000</v>
       </c>
-      <c r="AF20" s="9">
+      <c r="AF20" s="8">
         <v>518018000</v>
       </c>
-      <c r="AG20" s="9">
+      <c r="AG20" s="8">
         <v>701997000</v>
       </c>
       <c r="AH20" s="5">
@@ -3008,100 +3379,100 @@
       <c r="A21" s="1">
         <v>45412</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="8">
         <v>107367000</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>168218000</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>38527000</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>23044000</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>345958000</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>111338000</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>16066000</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>137110000</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <v>31403000</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="8">
         <v>9564000</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="8">
         <v>20966000</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="8">
         <v>2199000</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="8">
         <v>674604000</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="8">
         <v>3131000</v>
       </c>
-      <c r="P21" s="9">
+      <c r="P21" s="8">
         <v>43361000</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q21" s="8">
         <v>63646000</v>
       </c>
-      <c r="R21" s="9">
+      <c r="R21" s="8">
         <v>8068000</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S21" s="8">
         <v>8175000</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="8">
         <v>126381000</v>
       </c>
-      <c r="U21" s="9">
+      <c r="U21" s="8">
         <v>13247000</v>
       </c>
-      <c r="V21" s="9">
+      <c r="V21" s="8">
         <v>9261000</v>
       </c>
-      <c r="W21" s="9">
+      <c r="W21" s="8">
         <v>1431000</v>
       </c>
-      <c r="X21" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="9">
+      <c r="X21" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="8">
         <v>15207000</v>
       </c>
-      <c r="Z21" s="9">
+      <c r="Z21" s="8">
         <v>2915000</v>
       </c>
-      <c r="AA21" s="9">
+      <c r="AA21" s="8">
         <v>5837000</v>
       </c>
-      <c r="AB21" s="9">
+      <c r="AB21" s="8">
         <v>174279000</v>
       </c>
-      <c r="AC21" s="9">
+      <c r="AC21" s="8">
         <v>1608847000</v>
       </c>
-      <c r="AD21" s="9">
+      <c r="AD21" s="8">
         <v>548000</v>
       </c>
-      <c r="AE21" s="9">
+      <c r="AE21" s="8">
         <v>-1109098000</v>
       </c>
-      <c r="AF21" s="9">
+      <c r="AF21" s="8">
         <v>500325000</v>
       </c>
-      <c r="AG21" s="9">
+      <c r="AG21" s="8">
         <v>674604000</v>
       </c>
       <c r="AH21" s="5">
@@ -3163,4 +3534,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9840AC-F14A-4C58-BDF4-7D814B7753BE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DATA] interpolate missing planet.xlsx data - copy/paste values and remove in-cell interpolations (issues when reading this in python)
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6208252B-8241-4C13-8C3F-7077B95E5A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEEBFC-EC99-4D0C-AFBD-1E28D9EA84C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -281,9 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="42" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1446,69 +1443,55 @@
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="1">
         <v>44316</v>
       </c>
       <c r="B9" s="10">
-        <f xml:space="preserve"> B$8 +(($A$9-$A$8)/($A$12-$A$8))*(B$12-B$8)</f>
         <v>173491304.10958904</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
       </c>
       <c r="D9" s="10">
-        <f xml:space="preserve"> D$8 +(($A$9-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
         <v>46442621.91780822</v>
       </c>
       <c r="E9" s="10">
-        <f xml:space="preserve"> E$8 +(($A$9-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
         <v>9389723.2876712326</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" ref="F9:J9" si="0" xml:space="preserve"> F$8 +(($A$9-$A$8)/($A$12-$A$8))*(F$12-F$8)</f>
         <v>229323649.31506848</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" si="0"/>
         <v>153375068.49315068</v>
       </c>
       <c r="H9" s="10">
-        <f t="shared" si="0"/>
         <v>11695057.534246575</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="0"/>
         <v>92008106.849315062</v>
       </c>
       <c r="J9" s="10">
-        <f t="shared" si="0"/>
         <v>7751454.7945205476</v>
       </c>
       <c r="K9" s="10">
-        <f xml:space="preserve"> K$8 +(($A$9-$A$8)/($A$12-$A$8))*(K$12-K$8)</f>
         <v>5167558.9041095888</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
       </c>
       <c r="M9" s="10">
-        <f xml:space="preserve"> M$8 +(($A$9-$A$8)/($A$12-$A$8))*(M$12-M$8)</f>
         <v>2918164.3835616438</v>
       </c>
       <c r="N9" s="10">
-        <f t="shared" ref="N9:X9" si="1" xml:space="preserve"> N$8 +(($A$9-$A$8)/($A$12-$A$8))*(N$12-N$8)</f>
         <v>502239060.27397263</v>
       </c>
       <c r="O9" s="10">
-        <f t="shared" si="1"/>
         <v>1788345.2054794519</v>
       </c>
       <c r="P9" s="10">
-        <f t="shared" si="1"/>
         <v>34737169.8630137</v>
       </c>
       <c r="Q9" s="10">
-        <f t="shared" si="1"/>
         <v>59194676.712328769</v>
       </c>
       <c r="R9" s="10">
@@ -1518,22 +1501,18 @@
         <v>0</v>
       </c>
       <c r="T9" s="10">
-        <f t="shared" si="1"/>
         <v>114477569.8630137</v>
       </c>
       <c r="U9" s="10">
-        <f t="shared" si="1"/>
         <v>12307405.479452055</v>
       </c>
       <c r="V9" s="10">
-        <f t="shared" si="1"/>
         <v>8989745.2054794524</v>
       </c>
       <c r="W9" s="10">
         <v>0</v>
       </c>
       <c r="X9" s="10">
-        <f t="shared" si="1"/>
         <v>2456268.493150685</v>
       </c>
       <c r="Y9" s="10">
@@ -1543,31 +1522,24 @@
         <v>0</v>
       </c>
       <c r="AA9" s="10">
-        <f t="shared" ref="AA9:AG9" si="2" xml:space="preserve"> AA$8 +(($A$9-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
         <v>1315772.602739726</v>
       </c>
       <c r="AB9" s="10">
-        <f t="shared" si="2"/>
         <v>262877852.05479452</v>
       </c>
       <c r="AC9" s="10">
-        <f t="shared" si="2"/>
         <v>910833750.68493152</v>
       </c>
       <c r="AD9" s="10">
-        <f t="shared" si="2"/>
         <v>1848734.2465753425</v>
       </c>
       <c r="AE9" s="10">
-        <f t="shared" si="2"/>
         <v>-673340715.06849313</v>
       </c>
       <c r="AF9" s="10">
-        <f t="shared" si="2"/>
         <v>239361208.21917808</v>
       </c>
       <c r="AG9" s="10">
-        <f t="shared" si="2"/>
         <v>502239060.27397263</v>
       </c>
       <c r="AH9" s="5">
@@ -1623,69 +1595,55 @@
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="1">
         <v>44408</v>
       </c>
       <c r="B10" s="10">
-        <f xml:space="preserve"> B9 +((A10-A9)/(A12-A9))*(B12-B9)</f>
         <v>279248202.73972601</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
       </c>
       <c r="D10" s="10">
-        <f xml:space="preserve"> D$8 +(($A$10-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
         <v>45752747.94520548</v>
       </c>
       <c r="E10" s="10">
-        <f t="shared" ref="E10:Q10" si="3" xml:space="preserve"> E$8 +(($A$10-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
         <v>11721482.191780822</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="3"/>
         <v>336722432.87671232</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="3"/>
         <v>146676712.32876712</v>
       </c>
       <c r="H10" s="10">
-        <f t="shared" si="3"/>
         <v>11386038.356164383</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="3"/>
         <v>95745071.232876718</v>
       </c>
       <c r="J10" s="10">
-        <f t="shared" si="3"/>
         <v>9899969.8630136997</v>
       </c>
       <c r="K10" s="10">
-        <f t="shared" si="3"/>
         <v>5359372.6027397262</v>
       </c>
       <c r="L10" s="10">
         <v>0</v>
       </c>
       <c r="M10" s="10">
-        <f t="shared" si="3"/>
         <v>2850109.5890410957</v>
       </c>
       <c r="N10" s="10">
-        <f t="shared" si="3"/>
         <v>608639706.84931505</v>
       </c>
       <c r="O10" s="10">
-        <f t="shared" si="3"/>
         <v>2142230.1369863013</v>
       </c>
       <c r="P10" s="10">
-        <f t="shared" si="3"/>
         <v>39432446.575342461</v>
       </c>
       <c r="Q10" s="10">
-        <f t="shared" si="3"/>
         <v>60874117.80821918</v>
       </c>
       <c r="R10" s="10">
@@ -1695,22 +1653,18 @@
         <v>0</v>
       </c>
       <c r="T10" s="10">
-        <f t="shared" ref="T10:X10" si="4" xml:space="preserve"> T$8 +(($A$10-$A$8)/($A$12-$A$8))*(T$12-T$8)</f>
         <v>120332046.57534246</v>
       </c>
       <c r="U10" s="10">
-        <f t="shared" si="4"/>
         <v>9397936.98630137</v>
       </c>
       <c r="V10" s="10">
-        <f t="shared" si="4"/>
         <v>10042830.136986302</v>
       </c>
       <c r="W10" s="10">
         <v>0</v>
       </c>
       <c r="X10" s="10">
-        <f t="shared" si="4"/>
         <v>1903512.3287671232</v>
       </c>
       <c r="Y10" s="10">
@@ -1720,31 +1674,24 @@
         <v>0</v>
       </c>
       <c r="AA10" s="10">
-        <f t="shared" ref="AA10:AG10" si="5" xml:space="preserve"> AA$8 +(($A$10-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
         <v>1345515.0684931506</v>
       </c>
       <c r="AB10" s="10">
-        <f t="shared" si="5"/>
         <v>232983901.369863</v>
       </c>
       <c r="AC10" s="10">
-        <f t="shared" si="5"/>
         <v>1081606167.1232877</v>
       </c>
       <c r="AD10" s="10">
-        <f t="shared" si="5"/>
         <v>1931156.1643835616</v>
       </c>
       <c r="AE10" s="10">
-        <f t="shared" si="5"/>
         <v>-707903476.71232879</v>
       </c>
       <c r="AF10" s="10">
-        <f t="shared" si="5"/>
         <v>375655805.47945207</v>
       </c>
       <c r="AG10" s="10">
-        <f t="shared" si="5"/>
         <v>608639706.84931505</v>
       </c>
       <c r="AH10" s="5">
@@ -1800,69 +1747,55 @@
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="1">
         <v>44500</v>
       </c>
       <c r="B11" s="10">
-        <f xml:space="preserve"> B10 +((A11-A10)/(A12-A10))*(B12-B10)</f>
         <v>385005101.36986303</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
       </c>
       <c r="D11" s="10">
-        <f xml:space="preserve"> D$8 +(($A$11-$A$8)/($A$12-$A$8))*(D$12-D$8)</f>
         <v>45062873.97260274</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" ref="E11:Q11" si="6" xml:space="preserve"> E$8 +(($A$11-$A$8)/($A$12-$A$8))*(E$12-E$8)</f>
         <v>14053241.09589041</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="6"/>
         <v>444121216.43835616</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="6"/>
         <v>139978356.16438356</v>
       </c>
       <c r="H11" s="10">
-        <f t="shared" si="6"/>
         <v>11077019.178082192</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="6"/>
         <v>99482035.616438359</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" si="6"/>
         <v>12048484.93150685</v>
       </c>
       <c r="K11" s="10">
-        <f t="shared" si="6"/>
         <v>5551186.3013698626</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="M11" s="10">
-        <f t="shared" si="6"/>
         <v>2782054.7945205481</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" si="6"/>
         <v>715040353.42465758</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" si="6"/>
         <v>2496115.0684931506</v>
       </c>
       <c r="P11" s="10">
-        <f t="shared" si="6"/>
         <v>44127723.287671238</v>
       </c>
       <c r="Q11" s="10">
-        <f t="shared" si="6"/>
         <v>62553558.90410959</v>
       </c>
       <c r="R11" s="10">
@@ -1872,22 +1805,18 @@
         <v>0</v>
       </c>
       <c r="T11" s="10">
-        <f t="shared" ref="T11:X11" si="7" xml:space="preserve"> T$8 +(($A$11-$A$8)/($A$12-$A$8))*(T$12-T$8)</f>
         <v>126186523.28767124</v>
       </c>
       <c r="U11" s="10">
-        <f t="shared" si="7"/>
         <v>6488468.493150685</v>
       </c>
       <c r="V11" s="10">
-        <f t="shared" si="7"/>
         <v>11095915.06849315</v>
       </c>
       <c r="W11" s="10">
         <v>0</v>
       </c>
       <c r="X11" s="10">
-        <f t="shared" si="7"/>
         <v>1350756.1643835616</v>
       </c>
       <c r="Y11" s="10">
@@ -1897,31 +1826,24 @@
         <v>0</v>
       </c>
       <c r="AA11" s="10">
-        <f t="shared" ref="AA11:AG11" si="8" xml:space="preserve"> AA$8 +(($A$11-$A$8)/($A$12-$A$8))*(AA$12-AA$8)</f>
         <v>1375257.5342465753</v>
       </c>
       <c r="AB11" s="10">
-        <f t="shared" si="8"/>
         <v>203089950.68493152</v>
       </c>
       <c r="AC11" s="10">
-        <f t="shared" si="8"/>
         <v>1252378583.5616438</v>
       </c>
       <c r="AD11" s="10">
-        <f t="shared" si="8"/>
         <v>2013578.0821917809</v>
       </c>
       <c r="AE11" s="10">
-        <f t="shared" si="8"/>
         <v>-742466238.35616446</v>
       </c>
       <c r="AF11" s="10">
-        <f t="shared" si="8"/>
         <v>511950402.73972607</v>
       </c>
       <c r="AG11" s="10">
-        <f t="shared" si="8"/>
         <v>715040353.42465758</v>
       </c>
       <c r="AH11" s="5">
@@ -2281,134 +2203,103 @@
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="1">
         <v>44773</v>
       </c>
       <c r="B14" s="10">
-        <f xml:space="preserve"> B$13 + (($A$14-$A$13)/($A$15-$A$13))*(B$15-B$13)</f>
         <v>341806500</v>
       </c>
       <c r="C14" s="10">
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <f xml:space="preserve"> D$13 + (($A$14-$A$13)/($A$15-$A$13))*(D$15-D$13)</f>
         <v>26795000</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" ref="E14:AG14" si="9" xml:space="preserve"> E$13 + (($A$14-$A$13)/($A$15-$A$13))*(E$15-E$13)</f>
         <v>22269500</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="9"/>
         <v>503952500</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="9"/>
         <v>120357000</v>
       </c>
       <c r="H14" s="10">
-        <f t="shared" si="9"/>
         <v>11143000</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="9"/>
         <v>103219000</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="9"/>
         <v>13011500</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="9"/>
         <v>5408000</v>
       </c>
       <c r="L14" s="10">
-        <f t="shared" si="9"/>
         <v>11420500</v>
       </c>
       <c r="M14" s="10">
-        <f t="shared" si="9"/>
         <v>3099500</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="9"/>
         <v>771611000</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="9"/>
         <v>2862500</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="9"/>
         <v>42906500</v>
       </c>
       <c r="Q14" s="10">
-        <f t="shared" si="9"/>
         <v>54185000</v>
       </c>
       <c r="R14" s="10">
-        <f t="shared" si="9"/>
         <v>14342500</v>
       </c>
       <c r="S14" s="10">
-        <f t="shared" si="9"/>
         <v>5363000</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="9"/>
         <v>119659500</v>
       </c>
       <c r="U14" s="10">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V14" s="10">
-        <f t="shared" si="9"/>
         <v>11026000</v>
       </c>
       <c r="W14" s="10">
-        <f t="shared" si="9"/>
         <v>18901500</v>
       </c>
       <c r="X14" s="10">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y14" s="10">
-        <f t="shared" si="9"/>
         <v>8147500</v>
       </c>
       <c r="Z14" s="10">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA14" s="10">
-        <f t="shared" si="9"/>
         <v>1440000</v>
       </c>
       <c r="AB14" s="10">
-        <f t="shared" si="9"/>
         <v>159174500</v>
       </c>
       <c r="AC14" s="10">
-        <f t="shared" si="9"/>
         <v>1472375000</v>
       </c>
       <c r="AD14" s="10">
-        <f t="shared" si="9"/>
         <v>1607000</v>
       </c>
       <c r="AE14" s="10">
-        <f t="shared" si="9"/>
         <v>-861572500</v>
       </c>
       <c r="AF14" s="10">
-        <f t="shared" si="9"/>
         <v>612436500</v>
       </c>
       <c r="AG14" s="10">
-        <f t="shared" si="9"/>
         <v>771611000</v>
       </c>
       <c r="AH14" s="5">

</xml_diff>

<commit_message>
[MINOR] minor format updates to make format consistent between sheets
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEEBFC-EC99-4D0C-AFBD-1E28D9EA84C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A3D705-393A-4ADC-B5D5-EAA0CD5C95CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="consolidated" sheetId="3" r:id="rId1"/>
-    <sheet name="key" sheetId="4" r:id="rId2"/>
+    <sheet name="key" sheetId="4" r:id="rId1"/>
+    <sheet name="consolidated" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -252,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -261,9 +261,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -281,6 +278,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="42" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -562,6 +565,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9840AC-F14A-4C58-BDF4-7D814B7753BE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A537E283-6F73-4D72-9227-FEDBB5B10DFD}">
   <dimension ref="A1:AX21"/>
   <sheetViews>
@@ -610,155 +634,155 @@
     <col min="50" max="50" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="11" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AV1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AW1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AX1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -798,55 +822,55 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
-      <c r="AH2" s="5">
+      <c r="AH2" s="4">
         <v>23934000</v>
       </c>
-      <c r="AI2" s="5">
+      <c r="AI2" s="4">
         <v>25598250</v>
       </c>
-      <c r="AJ2" s="5">
+      <c r="AJ2" s="4">
         <v>-1664250</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AK2" s="4">
         <v>9467750</v>
       </c>
-      <c r="AL2" s="5">
+      <c r="AL2" s="4">
         <v>8728250</v>
       </c>
-      <c r="AM2" s="5">
+      <c r="AM2" s="4">
         <v>6754750</v>
       </c>
-      <c r="AN2" s="5">
+      <c r="AN2" s="4">
         <v>24950750</v>
       </c>
-      <c r="AO2" s="5">
+      <c r="AO2" s="4">
         <v>-26615000</v>
       </c>
-      <c r="AP2" s="5">
+      <c r="AP2" s="4">
         <v>-2882250</v>
       </c>
-      <c r="AQ2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="5">
+      <c r="AQ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="4">
         <v>-1736500</v>
       </c>
-      <c r="AS2" s="5">
+      <c r="AS2" s="4">
         <v>51750</v>
       </c>
-      <c r="AT2" s="5">
+      <c r="AT2" s="4">
         <v>286000</v>
       </c>
-      <c r="AU2" s="5">
+      <c r="AU2" s="4">
         <v>-4281000</v>
       </c>
-      <c r="AV2" s="5">
+      <c r="AV2" s="4">
         <v>-30896000</v>
       </c>
-      <c r="AW2" s="5">
+      <c r="AW2" s="4">
         <v>32500</v>
       </c>
-      <c r="AX2" s="5">
+      <c r="AX2" s="4">
         <v>-30928500</v>
       </c>
     </row>
@@ -886,55 +910,55 @@
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
-      <c r="AH3" s="5">
+      <c r="AH3" s="4">
         <v>23934000</v>
       </c>
-      <c r="AI3" s="5">
+      <c r="AI3" s="4">
         <v>25598250</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3" s="4">
         <v>-1664250</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AK3" s="4">
         <v>9467750</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AL3" s="4">
         <v>8728250</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AM3" s="4">
         <v>6754750</v>
       </c>
-      <c r="AN3" s="5">
+      <c r="AN3" s="4">
         <v>24950750</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AO3" s="4">
         <v>-26615000</v>
       </c>
-      <c r="AP3" s="5">
+      <c r="AP3" s="4">
         <v>-2882250</v>
       </c>
-      <c r="AQ3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="5">
+      <c r="AQ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="4">
         <v>-1736500</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AS3" s="4">
         <v>51750</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AT3" s="4">
         <v>286000</v>
       </c>
-      <c r="AU3" s="5">
+      <c r="AU3" s="4">
         <v>-4281000</v>
       </c>
-      <c r="AV3" s="5">
+      <c r="AV3" s="4">
         <v>-30896000</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="AW3" s="4">
         <v>32500</v>
       </c>
-      <c r="AX3" s="5">
+      <c r="AX3" s="4">
         <v>-30928500</v>
       </c>
     </row>
@@ -974,55 +998,55 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
-      <c r="AH4" s="5">
+      <c r="AH4" s="4">
         <v>23934000</v>
       </c>
-      <c r="AI4" s="5">
+      <c r="AI4" s="4">
         <v>25598250</v>
       </c>
-      <c r="AJ4" s="5">
+      <c r="AJ4" s="4">
         <v>-1664250</v>
       </c>
-      <c r="AK4" s="5">
+      <c r="AK4" s="4">
         <v>9467750</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AL4" s="4">
         <v>8728250</v>
       </c>
-      <c r="AM4" s="5">
+      <c r="AM4" s="4">
         <v>6754750</v>
       </c>
-      <c r="AN4" s="5">
+      <c r="AN4" s="4">
         <v>24950750</v>
       </c>
-      <c r="AO4" s="5">
+      <c r="AO4" s="4">
         <v>-26615000</v>
       </c>
-      <c r="AP4" s="5">
+      <c r="AP4" s="4">
         <v>-2882250</v>
       </c>
-      <c r="AQ4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="5">
+      <c r="AQ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="4">
         <v>-1736500</v>
       </c>
-      <c r="AS4" s="5">
+      <c r="AS4" s="4">
         <v>51750</v>
       </c>
-      <c r="AT4" s="5">
+      <c r="AT4" s="4">
         <v>286000</v>
       </c>
-      <c r="AU4" s="5">
+      <c r="AU4" s="4">
         <v>-4281000</v>
       </c>
-      <c r="AV4" s="5">
+      <c r="AV4" s="4">
         <v>-30896000</v>
       </c>
-      <c r="AW4" s="5">
+      <c r="AW4" s="4">
         <v>32500</v>
       </c>
-      <c r="AX4" s="5">
+      <c r="AX4" s="4">
         <v>-30928500</v>
       </c>
     </row>
@@ -1062,55 +1086,55 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
-      <c r="AH5" s="5">
+      <c r="AH5" s="4">
         <v>28292000</v>
       </c>
-      <c r="AI5" s="5">
+      <c r="AI5" s="4">
         <v>21845750</v>
       </c>
-      <c r="AJ5" s="5">
+      <c r="AJ5" s="4">
         <v>6446250</v>
       </c>
-      <c r="AK5" s="5">
+      <c r="AK5" s="4">
         <v>10956250</v>
       </c>
-      <c r="AL5" s="5">
+      <c r="AL5" s="4">
         <v>9317000</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AM5" s="4">
         <v>8033500</v>
       </c>
-      <c r="AN5" s="5">
+      <c r="AN5" s="4">
         <v>28306750</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AO5" s="4">
         <v>-21860500</v>
       </c>
-      <c r="AP5" s="5">
+      <c r="AP5" s="4">
         <v>168250</v>
       </c>
-      <c r="AQ5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="5">
+      <c r="AQ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="4">
         <v>-2361750</v>
       </c>
-      <c r="AS5" s="5">
+      <c r="AS5" s="4">
         <v>-7513250</v>
       </c>
-      <c r="AT5" s="5">
+      <c r="AT5" s="4">
         <v>59750</v>
       </c>
-      <c r="AU5" s="5">
+      <c r="AU5" s="4">
         <v>-9647000</v>
       </c>
-      <c r="AV5" s="5">
+      <c r="AV5" s="4">
         <v>-31507500</v>
       </c>
-      <c r="AW5" s="5">
+      <c r="AW5" s="4">
         <v>268250</v>
       </c>
-      <c r="AX5" s="5">
+      <c r="AX5" s="4">
         <v>-31775750</v>
       </c>
     </row>
@@ -1150,55 +1174,55 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
-      <c r="AH6" s="5">
+      <c r="AH6" s="4">
         <v>28292000</v>
       </c>
-      <c r="AI6" s="5">
+      <c r="AI6" s="4">
         <v>21845750</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="4">
         <v>6446250</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AK6" s="4">
         <v>10956250</v>
       </c>
-      <c r="AL6" s="5">
+      <c r="AL6" s="4">
         <v>9317000</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="4">
         <v>8033500</v>
       </c>
-      <c r="AN6" s="5">
+      <c r="AN6" s="4">
         <v>28306750</v>
       </c>
-      <c r="AO6" s="5">
+      <c r="AO6" s="4">
         <v>-21860500</v>
       </c>
-      <c r="AP6" s="5">
+      <c r="AP6" s="4">
         <v>168250</v>
       </c>
-      <c r="AQ6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="5">
+      <c r="AQ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="4">
         <v>-2361750</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AS6" s="4">
         <v>-7513250</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AT6" s="4">
         <v>59750</v>
       </c>
-      <c r="AU6" s="5">
+      <c r="AU6" s="4">
         <v>-9647000</v>
       </c>
-      <c r="AV6" s="5">
+      <c r="AV6" s="4">
         <v>-31507500</v>
       </c>
-      <c r="AW6" s="5">
+      <c r="AW6" s="4">
         <v>268250</v>
       </c>
-      <c r="AX6" s="5">
+      <c r="AX6" s="4">
         <v>-31775750</v>
       </c>
     </row>
@@ -1238,55 +1262,55 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
-      <c r="AH7" s="5">
+      <c r="AH7" s="4">
         <v>28292000</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AI7" s="4">
         <v>21845750</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="4">
         <v>6446250</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AK7" s="4">
         <v>10956250</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="4">
         <v>9317000</v>
       </c>
-      <c r="AM7" s="5">
+      <c r="AM7" s="4">
         <v>8033500</v>
       </c>
-      <c r="AN7" s="5">
+      <c r="AN7" s="4">
         <v>28306750</v>
       </c>
-      <c r="AO7" s="5">
+      <c r="AO7" s="4">
         <v>-21860500</v>
       </c>
-      <c r="AP7" s="5">
+      <c r="AP7" s="4">
         <v>168250</v>
       </c>
-      <c r="AQ7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="5">
+      <c r="AQ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="4">
         <v>-2361750</v>
       </c>
-      <c r="AS7" s="5">
+      <c r="AS7" s="4">
         <v>-7513250</v>
       </c>
-      <c r="AT7" s="5">
+      <c r="AT7" s="4">
         <v>59750</v>
       </c>
-      <c r="AU7" s="5">
+      <c r="AU7" s="4">
         <v>-9647000</v>
       </c>
-      <c r="AV7" s="5">
+      <c r="AV7" s="4">
         <v>-31507500</v>
       </c>
-      <c r="AW7" s="5">
+      <c r="AW7" s="4">
         <v>268250</v>
       </c>
-      <c r="AX7" s="5">
+      <c r="AX7" s="4">
         <v>-31775750</v>
       </c>
     </row>
@@ -1294,151 +1318,151 @@
       <c r="A8" s="1">
         <v>44227</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>71183000</v>
       </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
         <v>47110000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>7134000</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>125427000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>159855000</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>11994000</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>88393000</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>5673000</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>4982000</v>
       </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
         <v>2984000</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <v>399308000</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <v>1446000</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="4">
         <v>30195000</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <v>57570000</v>
       </c>
-      <c r="R8" s="5">
-        <v>0</v>
-      </c>
-      <c r="S8" s="5">
-        <v>0</v>
-      </c>
-      <c r="T8" s="5">
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
         <v>108814000</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <v>15122000</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8" s="4">
         <v>7971000</v>
       </c>
-      <c r="W8" s="5">
-        <v>0</v>
-      </c>
-      <c r="X8" s="5">
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
         <v>2991000</v>
       </c>
-      <c r="Y8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="5">
+      <c r="Y8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4">
         <v>1287000</v>
       </c>
-      <c r="AB8" s="5">
+      <c r="AB8" s="4">
         <v>291797000</v>
       </c>
-      <c r="AC8" s="5">
+      <c r="AC8" s="4">
         <v>745630000</v>
       </c>
-      <c r="AD8" s="5">
+      <c r="AD8" s="4">
         <v>1769000</v>
       </c>
-      <c r="AE8" s="5">
+      <c r="AE8" s="4">
         <v>-639905000</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AF8" s="4">
         <v>107511000</v>
       </c>
-      <c r="AG8" s="5">
+      <c r="AG8" s="4">
         <v>399308000</v>
       </c>
-      <c r="AH8" s="5">
+      <c r="AH8" s="4">
         <v>28292000</v>
       </c>
-      <c r="AI8" s="5">
+      <c r="AI8" s="4">
         <v>21845750</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AJ8" s="4">
         <v>6446250</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AK8" s="4">
         <v>10956250</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AL8" s="4">
         <v>9317000</v>
       </c>
-      <c r="AM8" s="5">
+      <c r="AM8" s="4">
         <v>8033500</v>
       </c>
-      <c r="AN8" s="5">
+      <c r="AN8" s="4">
         <v>28306750</v>
       </c>
-      <c r="AO8" s="5">
+      <c r="AO8" s="4">
         <v>-21860500</v>
       </c>
-      <c r="AP8" s="5">
+      <c r="AP8" s="4">
         <v>168250</v>
       </c>
-      <c r="AQ8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="5">
+      <c r="AQ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="4">
         <v>-2361750</v>
       </c>
-      <c r="AS8" s="5">
+      <c r="AS8" s="4">
         <v>-7513250</v>
       </c>
-      <c r="AT8" s="5">
+      <c r="AT8" s="4">
         <v>59750</v>
       </c>
-      <c r="AU8" s="5">
+      <c r="AU8" s="4">
         <v>-9647000</v>
       </c>
-      <c r="AV8" s="5">
+      <c r="AV8" s="4">
         <v>-31507500</v>
       </c>
-      <c r="AW8" s="5">
+      <c r="AW8" s="4">
         <v>268250</v>
       </c>
-      <c r="AX8" s="5">
+      <c r="AX8" s="4">
         <v>-31775750</v>
       </c>
     </row>
@@ -1446,151 +1470,151 @@
       <c r="A9" s="1">
         <v>44316</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>173491304.10958904</v>
       </c>
-      <c r="C9" s="10">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
         <v>46442621.91780822</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>9389723.2876712326</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>229323649.31506848</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>153375068.49315068</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>11695057.534246575</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>92008106.849315062</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>7751454.7945205476</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <v>5167558.9041095888</v>
       </c>
-      <c r="L9" s="10">
-        <v>0</v>
-      </c>
-      <c r="M9" s="10">
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
         <v>2918164.3835616438</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="9">
         <v>502239060.27397263</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>1788345.2054794519</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="9">
         <v>34737169.8630137</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="9">
         <v>59194676.712328769</v>
       </c>
-      <c r="R9" s="10">
-        <v>0</v>
-      </c>
-      <c r="S9" s="10">
-        <v>0</v>
-      </c>
-      <c r="T9" s="10">
+      <c r="R9" s="9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="9">
         <v>114477569.8630137</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="9">
         <v>12307405.479452055</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="9">
         <v>8989745.2054794524</v>
       </c>
-      <c r="W9" s="10">
-        <v>0</v>
-      </c>
-      <c r="X9" s="10">
+      <c r="W9" s="9">
+        <v>0</v>
+      </c>
+      <c r="X9" s="9">
         <v>2456268.493150685</v>
       </c>
-      <c r="Y9" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="10">
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="9">
         <v>1315772.602739726</v>
       </c>
-      <c r="AB9" s="10">
+      <c r="AB9" s="9">
         <v>262877852.05479452</v>
       </c>
-      <c r="AC9" s="10">
+      <c r="AC9" s="9">
         <v>910833750.68493152</v>
       </c>
-      <c r="AD9" s="10">
+      <c r="AD9" s="9">
         <v>1848734.2465753425</v>
       </c>
-      <c r="AE9" s="10">
+      <c r="AE9" s="9">
         <v>-673340715.06849313</v>
       </c>
-      <c r="AF9" s="10">
+      <c r="AF9" s="9">
         <v>239361208.21917808</v>
       </c>
-      <c r="AG9" s="10">
+      <c r="AG9" s="9">
         <v>502239060.27397263</v>
       </c>
-      <c r="AH9" s="5">
+      <c r="AH9" s="4">
         <v>31957000</v>
       </c>
-      <c r="AI9" s="5">
+      <c r="AI9" s="4">
         <v>19126000</v>
       </c>
-      <c r="AJ9" s="5">
+      <c r="AJ9" s="4">
         <v>12831000</v>
       </c>
-      <c r="AK9" s="5">
+      <c r="AK9" s="4">
         <v>12130000</v>
       </c>
-      <c r="AL9" s="5">
+      <c r="AL9" s="4">
         <v>10653000</v>
       </c>
-      <c r="AM9" s="5">
+      <c r="AM9" s="4">
         <v>8315000</v>
       </c>
-      <c r="AN9" s="5">
+      <c r="AN9" s="4">
         <v>31098000</v>
       </c>
-      <c r="AO9" s="5">
+      <c r="AO9" s="4">
         <v>-18267000</v>
       </c>
-      <c r="AP9" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="5">
+      <c r="AP9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="4">
         <v>-2527000</v>
       </c>
-      <c r="AS9" s="5">
+      <c r="AS9" s="4">
         <v>-8026000</v>
       </c>
-      <c r="AT9" s="5">
+      <c r="AT9" s="4">
         <v>-177000</v>
       </c>
-      <c r="AU9" s="5">
+      <c r="AU9" s="4">
         <v>-10730000</v>
       </c>
-      <c r="AV9" s="5">
+      <c r="AV9" s="4">
         <v>-28997000</v>
       </c>
-      <c r="AW9" s="5">
+      <c r="AW9" s="4">
         <v>258000</v>
       </c>
-      <c r="AX9" s="5">
+      <c r="AX9" s="4">
         <v>-29255000</v>
       </c>
     </row>
@@ -1598,151 +1622,151 @@
       <c r="A10" s="1">
         <v>44408</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>279248202.73972601</v>
       </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
         <v>45752747.94520548</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>11721482.191780822</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>336722432.87671232</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>146676712.32876712</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>11386038.356164383</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>95745071.232876718</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>9899969.8630136997</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>5359372.6027397262</v>
       </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10">
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
         <v>2850109.5890410957</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="9">
         <v>608639706.84931505</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>2142230.1369863013</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <v>39432446.575342461</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="9">
         <v>60874117.80821918</v>
       </c>
-      <c r="R10" s="10">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10">
-        <v>0</v>
-      </c>
-      <c r="T10" s="10">
+      <c r="R10" s="9">
+        <v>0</v>
+      </c>
+      <c r="S10" s="9">
+        <v>0</v>
+      </c>
+      <c r="T10" s="9">
         <v>120332046.57534246</v>
       </c>
-      <c r="U10" s="10">
+      <c r="U10" s="9">
         <v>9397936.98630137</v>
       </c>
-      <c r="V10" s="10">
+      <c r="V10" s="9">
         <v>10042830.136986302</v>
       </c>
-      <c r="W10" s="10">
-        <v>0</v>
-      </c>
-      <c r="X10" s="10">
+      <c r="W10" s="9">
+        <v>0</v>
+      </c>
+      <c r="X10" s="9">
         <v>1903512.3287671232</v>
       </c>
-      <c r="Y10" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="10">
+      <c r="Y10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="9">
         <v>1345515.0684931506</v>
       </c>
-      <c r="AB10" s="10">
+      <c r="AB10" s="9">
         <v>232983901.369863</v>
       </c>
-      <c r="AC10" s="10">
+      <c r="AC10" s="9">
         <v>1081606167.1232877</v>
       </c>
-      <c r="AD10" s="10">
+      <c r="AD10" s="9">
         <v>1931156.1643835616</v>
       </c>
-      <c r="AE10" s="10">
+      <c r="AE10" s="9">
         <v>-707903476.71232879</v>
       </c>
-      <c r="AF10" s="10">
+      <c r="AF10" s="9">
         <v>375655805.47945207</v>
       </c>
-      <c r="AG10" s="10">
+      <c r="AG10" s="9">
         <v>608639706.84931505</v>
       </c>
-      <c r="AH10" s="5">
+      <c r="AH10" s="4">
         <v>30406000</v>
       </c>
-      <c r="AI10" s="5">
+      <c r="AI10" s="4">
         <v>19820000</v>
       </c>
-      <c r="AJ10" s="5">
+      <c r="AJ10" s="4">
         <v>10586000</v>
       </c>
-      <c r="AK10" s="5">
+      <c r="AK10" s="4">
         <v>12432000</v>
       </c>
-      <c r="AL10" s="5">
+      <c r="AL10" s="4">
         <v>10597000</v>
       </c>
-      <c r="AM10" s="5">
+      <c r="AM10" s="4">
         <v>11824000</v>
       </c>
-      <c r="AN10" s="5">
+      <c r="AN10" s="4">
         <v>34853000</v>
       </c>
-      <c r="AO10" s="5">
+      <c r="AO10" s="4">
         <v>-24267000</v>
       </c>
-      <c r="AP10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="5">
+      <c r="AP10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="4">
         <v>-2611000</v>
       </c>
-      <c r="AS10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="5">
+      <c r="AS10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="4">
         <v>-84000</v>
       </c>
-      <c r="AU10" s="5">
+      <c r="AU10" s="4">
         <v>4074000</v>
       </c>
-      <c r="AV10" s="5">
+      <c r="AV10" s="4">
         <v>-20193000</v>
       </c>
-      <c r="AW10" s="5">
+      <c r="AW10" s="4">
         <v>170000</v>
       </c>
-      <c r="AX10" s="5">
+      <c r="AX10" s="4">
         <v>-20363000</v>
       </c>
     </row>
@@ -1750,151 +1774,151 @@
       <c r="A11" s="1">
         <v>44500</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>385005101.36986303</v>
       </c>
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
         <v>45062873.97260274</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>14053241.09589041</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>444121216.43835616</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>139978356.16438356</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>11077019.178082192</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>99482035.616438359</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>12048484.93150685</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>5551186.3013698626</v>
       </c>
-      <c r="L11" s="10">
-        <v>0</v>
-      </c>
-      <c r="M11" s="10">
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
         <v>2782054.7945205481</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="9">
         <v>715040353.42465758</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>2496115.0684931506</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="9">
         <v>44127723.287671238</v>
       </c>
-      <c r="Q11" s="10">
-        <v>62553558.90410959</v>
-      </c>
-      <c r="R11" s="10">
-        <v>0</v>
-      </c>
-      <c r="S11" s="10">
-        <v>0</v>
-      </c>
-      <c r="T11" s="10">
+      <c r="Q11" s="9">
+        <v>62553558.904109597</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0</v>
+      </c>
+      <c r="S11" s="9">
+        <v>0</v>
+      </c>
+      <c r="T11" s="9">
         <v>126186523.28767124</v>
       </c>
-      <c r="U11" s="10">
+      <c r="U11" s="9">
         <v>6488468.493150685</v>
       </c>
-      <c r="V11" s="10">
+      <c r="V11" s="9">
         <v>11095915.06849315</v>
       </c>
-      <c r="W11" s="10">
-        <v>0</v>
-      </c>
-      <c r="X11" s="10">
+      <c r="W11" s="9">
+        <v>0</v>
+      </c>
+      <c r="X11" s="9">
         <v>1350756.1643835616</v>
       </c>
-      <c r="Y11" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="10">
+      <c r="Y11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="9">
         <v>1375257.5342465753</v>
       </c>
-      <c r="AB11" s="10">
+      <c r="AB11" s="9">
         <v>203089950.68493152</v>
       </c>
-      <c r="AC11" s="10">
+      <c r="AC11" s="9">
         <v>1252378583.5616438</v>
       </c>
-      <c r="AD11" s="10">
+      <c r="AD11" s="9">
         <v>2013578.0821917809</v>
       </c>
-      <c r="AE11" s="10">
+      <c r="AE11" s="9">
         <v>-742466238.35616446</v>
       </c>
-      <c r="AF11" s="10">
+      <c r="AF11" s="9">
         <v>511950402.73972607</v>
       </c>
-      <c r="AG11" s="10">
+      <c r="AG11" s="9">
         <v>715040353.42465758</v>
       </c>
-      <c r="AH11" s="5">
+      <c r="AH11" s="4">
         <v>31700000</v>
       </c>
-      <c r="AI11" s="5">
+      <c r="AI11" s="4">
         <v>20811000</v>
       </c>
-      <c r="AJ11" s="5">
+      <c r="AJ11" s="4">
         <v>10889000</v>
       </c>
-      <c r="AK11" s="5">
+      <c r="AK11" s="4">
         <v>14959000</v>
       </c>
-      <c r="AL11" s="5">
+      <c r="AL11" s="4">
         <v>12441000</v>
       </c>
-      <c r="AM11" s="5">
+      <c r="AM11" s="4">
         <v>11800000</v>
       </c>
-      <c r="AN11" s="5">
+      <c r="AN11" s="4">
         <v>39200000</v>
       </c>
-      <c r="AO11" s="5">
+      <c r="AO11" s="4">
         <v>-28311000</v>
       </c>
-      <c r="AP11" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="5">
+      <c r="AP11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="4">
         <v>8000</v>
       </c>
-      <c r="AR11" s="5">
+      <c r="AR11" s="4">
         <v>-2612000</v>
       </c>
-      <c r="AS11" s="5">
+      <c r="AS11" s="4">
         <v>-10172000</v>
       </c>
-      <c r="AT11" s="5">
+      <c r="AT11" s="4">
         <v>-60000</v>
       </c>
-      <c r="AU11" s="5">
+      <c r="AU11" s="4">
         <v>-12836000</v>
       </c>
-      <c r="AV11" s="5">
+      <c r="AV11" s="4">
         <v>-41147000</v>
       </c>
-      <c r="AW11" s="5">
+      <c r="AW11" s="4">
         <v>394000</v>
       </c>
-      <c r="AX11" s="5">
+      <c r="AX11" s="4">
         <v>-41541000</v>
       </c>
     </row>
@@ -1902,151 +1926,151 @@
       <c r="A12" s="1">
         <v>44592</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>490762000</v>
       </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
         <v>44373000</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>16385000</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>551520000</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>133280000</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>10768000</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>103219000</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>14197000</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>5743000</v>
       </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
         <v>2714000</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <v>821441000</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="5">
         <v>2850000</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="5">
         <v>48823000</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="5">
         <v>64233000</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="5">
         <v>16135000</v>
       </c>
-      <c r="S12" s="5">
-        <v>0</v>
-      </c>
-      <c r="T12" s="6">
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="5">
         <v>132041000</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="5">
         <v>3579000</v>
       </c>
-      <c r="V12" s="6">
+      <c r="V12" s="5">
         <v>12149000</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12" s="5">
         <v>23224000</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12" s="5">
         <v>798000</v>
       </c>
-      <c r="Y12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="6">
+      <c r="Y12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="5">
         <v>1405000</v>
       </c>
-      <c r="AB12" s="6">
+      <c r="AB12" s="5">
         <v>173196000</v>
       </c>
-      <c r="AC12" s="6">
+      <c r="AC12" s="5">
         <v>1423151000</v>
       </c>
-      <c r="AD12" s="6">
+      <c r="AD12" s="5">
         <v>2096000</v>
       </c>
-      <c r="AE12" s="6">
+      <c r="AE12" s="5">
         <v>-777029000</v>
       </c>
-      <c r="AF12" s="6">
+      <c r="AF12" s="5">
         <v>648245000</v>
       </c>
-      <c r="AG12" s="6">
+      <c r="AG12" s="5">
         <v>821441000</v>
       </c>
-      <c r="AH12" s="5">
+      <c r="AH12" s="4">
         <v>37146000</v>
       </c>
-      <c r="AI12" s="5">
+      <c r="AI12" s="4">
         <v>23230000</v>
       </c>
-      <c r="AJ12" s="5">
+      <c r="AJ12" s="4">
         <v>13916000</v>
       </c>
-      <c r="AK12" s="5">
+      <c r="AK12" s="4">
         <v>27163000</v>
       </c>
-      <c r="AL12" s="5">
+      <c r="AL12" s="4">
         <v>19226000</v>
       </c>
-      <c r="AM12" s="5">
+      <c r="AM12" s="4">
         <v>24733000</v>
       </c>
-      <c r="AN12" s="5">
+      <c r="AN12" s="4">
         <v>71122000</v>
       </c>
-      <c r="AO12" s="5">
+      <c r="AO12" s="4">
         <v>-57206000</v>
       </c>
-      <c r="AP12" s="5">
+      <c r="AP12" s="4">
         <v>-1690000</v>
       </c>
-      <c r="AQ12" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="5">
+      <c r="AQ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="4">
         <v>-1022000</v>
       </c>
-      <c r="AS12" s="5">
+      <c r="AS12" s="4">
         <v>23924000</v>
       </c>
-      <c r="AT12" s="5">
+      <c r="AT12" s="4">
         <v>-1906000</v>
       </c>
-      <c r="AU12" s="5">
+      <c r="AU12" s="4">
         <v>12529000</v>
       </c>
-      <c r="AV12" s="5">
+      <c r="AV12" s="4">
         <v>-44677000</v>
       </c>
-      <c r="AW12" s="5">
+      <c r="AW12" s="4">
         <v>1288000</v>
       </c>
-      <c r="AX12" s="5">
+      <c r="AX12" s="4">
         <v>-45965000</v>
       </c>
     </row>
@@ -2054,151 +2078,151 @@
       <c r="A13" s="1">
         <v>44681</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>484489000</v>
       </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
         <v>24581000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>18192000</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>527262000</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>125329000</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>11105000</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>103219000</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>13604000</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <v>5653000</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>7035000</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <v>2787000</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="4">
         <v>795994000</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <v>3168000</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="4">
         <v>43184000</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="4">
         <v>60672000</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="4">
         <v>15239000</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="4">
         <v>7188000</v>
       </c>
-      <c r="T13" s="5">
+      <c r="T13" s="4">
         <v>129451000</v>
       </c>
-      <c r="U13" s="5">
-        <v>0</v>
-      </c>
-      <c r="V13" s="5">
+      <c r="U13" s="4">
+        <v>0</v>
+      </c>
+      <c r="V13" s="4">
         <v>12199000</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="4">
         <v>19948000</v>
       </c>
-      <c r="X13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="5">
+      <c r="X13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="4">
         <v>2271000</v>
       </c>
-      <c r="Z13" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="5">
+      <c r="Z13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="4">
         <v>1419000</v>
       </c>
-      <c r="AB13" s="5">
+      <c r="AB13" s="4">
         <v>165288000</v>
       </c>
-      <c r="AC13" s="5">
+      <c r="AC13" s="4">
         <v>1450098000</v>
       </c>
-      <c r="AD13" s="5">
+      <c r="AD13" s="4">
         <v>2271000</v>
       </c>
-      <c r="AE13" s="5">
+      <c r="AE13" s="4">
         <v>-821690000</v>
       </c>
-      <c r="AF13" s="5">
+      <c r="AF13" s="4">
         <v>630706000</v>
       </c>
-      <c r="AG13" s="5">
+      <c r="AG13" s="4">
         <v>795994000</v>
       </c>
-      <c r="AH13" s="5">
+      <c r="AH13" s="4">
         <v>40127000</v>
       </c>
-      <c r="AI13" s="5">
+      <c r="AI13" s="4">
         <v>23628000</v>
       </c>
-      <c r="AJ13" s="5">
+      <c r="AJ13" s="4">
         <v>16499000</v>
       </c>
-      <c r="AK13" s="5">
+      <c r="AK13" s="4">
         <v>24750000</v>
       </c>
-      <c r="AL13" s="5">
+      <c r="AL13" s="4">
         <v>18855000</v>
       </c>
-      <c r="AM13" s="5">
+      <c r="AM13" s="4">
         <v>20608000</v>
       </c>
-      <c r="AN13" s="5">
+      <c r="AN13" s="4">
         <v>64213000</v>
       </c>
-      <c r="AO13" s="5">
+      <c r="AO13" s="4">
         <v>-47714000</v>
       </c>
-      <c r="AP13" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="5">
+      <c r="AP13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="4">
         <v>3276000</v>
       </c>
-      <c r="AT13" s="5">
+      <c r="AT13" s="4">
         <v>392000</v>
       </c>
-      <c r="AU13" s="5">
+      <c r="AU13" s="4">
         <v>3668000</v>
       </c>
-      <c r="AV13" s="5">
+      <c r="AV13" s="4">
         <v>-44046000</v>
       </c>
-      <c r="AW13" s="5">
+      <c r="AW13" s="4">
         <v>314000</v>
       </c>
-      <c r="AX13" s="5">
+      <c r="AX13" s="4">
         <v>-44360000</v>
       </c>
     </row>
@@ -2206,151 +2230,151 @@
       <c r="A14" s="1">
         <v>44773</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>341806500</v>
       </c>
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
         <v>26795000</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>22269500</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>503952500</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>120357000</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>11143000</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>103219000</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>13011500</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>5408000</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <v>11420500</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <v>3099500</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <v>771611000</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>2862500</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="9">
         <v>42906500</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="9">
         <v>54185000</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="9">
         <v>14342500</v>
       </c>
-      <c r="S14" s="10">
+      <c r="S14" s="9">
         <v>5363000</v>
       </c>
-      <c r="T14" s="10">
+      <c r="T14" s="9">
         <v>119659500</v>
       </c>
-      <c r="U14" s="10">
-        <v>0</v>
-      </c>
-      <c r="V14" s="10">
+      <c r="U14" s="9">
+        <v>0</v>
+      </c>
+      <c r="V14" s="9">
         <v>11026000</v>
       </c>
-      <c r="W14" s="10">
+      <c r="W14" s="9">
         <v>18901500</v>
       </c>
-      <c r="X14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="10">
+      <c r="X14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="9">
         <v>8147500</v>
       </c>
-      <c r="Z14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="10">
+      <c r="Z14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="9">
         <v>1440000</v>
       </c>
-      <c r="AB14" s="10">
+      <c r="AB14" s="9">
         <v>159174500</v>
       </c>
-      <c r="AC14" s="10">
+      <c r="AC14" s="9">
         <v>1472375000</v>
       </c>
-      <c r="AD14" s="10">
+      <c r="AD14" s="9">
         <v>1607000</v>
       </c>
-      <c r="AE14" s="10">
+      <c r="AE14" s="9">
         <v>-861572500</v>
       </c>
-      <c r="AF14" s="10">
+      <c r="AF14" s="9">
         <v>612436500</v>
       </c>
-      <c r="AG14" s="10">
+      <c r="AG14" s="9">
         <v>771611000</v>
       </c>
-      <c r="AH14" s="5">
+      <c r="AH14" s="4">
         <v>48450000</v>
       </c>
-      <c r="AI14" s="5">
+      <c r="AI14" s="4">
         <v>24977000</v>
       </c>
-      <c r="AJ14" s="5">
+      <c r="AJ14" s="4">
         <v>23473000</v>
       </c>
-      <c r="AK14" s="5">
+      <c r="AK14" s="4">
         <v>26737000</v>
       </c>
-      <c r="AL14" s="5">
+      <c r="AL14" s="4">
         <v>19483000</v>
       </c>
-      <c r="AM14" s="5">
+      <c r="AM14" s="4">
         <v>19893000</v>
       </c>
-      <c r="AN14" s="5">
+      <c r="AN14" s="4">
         <v>66113000</v>
       </c>
-      <c r="AO14" s="5">
+      <c r="AO14" s="4">
         <v>-42640000</v>
       </c>
-      <c r="AP14" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="5">
+      <c r="AP14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="4">
         <v>1153000</v>
       </c>
-      <c r="AU14" s="5">
+      <c r="AU14" s="4">
         <v>3265000</v>
       </c>
-      <c r="AV14" s="5">
+      <c r="AV14" s="4">
         <v>-39375000</v>
       </c>
-      <c r="AW14" s="5">
+      <c r="AW14" s="4">
         <v>154000</v>
       </c>
-      <c r="AX14" s="5">
+      <c r="AX14" s="4">
         <v>-39529000</v>
       </c>
     </row>
@@ -2358,151 +2382,151 @@
       <c r="A15" s="1">
         <v>44865</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>199124000</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>226163000</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>29009000</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>26347000</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>480643000</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>115385000</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>11181000</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>103219000</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>12419000</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>5163000</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>15806000</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="5">
         <v>3412000</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="5">
         <v>747228000</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="5">
         <v>2557000</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="5">
         <v>42629000</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="5">
         <v>47698000</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="5">
         <v>13446000</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <v>3538000</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="5">
         <v>109868000</v>
       </c>
-      <c r="U15" s="6">
-        <v>0</v>
-      </c>
-      <c r="V15" s="6">
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5">
         <v>9853000</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="5">
         <v>17855000</v>
       </c>
-      <c r="X15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="6">
+      <c r="X15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="5">
         <v>14024000</v>
       </c>
-      <c r="Z15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="6">
+      <c r="Z15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="5">
         <v>1461000</v>
       </c>
-      <c r="AB15" s="6">
+      <c r="AB15" s="5">
         <v>153061000</v>
       </c>
-      <c r="AC15" s="6">
+      <c r="AC15" s="5">
         <v>1494652000</v>
       </c>
-      <c r="AD15" s="6">
+      <c r="AD15" s="5">
         <v>943000</v>
       </c>
-      <c r="AE15" s="6">
+      <c r="AE15" s="5">
         <v>-901455000</v>
       </c>
-      <c r="AF15" s="6">
+      <c r="AF15" s="5">
         <v>594167000</v>
       </c>
-      <c r="AG15" s="6">
+      <c r="AG15" s="5">
         <v>747228000</v>
       </c>
-      <c r="AH15" s="5">
+      <c r="AH15" s="4">
         <v>49704000</v>
       </c>
-      <c r="AI15" s="5">
+      <c r="AI15" s="4">
         <v>24728000</v>
       </c>
-      <c r="AJ15" s="5">
+      <c r="AJ15" s="4">
         <v>24976000</v>
       </c>
-      <c r="AK15" s="5">
+      <c r="AK15" s="4">
         <v>27598000</v>
       </c>
-      <c r="AL15" s="5">
+      <c r="AL15" s="4">
         <v>19383000</v>
       </c>
-      <c r="AM15" s="5">
+      <c r="AM15" s="4">
         <v>20627000</v>
       </c>
-      <c r="AN15" s="5">
+      <c r="AN15" s="4">
         <v>67608000</v>
       </c>
-      <c r="AO15" s="5">
+      <c r="AO15" s="4">
         <v>-42632000</v>
       </c>
-      <c r="AP15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="5">
+      <c r="AP15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="4">
         <v>2853000</v>
       </c>
-      <c r="AR15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS15" s="5">
+      <c r="AR15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="4">
         <v>-19000</v>
       </c>
-      <c r="AT15" s="5">
+      <c r="AT15" s="4">
         <v>1000</v>
       </c>
-      <c r="AU15" s="5">
+      <c r="AU15" s="4">
         <v>2835000</v>
       </c>
-      <c r="AV15" s="5">
+      <c r="AV15" s="4">
         <v>-39797000</v>
       </c>
-      <c r="AW15" s="5">
+      <c r="AW15" s="4">
         <v>439000</v>
       </c>
-      <c r="AX15" s="5">
+      <c r="AX15" s="4">
         <v>-40236000</v>
       </c>
     </row>
@@ -2510,151 +2534,151 @@
       <c r="A16" s="1">
         <v>44957</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>181892000</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>226868000</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>38952000</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>27943000</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>475655000</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>108091000</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>11417000</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <v>112748000</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>14831000</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>5657000</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="5">
         <v>20403000</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="5">
         <v>3921000</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="5">
         <v>752723000</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="5">
         <v>6900000</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="5">
         <v>46022000</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16" s="5">
         <v>51900000</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16" s="5">
         <v>12550000</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="5">
         <v>4885000</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T16" s="5">
         <v>122257000</v>
       </c>
-      <c r="U16" s="6">
+      <c r="U16" s="5">
         <v>2882000</v>
       </c>
-      <c r="V16" s="6">
+      <c r="V16" s="5">
         <v>8679000</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W16" s="5">
         <v>16670000</v>
       </c>
-      <c r="X16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="6">
+      <c r="X16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="5">
         <v>17145000</v>
       </c>
-      <c r="Z16" s="6">
+      <c r="Z16" s="5">
         <v>7499000</v>
       </c>
-      <c r="AA16" s="6">
+      <c r="AA16" s="5">
         <v>1487000</v>
       </c>
-      <c r="AB16" s="6">
+      <c r="AB16" s="5">
         <v>176619000</v>
       </c>
-      <c r="AC16" s="6">
+      <c r="AC16" s="5">
         <v>1513102000</v>
       </c>
-      <c r="AD16" s="6">
+      <c r="AD16" s="5">
         <v>2271000</v>
       </c>
-      <c r="AE16" s="6">
+      <c r="AE16" s="5">
         <v>-939296000</v>
       </c>
-      <c r="AF16" s="6">
+      <c r="AF16" s="5">
         <v>576104000</v>
       </c>
-      <c r="AG16" s="6">
+      <c r="AG16" s="5">
         <v>752723000</v>
       </c>
-      <c r="AH16" s="5">
+      <c r="AH16" s="4">
         <v>52975000</v>
       </c>
-      <c r="AI16" s="5">
+      <c r="AI16" s="4">
         <v>23915000</v>
       </c>
-      <c r="AJ16" s="5">
+      <c r="AJ16" s="4">
         <v>29060000</v>
       </c>
-      <c r="AK16" s="5">
+      <c r="AK16" s="4">
         <v>31831000</v>
       </c>
-      <c r="AL16" s="5">
+      <c r="AL16" s="4">
         <v>20299000</v>
       </c>
-      <c r="AM16" s="5">
+      <c r="AM16" s="4">
         <v>19619000</v>
       </c>
-      <c r="AN16" s="5">
+      <c r="AN16" s="4">
         <v>71749000</v>
       </c>
-      <c r="AO16" s="5">
+      <c r="AO16" s="4">
         <v>-42689000</v>
       </c>
-      <c r="AP16" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="5">
+      <c r="AP16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="4">
         <v>4819000</v>
       </c>
-      <c r="AR16" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS16" s="5">
+      <c r="AR16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="4">
         <v>3297000</v>
       </c>
-      <c r="AT16" s="5">
+      <c r="AT16" s="4">
         <v>-1216000</v>
       </c>
-      <c r="AU16" s="5">
+      <c r="AU16" s="4">
         <v>4788000</v>
       </c>
-      <c r="AV16" s="5">
+      <c r="AV16" s="4">
         <v>-37901000</v>
       </c>
-      <c r="AW16" s="5">
+      <c r="AW16" s="4">
         <v>-60000</v>
       </c>
-      <c r="AX16" s="5">
+      <c r="AX16" s="4">
         <v>-37841000</v>
       </c>
     </row>
@@ -2662,151 +2686,151 @@
       <c r="A17" s="1">
         <v>45046</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>140763000</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>235415000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>39072000</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>19275000</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>434525000</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>118193000</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>11878000</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>112748000</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>13999000</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>5660000</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <v>23697000</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="5">
         <v>2757000</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="5">
         <v>723457000</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="5">
         <v>14657000</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="5">
         <v>34432000</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17" s="5">
         <v>44620000</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="5">
         <v>11653000</v>
       </c>
-      <c r="S17" s="6">
+      <c r="S17" s="5">
         <v>6320000</v>
       </c>
-      <c r="T17" s="6">
+      <c r="T17" s="5">
         <v>111682000</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="5">
         <v>2474000</v>
       </c>
-      <c r="V17" s="6">
+      <c r="V17" s="5">
         <v>10671000</v>
       </c>
-      <c r="W17" s="6">
+      <c r="W17" s="5">
         <v>10725000</v>
       </c>
-      <c r="X17" s="6">
+      <c r="X17" s="5">
         <v>19912000</v>
       </c>
-      <c r="Y17" s="6">
+      <c r="Y17" s="5">
         <v>7142000</v>
       </c>
-      <c r="Z17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="6">
+      <c r="Z17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="5">
         <v>1502000</v>
       </c>
-      <c r="AB17" s="6">
+      <c r="AB17" s="5">
         <v>164108000</v>
       </c>
-      <c r="AC17" s="6">
+      <c r="AC17" s="5">
         <v>1531380000</v>
       </c>
-      <c r="AD17" s="6">
+      <c r="AD17" s="5">
         <v>1682000</v>
       </c>
-      <c r="AE17" s="6">
+      <c r="AE17" s="5">
         <v>-973740000</v>
       </c>
-      <c r="AF17" s="6">
+      <c r="AF17" s="5">
         <v>559349000</v>
       </c>
-      <c r="AG17" s="6">
+      <c r="AG17" s="5">
         <v>723457000</v>
       </c>
-      <c r="AH17" s="5">
+      <c r="AH17" s="4">
         <v>52703000</v>
       </c>
-      <c r="AI17" s="5">
+      <c r="AI17" s="4">
         <v>24556000</v>
       </c>
-      <c r="AJ17" s="5">
+      <c r="AJ17" s="4">
         <v>28147000</v>
       </c>
-      <c r="AK17" s="5">
+      <c r="AK17" s="4">
         <v>28186000</v>
       </c>
-      <c r="AL17" s="5">
+      <c r="AL17" s="4">
         <v>23125000</v>
       </c>
-      <c r="AM17" s="5">
+      <c r="AM17" s="4">
         <v>21528000</v>
       </c>
-      <c r="AN17" s="5">
+      <c r="AN17" s="4">
         <v>72839000</v>
       </c>
-      <c r="AO17" s="5">
+      <c r="AO17" s="4">
         <v>-44692000</v>
       </c>
-      <c r="AP17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="5">
+      <c r="AP17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="4">
         <v>4506000</v>
       </c>
-      <c r="AR17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="5">
+      <c r="AR17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="4">
         <v>-5945000</v>
       </c>
-      <c r="AT17" s="5">
+      <c r="AT17" s="4">
         <v>104000</v>
       </c>
-      <c r="AU17" s="5">
+      <c r="AU17" s="4">
         <v>10555000</v>
       </c>
-      <c r="AV17" s="5">
+      <c r="AV17" s="4">
         <v>-34137000</v>
       </c>
-      <c r="AW17" s="5">
+      <c r="AW17" s="4">
         <v>307000</v>
       </c>
-      <c r="AX17" s="5">
+      <c r="AX17" s="4">
         <v>-34444000</v>
       </c>
     </row>
@@ -2814,151 +2838,151 @@
       <c r="A18" s="1">
         <v>45138</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>118808000</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>248979000</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>40349000</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>19725000</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>427861000</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>120193000</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>12992000</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>112750000</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>14867000</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="4">
         <v>5707000</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="4">
         <v>23485000</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="4">
         <v>2562000</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="4">
         <v>720417000</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="4">
         <v>3825000</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="6">
         <v>37841000</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="6">
         <v>56575000</v>
       </c>
-      <c r="R18" s="5">
+      <c r="R18" s="4">
         <v>10757000</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="4">
         <v>7261000</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="4">
         <v>116259000</v>
       </c>
-      <c r="U18" s="7">
+      <c r="U18" s="6">
         <v>18186000</v>
       </c>
-      <c r="V18" s="7">
+      <c r="V18" s="6">
         <v>9605000</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="4">
         <v>9499000</v>
       </c>
-      <c r="X18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="5">
+      <c r="X18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="4">
         <v>19139000</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="Z18" s="4">
         <v>5926000</v>
       </c>
-      <c r="AA18" s="5">
+      <c r="AA18" s="4">
         <v>2235000</v>
       </c>
-      <c r="AB18" s="5">
+      <c r="AB18" s="4">
         <v>180849000</v>
       </c>
-      <c r="AC18" s="5">
+      <c r="AC18" s="4">
         <v>1549920000</v>
       </c>
-      <c r="AD18" s="5">
+      <c r="AD18" s="4">
         <v>1336000</v>
       </c>
-      <c r="AE18" s="5">
+      <c r="AE18" s="4">
         <v>-1011715000</v>
       </c>
-      <c r="AF18" s="5">
+      <c r="AF18" s="4">
         <v>539568000</v>
       </c>
-      <c r="AG18" s="5">
+      <c r="AG18" s="4">
         <v>720417000</v>
       </c>
-      <c r="AH18" s="5">
+      <c r="AH18" s="4">
         <v>53761000</v>
       </c>
-      <c r="AI18" s="5">
+      <c r="AI18" s="4">
         <v>27469000</v>
       </c>
-      <c r="AJ18" s="5">
+      <c r="AJ18" s="4">
         <v>26292000</v>
       </c>
-      <c r="AK18" s="5">
+      <c r="AK18" s="4">
         <v>26741000</v>
       </c>
-      <c r="AL18" s="5">
+      <c r="AL18" s="4">
         <v>22310000</v>
       </c>
-      <c r="AM18" s="5">
+      <c r="AM18" s="4">
         <v>20521000</v>
       </c>
-      <c r="AN18" s="5">
+      <c r="AN18" s="4">
         <v>69572000</v>
       </c>
-      <c r="AO18" s="5">
+      <c r="AO18" s="4">
         <v>-43280000</v>
       </c>
-      <c r="AP18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="5">
+      <c r="AP18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="4">
         <v>3802000</v>
       </c>
-      <c r="AR18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="5">
+      <c r="AR18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="4">
         <v>1226000</v>
       </c>
-      <c r="AT18" s="5">
+      <c r="AT18" s="4">
         <v>859000</v>
       </c>
-      <c r="AU18" s="5">
+      <c r="AU18" s="4">
         <v>5887000</v>
       </c>
-      <c r="AV18" s="5">
+      <c r="AV18" s="4">
         <v>-37393000</v>
       </c>
-      <c r="AW18" s="5">
+      <c r="AW18" s="4">
         <v>582000</v>
       </c>
-      <c r="AX18" s="5">
+      <c r="AX18" s="4">
         <v>-37975000</v>
       </c>
     </row>
@@ -2966,151 +2990,151 @@
       <c r="A19" s="1">
         <v>45230</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>101547000</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>213347000</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>45145000</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>19616000</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>387535000</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>114058000</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>14050000</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>135701000</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <v>27427000</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="4">
         <v>10321000</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="4">
         <v>22091000</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="4">
         <v>2337000</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="4">
         <v>713520000</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <v>4589000</v>
       </c>
-      <c r="P19" s="5">
+      <c r="P19" s="4">
         <v>41961000</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="Q19" s="4">
         <v>67228000</v>
       </c>
-      <c r="R19" s="5">
+      <c r="R19" s="4">
         <v>9860000</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S19" s="4">
         <v>7500000</v>
       </c>
-      <c r="T19" s="5">
+      <c r="T19" s="4">
         <v>131138000</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="4">
         <v>7763000</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="4">
         <v>8353000</v>
       </c>
-      <c r="W19" s="5">
+      <c r="W19" s="4">
         <v>2666000</v>
       </c>
-      <c r="X19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="5">
+      <c r="X19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="4">
         <v>17321000</v>
       </c>
-      <c r="Z19" s="5">
+      <c r="Z19" s="4">
         <v>5588000</v>
       </c>
-      <c r="AA19" s="5">
+      <c r="AA19" s="4">
         <v>7093000</v>
       </c>
-      <c r="AB19" s="5">
+      <c r="AB19" s="4">
         <v>179922000</v>
       </c>
-      <c r="AC19" s="5">
+      <c r="AC19" s="4">
         <v>1583531000</v>
       </c>
-      <c r="AD19" s="5">
+      <c r="AD19" s="4">
         <v>-242000</v>
       </c>
-      <c r="AE19" s="5">
+      <c r="AE19" s="4">
         <v>-1049719000</v>
       </c>
-      <c r="AF19" s="5">
+      <c r="AF19" s="4">
         <v>533598000</v>
       </c>
-      <c r="AG19" s="5">
+      <c r="AG19" s="4">
         <v>713520000</v>
       </c>
-      <c r="AH19" s="5">
+      <c r="AH19" s="4">
         <v>55380000</v>
       </c>
-      <c r="AI19" s="5">
+      <c r="AI19" s="4">
         <v>29350000</v>
       </c>
-      <c r="AJ19" s="5">
+      <c r="AJ19" s="4">
         <v>26030000</v>
       </c>
-      <c r="AK19" s="5">
+      <c r="AK19" s="4">
         <v>33002000</v>
       </c>
-      <c r="AL19" s="5">
+      <c r="AL19" s="4">
         <v>20774000</v>
       </c>
-      <c r="AM19" s="5">
+      <c r="AM19" s="4">
         <v>20112000</v>
       </c>
-      <c r="AN19" s="5">
+      <c r="AN19" s="4">
         <v>73888000</v>
       </c>
-      <c r="AO19" s="5">
+      <c r="AO19" s="4">
         <v>-47858000</v>
       </c>
-      <c r="AP19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="5">
+      <c r="AP19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="4">
         <v>3445000</v>
       </c>
-      <c r="AR19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="5">
+      <c r="AR19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="4">
         <v>6833000</v>
       </c>
-      <c r="AT19" s="5">
+      <c r="AT19" s="4">
         <v>-69000</v>
       </c>
-      <c r="AU19" s="5">
+      <c r="AU19" s="4">
         <v>10209000</v>
       </c>
-      <c r="AV19" s="5">
+      <c r="AV19" s="4">
         <v>-37649000</v>
       </c>
-      <c r="AW19" s="5">
+      <c r="AW19" s="4">
         <v>355000</v>
       </c>
-      <c r="AX19" s="5">
+      <c r="AX19" s="4">
         <v>-38004000</v>
       </c>
     </row>
@@ -3118,151 +3142,151 @@
       <c r="A20" s="1">
         <v>45322</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>83866000</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>215041000</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>43320000</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>19564000</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>370151000</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>113429000</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>14973000</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>136256000</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>32448000</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>9972000</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <v>22339000</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20" s="7">
         <v>2429000</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="7">
         <v>701997000</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O20" s="7">
         <v>2601000</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="7">
         <v>44779000</v>
       </c>
-      <c r="Q20" s="8">
+      <c r="Q20" s="7">
         <v>72327000</v>
       </c>
-      <c r="R20" s="8">
+      <c r="R20" s="7">
         <v>8964000</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="7">
         <v>7978000</v>
       </c>
-      <c r="T20" s="8">
+      <c r="T20" s="7">
         <v>136649000</v>
       </c>
-      <c r="U20" s="8">
+      <c r="U20" s="7">
         <v>5293000</v>
       </c>
-      <c r="V20" s="8">
+      <c r="V20" s="7">
         <v>7101000</v>
       </c>
-      <c r="W20" s="8">
+      <c r="W20" s="7">
         <v>2961000</v>
       </c>
-      <c r="X20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="8">
+      <c r="X20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="7">
         <v>16952000</v>
       </c>
-      <c r="Z20" s="8">
+      <c r="Z20" s="7">
         <v>5885000</v>
       </c>
-      <c r="AA20" s="8">
+      <c r="AA20" s="7">
         <v>9138000</v>
       </c>
-      <c r="AB20" s="8">
+      <c r="AB20" s="7">
         <v>183979000</v>
       </c>
-      <c r="AC20" s="8">
+      <c r="AC20" s="7">
         <v>1596201000</v>
       </c>
-      <c r="AD20" s="8">
+      <c r="AD20" s="7">
         <v>1594000</v>
       </c>
-      <c r="AE20" s="8">
+      <c r="AE20" s="7">
         <v>-1079805000</v>
       </c>
-      <c r="AF20" s="8">
+      <c r="AF20" s="7">
         <v>518018000</v>
       </c>
-      <c r="AG20" s="8">
+      <c r="AG20" s="7">
         <v>701997000</v>
       </c>
-      <c r="AH20" s="5">
+      <c r="AH20" s="4">
         <v>220696000</v>
       </c>
-      <c r="AI20" s="5">
+      <c r="AI20" s="4">
         <v>107746000</v>
       </c>
-      <c r="AJ20" s="5">
+      <c r="AJ20" s="4">
         <v>112950000</v>
       </c>
-      <c r="AK20" s="5">
+      <c r="AK20" s="4">
         <v>116339000</v>
       </c>
-      <c r="AL20" s="5">
+      <c r="AL20" s="4">
         <v>86304000</v>
       </c>
-      <c r="AM20" s="5">
+      <c r="AM20" s="4">
         <v>80055000</v>
       </c>
-      <c r="AN20" s="5">
+      <c r="AN20" s="4">
         <v>282698000</v>
       </c>
-      <c r="AO20" s="5">
+      <c r="AO20" s="4">
         <v>-169748000</v>
       </c>
-      <c r="AP20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="5">
+      <c r="AP20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="4">
         <v>15414000</v>
       </c>
-      <c r="AR20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="5">
+      <c r="AR20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="4">
         <v>13709000</v>
       </c>
-      <c r="AT20" s="5">
+      <c r="AT20" s="4">
         <v>931000</v>
       </c>
-      <c r="AU20" s="5">
+      <c r="AU20" s="4">
         <v>30054000</v>
       </c>
-      <c r="AV20" s="5">
+      <c r="AV20" s="4">
         <v>-139694000</v>
       </c>
-      <c r="AW20" s="5">
+      <c r="AW20" s="4">
         <v>815000</v>
       </c>
-      <c r="AX20" s="5">
+      <c r="AX20" s="4">
         <v>-140509000</v>
       </c>
     </row>
@@ -3270,151 +3294,151 @@
       <c r="A21" s="1">
         <v>45412</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>107367000</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>168218000</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>38527000</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>23044000</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>345958000</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>111338000</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="7">
         <v>16066000</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>137110000</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <v>31403000</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <v>9564000</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="7">
         <v>20966000</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21" s="7">
         <v>2199000</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="7">
         <v>674604000</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O21" s="7">
         <v>3131000</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P21" s="7">
         <v>43361000</v>
       </c>
-      <c r="Q21" s="8">
+      <c r="Q21" s="7">
         <v>63646000</v>
       </c>
-      <c r="R21" s="8">
+      <c r="R21" s="7">
         <v>8068000</v>
       </c>
-      <c r="S21" s="8">
+      <c r="S21" s="7">
         <v>8175000</v>
       </c>
-      <c r="T21" s="8">
+      <c r="T21" s="7">
         <v>126381000</v>
       </c>
-      <c r="U21" s="8">
+      <c r="U21" s="7">
         <v>13247000</v>
       </c>
-      <c r="V21" s="8">
+      <c r="V21" s="7">
         <v>9261000</v>
       </c>
-      <c r="W21" s="8">
+      <c r="W21" s="7">
         <v>1431000</v>
       </c>
-      <c r="X21" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="8">
+      <c r="X21" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="7">
         <v>15207000</v>
       </c>
-      <c r="Z21" s="8">
+      <c r="Z21" s="7">
         <v>2915000</v>
       </c>
-      <c r="AA21" s="8">
+      <c r="AA21" s="7">
         <v>5837000</v>
       </c>
-      <c r="AB21" s="8">
+      <c r="AB21" s="7">
         <v>174279000</v>
       </c>
-      <c r="AC21" s="8">
+      <c r="AC21" s="7">
         <v>1608847000</v>
       </c>
-      <c r="AD21" s="8">
+      <c r="AD21" s="7">
         <v>548000</v>
       </c>
-      <c r="AE21" s="8">
+      <c r="AE21" s="7">
         <v>-1109098000</v>
       </c>
-      <c r="AF21" s="8">
+      <c r="AF21" s="7">
         <v>500325000</v>
       </c>
-      <c r="AG21" s="8">
+      <c r="AG21" s="7">
         <v>674604000</v>
       </c>
-      <c r="AH21" s="5">
+      <c r="AH21" s="4">
         <v>60440000</v>
       </c>
-      <c r="AI21" s="5">
+      <c r="AI21" s="4">
         <v>28757000</v>
       </c>
-      <c r="AJ21" s="5">
+      <c r="AJ21" s="4">
         <v>31683000</v>
       </c>
-      <c r="AK21" s="5">
+      <c r="AK21" s="4">
         <v>25589000</v>
       </c>
-      <c r="AL21" s="5">
+      <c r="AL21" s="4">
         <v>21485000</v>
       </c>
-      <c r="AM21" s="5">
+      <c r="AM21" s="4">
         <v>19180000</v>
       </c>
-      <c r="AN21" s="5">
+      <c r="AN21" s="4">
         <v>66254000</v>
       </c>
-      <c r="AO21" s="5">
+      <c r="AO21" s="4">
         <v>-34571000</v>
       </c>
-      <c r="AP21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ21" s="5">
+      <c r="AP21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="4">
         <v>3107000</v>
       </c>
-      <c r="AR21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS21" s="5">
+      <c r="AR21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="4">
         <v>1530000</v>
       </c>
-      <c r="AT21" s="5">
+      <c r="AT21" s="4">
         <v>1083000</v>
       </c>
-      <c r="AU21" s="5">
+      <c r="AU21" s="4">
         <v>5720000</v>
       </c>
-      <c r="AV21" s="5">
+      <c r="AV21" s="4">
         <v>-28851000</v>
       </c>
-      <c r="AW21" s="5">
+      <c r="AW21" s="4">
         <v>442000</v>
       </c>
-      <c r="AX21" s="5">
+      <c r="AX21" s="4">
         <v>-29293000</v>
       </c>
     </row>
@@ -3425,25 +3449,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9840AC-F14A-4C58-BDF4-7D814B7753BE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[DATA] update data formatting for data loading
</commit_message>
<xml_diff>
--- a/financial_data/planet.xlsx
+++ b/financial_data/planet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinten/Desktop/untitled folder 3/space_econometrics/financial_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81669736-DE79-7C4E-9428-076F1724FDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7533B-B488-483A-9CAB-D5E7DBFD0700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -576,998 +576,998 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1581,66 +1581,72 @@
   </sheetPr>
   <dimension ref="A1:BP21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="19" width="20.6640625" customWidth="1"/>
-    <col min="20" max="21" width="16.6640625" customWidth="1"/>
-    <col min="22" max="22" width="16.5" customWidth="1"/>
-    <col min="23" max="23" width="15.6640625" customWidth="1"/>
-    <col min="24" max="25" width="16.6640625" customWidth="1"/>
-    <col min="26" max="26" width="16.5" customWidth="1"/>
-    <col min="27" max="27" width="16.6640625" customWidth="1"/>
-    <col min="28" max="28" width="16.5" customWidth="1"/>
-    <col min="29" max="29" width="15.5" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" customWidth="1"/>
-    <col min="31" max="31" width="15.5" customWidth="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="33" width="16.5" customWidth="1"/>
-    <col min="34" max="35" width="15.5" customWidth="1"/>
-    <col min="36" max="36" width="15.6640625" customWidth="1"/>
-    <col min="37" max="37" width="14.6640625" customWidth="1"/>
-    <col min="38" max="38" width="16.6640625" customWidth="1"/>
-    <col min="39" max="39" width="16.5" customWidth="1"/>
-    <col min="40" max="42" width="15.5" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" customWidth="1"/>
-    <col min="44" max="45" width="14.6640625" customWidth="1"/>
-    <col min="46" max="46" width="16.6640625" customWidth="1"/>
-    <col min="47" max="47" width="18.5" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" customWidth="1"/>
-    <col min="49" max="49" width="19.1640625" customWidth="1"/>
-    <col min="50" max="51" width="16.6640625" customWidth="1"/>
-    <col min="52" max="55" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="24" max="25" width="16.7109375" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" customWidth="1"/>
+    <col min="29" max="29" width="15.42578125" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" customWidth="1"/>
+    <col min="34" max="35" width="15.42578125" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" customWidth="1"/>
+    <col min="38" max="38" width="16.7109375" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" customWidth="1"/>
+    <col min="40" max="42" width="15.42578125" customWidth="1"/>
+    <col min="43" max="43" width="15.7109375" customWidth="1"/>
+    <col min="44" max="45" width="14.7109375" customWidth="1"/>
+    <col min="46" max="46" width="16.7109375" customWidth="1"/>
+    <col min="47" max="47" width="18.42578125" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" customWidth="1"/>
+    <col min="49" max="49" width="19.140625" customWidth="1"/>
+    <col min="50" max="51" width="16.7109375" customWidth="1"/>
+    <col min="52" max="55" width="15.140625" customWidth="1"/>
     <col min="56" max="57" width="14" customWidth="1"/>
-    <col min="58" max="58" width="15.1640625" customWidth="1"/>
-    <col min="59" max="59" width="15.83203125" customWidth="1"/>
-    <col min="60" max="60" width="13.5" customWidth="1"/>
+    <col min="58" max="58" width="15.140625" customWidth="1"/>
+    <col min="59" max="59" width="15.85546875" customWidth="1"/>
+    <col min="60" max="60" width="13.42578125" customWidth="1"/>
     <col min="61" max="61" width="14" customWidth="1"/>
-    <col min="62" max="62" width="13.5" customWidth="1"/>
-    <col min="63" max="63" width="14.6640625" customWidth="1"/>
-    <col min="64" max="64" width="13.5" customWidth="1"/>
-    <col min="65" max="65" width="14.6640625" customWidth="1"/>
-    <col min="66" max="66" width="15.83203125" customWidth="1"/>
-    <col min="67" max="67" width="12.6640625" customWidth="1"/>
-    <col min="68" max="68" width="15.83203125" customWidth="1"/>
+    <col min="62" max="62" width="13.42578125" customWidth="1"/>
+    <col min="63" max="63" width="14.7109375" customWidth="1"/>
+    <col min="64" max="64" width="13.42578125" customWidth="1"/>
+    <col min="65" max="65" width="14.7109375" customWidth="1"/>
+    <col min="66" max="66" width="15.85546875" customWidth="1"/>
+    <col min="67" max="67" width="12.7109375" customWidth="1"/>
+    <col min="68" max="68" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43677</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>-30928500</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43769</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>-30928500</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43861</v>
       </c>
@@ -2170,7 +2176,7 @@
         <v>-30928500</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43951</v>
       </c>
@@ -2278,7 +2284,7 @@
         <v>-31775750</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44043</v>
       </c>
@@ -2386,7 +2392,7 @@
         <v>-31775750</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44135</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>-31775750</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44227</v>
       </c>
@@ -2700,7 +2706,7 @@
         <v>-31775750</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44316</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>-29255000</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44408</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>-20363000</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44500</v>
       </c>
@@ -3318,7 +3324,7 @@
         <v>-41541000</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44592</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>-45965000</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44681</v>
       </c>
@@ -3730,7 +3736,7 @@
         <v>-44360000</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44773</v>
       </c>
@@ -3936,7 +3942,7 @@
         <v>-39529000</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44865</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>-40236000</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44957</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>-37841000</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45046</v>
       </c>
@@ -4554,7 +4560,7 @@
         <v>-34444000</v>
       </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45138</v>
       </c>
@@ -4760,7 +4766,7 @@
         <v>-37975000</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45230</v>
       </c>
@@ -4966,7 +4972,7 @@
         <v>-38004000</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45322</v>
       </c>
@@ -5172,7 +5178,7 @@
         <v>-140509000</v>
       </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45412</v>
       </c>

</xml_diff>